<commit_message>
edit project settings for nunjucks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="Stories" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="META" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="META" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -77,26 +76,11 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
create macro file, headline function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet sheetId="1" name="META" state="visible" r:id="rId3"/>
-    <sheet sheetId="2" name="HEALTH" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="OVERVIEW" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="HEALTH" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -23,34 +24,62 @@
     <t>project_subtitle</t>
   </si>
   <si>
-    <t>After 14 years in the governor's office, Rick Perry has left a lasting mark on Texas</t>
+    <t>After 14 years in the governor's office, Rick Perry has left a lasting mark on Texas. </t>
   </si>
   <si>
     <t>byline</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Health Care</t>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>The Lasting Impact of Gov. Rick Perry</t>
   </si>
   <si>
     <t>byline</t>
   </si>
   <si>
+    <t>Jay Root</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/about/staff/jay-root</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
     <t>Alexa Ura</t>
+  </si>
+  <si>
+    <t>reporter_email</t>
+  </si>
+  <si>
+    <t>aura@texastribune.org</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -78,9 +107,15 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
   </cellXfs>
@@ -97,6 +132,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -123,7 +162,7 @@
       <c t="s" s="1" r="A2">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c t="s" s="2" r="B2">
         <v>3</v>
       </c>
     </row>
@@ -160,6 +199,56 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>9</v>
+      </c>
+      <c t="s" s="3" r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c s="1" r="A4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
create sub-nav with nunjucks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -6,6 +6,14 @@
     <sheet sheetId="1" name="META" state="visible" r:id="rId3"/>
     <sheet sheetId="2" name="OVERVIEW" state="visible" r:id="rId4"/>
     <sheet sheetId="3" name="HEALTH" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="PUBLIC_EDU" state="visible" r:id="rId6"/>
+    <sheet sheetId="5" name="HIGHER_EDU" state="visible" r:id="rId7"/>
+    <sheet sheetId="6" name="TRANSPO" state="visible" r:id="rId8"/>
+    <sheet sheetId="7" name="IMMIGRATION" state="visible" r:id="rId9"/>
+    <sheet sheetId="8" name="ENERGY" state="visible" r:id="rId10"/>
+    <sheet sheetId="9" name="ENVIRO" state="visible" r:id="rId11"/>
+    <sheet sheetId="10" name="TEF" state="visible" r:id="rId12"/>
+    <sheet sheetId="11" name="JUSTICE" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -30,6 +38,12 @@
     <t>byline</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
     <t>headline</t>
   </si>
   <si>
@@ -48,6 +62,12 @@
     <t>http://www.texastribune.org/about/staff/jay-root</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
     <t>headline</t>
   </si>
   <si>
@@ -60,17 +80,191 @@
     <t>Alexa Ura</t>
   </si>
   <si>
-    <t>reporter_email</t>
-  </si>
-  <si>
-    <t>aura@texastribune.org</t>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/about/staff/</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Public Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-book</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Immigration</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-group</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-tint</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-tree</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Texas Enterprise Fund</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-money</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Criminal Justice</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-legal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -80,13 +274,23 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF777777"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -107,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -118,6 +322,9 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -131,11 +338,43 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -176,6 +415,92 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>65</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>70</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
@@ -203,16 +528,21 @@
       <c t="s" s="1" r="A3">
         <v>9</v>
       </c>
-      <c t="s" s="3" r="B3">
+      <c t="s" s="1" r="B3">
         <v>10</v>
       </c>
     </row>
     <row r="4">
-      <c s="1" r="A4"/>
+      <c t="s" s="1" r="A4">
+        <v>11</v>
+      </c>
+      <c t="s" s="3" r="B4">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -227,29 +557,306 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
         <v>13</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>15</v>
+      </c>
       <c t="s" s="1" r="B2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>17</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>16</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>19</v>
+      </c>
+      <c t="s" s="3" r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>35</v>
+      </c>
+      <c t="s" s="4" r="B5">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add fixedtop settings for masthead
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -62,6 +62,18 @@
     <t>http://www.texastribune.org/about/staff/jay-root</t>
   </si>
   <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-star</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -92,6 +104,12 @@
     <t>fa-plus-square</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -113,6 +131,12 @@
     <t>fa-book</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>public-education</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -134,6 +158,12 @@
     <t>fa-graduation-cap</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>higher-education</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -155,6 +185,12 @@
     <t>fa-car</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -176,6 +212,12 @@
     <t>fa-group</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -197,6 +239,12 @@
     <t>fa-tint</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -218,6 +266,12 @@
     <t>fa-tree</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -239,6 +293,12 @@
     <t>fa-money</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>texas-enterprise-fund</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -258,6 +318,12 @@
   </si>
   <si>
     <t>fa-legal</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>criminal-justice</t>
   </si>
 </sst>
 </file>
@@ -424,33 +490,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>71</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -467,33 +541,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>73</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>74</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>76</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>78</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -540,6 +622,22 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
@@ -557,42 +655,50 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c t="s" s="3" r="B4">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>22</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -612,33 +718,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>29</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -655,33 +769,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c t="s" s="4" r="B5">
-        <v>36</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>45</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -698,33 +820,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>43</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -741,33 +871,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>50</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -784,33 +922,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>57</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -827,33 +973,41 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>64</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add secondary base template, create temp transportation page as example, edit masthead
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,15 +5,15 @@
   <sheets>
     <sheet sheetId="1" name="META" state="visible" r:id="rId3"/>
     <sheet sheetId="2" name="OVERVIEW" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="HEALTH" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="PUBLIC_EDU" state="visible" r:id="rId6"/>
+    <sheet sheetId="3" name="TRANSPO" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="HEALTH" state="visible" r:id="rId6"/>
     <sheet sheetId="5" name="HIGHER_EDU" state="visible" r:id="rId7"/>
-    <sheet sheetId="6" name="TRANSPO" state="visible" r:id="rId8"/>
-    <sheet sheetId="7" name="IMMIGRATION" state="visible" r:id="rId9"/>
+    <sheet sheetId="6" name="PUBLIC_EDU" state="visible" r:id="rId8"/>
+    <sheet sheetId="7" name="ENVIRO" state="visible" r:id="rId9"/>
     <sheet sheetId="8" name="ENERGY" state="visible" r:id="rId10"/>
-    <sheet sheetId="9" name="ENVIRO" state="visible" r:id="rId11"/>
-    <sheet sheetId="10" name="TEF" state="visible" r:id="rId12"/>
-    <sheet sheetId="11" name="JUSTICE" state="visible" r:id="rId13"/>
+    <sheet sheetId="9" name="IMMIGRATION" state="visible" r:id="rId11"/>
+    <sheet sheetId="10" name="JUSTICE" state="visible" r:id="rId12"/>
+    <sheet sheetId="11" name="TEF" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -77,6 +77,60 @@
     <t>topic</t>
   </si>
   <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio. Texas Governor Rick Perry helped with the ribbon cutting ceremony on the highway near Lockhart, Texas in Caldwell County.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>Health Care</t>
   </si>
   <si>
@@ -89,13 +143,10 @@
     <t>byline</t>
   </si>
   <si>
-    <t>Alexa Ura</t>
-  </si>
-  <si>
-    <t>reporter_bio</t>
-  </si>
-  <si>
-    <t>http://www.texastribune.org/about/staff/</t>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
@@ -113,6 +164,36 @@
     <t>topic</t>
   </si>
   <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>higher-education</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>Public Education</t>
   </si>
   <si>
@@ -122,7 +203,10 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
@@ -140,7 +224,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Higher Education</t>
+    <t>Environment</t>
   </si>
   <si>
     <t>headline</t>
@@ -149,25 +233,28 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Neena Satija](http://www.texastribune.org/about/staff/neena-satija/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
   </si>
   <si>
-    <t>fa-graduation-cap</t>
+    <t>fa-tree</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>higher-education</t>
+    <t>environment</t>
   </si>
   <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Transportation</t>
+    <t>Energy</t>
   </si>
   <si>
     <t>headline</t>
@@ -176,19 +263,22 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
   </si>
   <si>
-    <t>fa-car</t>
+    <t>fa-tint</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>transportation</t>
+    <t>energy</t>
   </si>
   <si>
     <t>topic</t>
@@ -203,7 +293,10 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
@@ -221,7 +314,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Energy</t>
+    <t>Criminal Justice</t>
   </si>
   <si>
     <t>headline</t>
@@ -230,25 +323,28 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Terri Langford](http://www.texastribune.org/about/staff/terri-langford/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
   </si>
   <si>
-    <t>fa-tint</t>
+    <t>fa-legal</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>energy</t>
+    <t>criminal-justice</t>
   </si>
   <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Environment</t>
+    <t>Texas Enterprise Fund</t>
   </si>
   <si>
     <t>headline</t>
@@ -257,73 +353,22 @@
     <t>byline</t>
   </si>
   <si>
-    <t>reporter_bio</t>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>icon</t>
   </si>
   <si>
-    <t>fa-tree</t>
+    <t>fa-money</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>environment</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Texas Enterprise Fund</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>reporter_bio</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-money</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
     <t>texas-enterprise-fund</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Criminal Justice</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>reporter_bio</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-legal</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>criminal-justice</t>
   </si>
 </sst>
 </file>
@@ -490,41 +535,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>86</v>
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>100</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>101</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>87</v>
+        <v>102</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>103</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -541,41 +587,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>93</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>94</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>95</v>
+        <v>109</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>96</v>
+        <v>112</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>99</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -652,6 +699,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="32.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
@@ -676,34 +726,58 @@
       <c t="s" s="1" r="B3">
         <v>22</v>
       </c>
+      <c t="s" s="1" r="C3">
+        <v>23</v>
+      </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>23</v>
-      </c>
-      <c t="s" s="3" r="B4">
         <v>24</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="B6">
         <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>29</v>
+      </c>
+      <c t="s" s="3" r="B7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>31</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="B9">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -718,41 +792,45 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>41</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>43</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -769,41 +847,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>41</v>
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>50</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>42</v>
+        <v>52</v>
+      </c>
+      <c t="s" s="4" r="B4">
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>43</v>
-      </c>
-      <c t="s" s="4" r="B5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -820,41 +899,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>60</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>51</v>
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -871,41 +951,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>70</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -922,41 +1003,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>68</v>
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>69</v>
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>72</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>73</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -973,41 +1055,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>75</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>78</v>
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>82</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add art edits to sub-navigation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -119,7 +119,7 @@
     <t>img_1_caption</t>
   </si>
   <si>
-    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio. Texas Governor Rick Perry helped with the ribbon cutting ceremony on the highway near Lockhart, Texas in Caldwell County.</t>
+    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
   </si>
   <si>
     <t>img_1_credit</t>
@@ -128,6 +128,17 @@
     <t>Bob Daemmrich</t>
   </si>
   <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, [consectetur](http://) adipiscing elit. Ut condimentum erat at lacinia egestas. Curabitur vitae nunc molestie, gravida nisi eu, tempor augue. Vestibulum mollis at quam ac ultricies. Morbi maximus, ex sit amet ultrices porta, justo nulla sagittis sem, quis imperdiet nulla felis lacinia purus. Ut nisi velit, scelerisque at leo ac, rutrum molestie leo. Mauris efficitur nisl et pharetra sagittis. Nulla ornare sit amet erat non cursus. Sed sit amet diam nec elit tempor sollicitudin. Nunc rutrum, elit et pellentesque euismod, mauris erat dignissim augue, et scelerisque ipsum odio vel nibh. Aenean ac nisi nisi. Proin aliquam, justo nec dictum ullamcorper, lacus lectus ultricies ex, quis venenatis purus ligula et diam. Aliquam at magna purus. Curabitur pulvinar urna vel leo malesuada, eget volutpat dolor sollicitudin. Etiam imperdiet leo ut mollis venenatis.
+Lorem ipsum dolor sit amet, consectetur adipiscing elit. Ut condimentum erat at lacinia egestas. Curabitur vitae nunc molestie, gravida nisi eu, tempor augue. Vestibulum mollis at quam ac ultricies. Morbi maximus, ex sit amet ultrices porta, justo nulla sagittis sem, quis imperdiet nulla felis lacinia purus. Ut nisi velit, scelerisque at leo ac, rutrum molestie leo. Mauris efficitur nisl et pharetra sagittis. Nulla ornare sit amet erat non cursus. Sed sit amet diam nec elit tempor sollicitudin. Nunc rutrum, elit et pellentesque euismod, mauris erat dignissim augue, et scelerisque ipsum odio vel nibh. Aenean ac nisi nisi. Proin aliquam, justo nec dictum ullamcorper, lacus lectus ultricies ex, quis venenatis purus ligula et diam. Aliquam at magna purus. Curabitur pulvinar urna vel leo malesuada, eget volutpat dolor sollicitudin. Etiam imperdiet leo ut mollis venenatis.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -272,7 +283,7 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-tint</t>
+    <t>fa-bolt</t>
   </si>
   <si>
     <t>slug</t>
@@ -302,7 +313,7 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-group</t>
+    <t>fa-globe</t>
   </si>
   <si>
     <t>slug</t>
@@ -375,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -389,8 +400,13 @@
       <sz val="11.0"/>
       <color rgb="FF777777"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +417,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -422,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -434,6 +456,9 @@
       <alignment/>
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4" applyFill="1">
       <alignment/>
     </xf>
   </cellXfs>
@@ -535,42 +560,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -587,42 +612,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -700,7 +725,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="32.29"/>
+    <col min="2" customWidth="1" max="2" width="59.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -773,6 +798,17 @@
       </c>
       <c t="s" s="1" r="B9">
         <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>35</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -789,48 +825,51 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="125.0"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -847,42 +886,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c t="s" s="4" r="B4">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -899,42 +938,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -951,42 +990,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1003,42 +1042,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c t="s" s="5" r="B4">
+        <v>86</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1055,42 +1094,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create macro for meta data, implement on TRANSPO
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -107,7 +107,28 @@
     <t>transportation</t>
   </si>
   <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/shale-life</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>Just a test</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
     <t>lead_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>img_1</t>
@@ -560,42 +581,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>106</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -612,42 +633,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -775,47 +796,77 @@
       <c t="s" s="1" r="A6">
         <v>28</v>
       </c>
+      <c t="s" s="3" r="B6">
+        <v>29</v>
+      </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>29</v>
-      </c>
-      <c t="s" s="3" r="B7">
         <v>30</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>31</v>
-      </c>
-      <c t="s" s="1" r="B8">
         <v>32</v>
+      </c>
+      <c t="s" s="3" r="B8">
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="B9">
         <v>34</v>
+      </c>
+      <c t="s" s="3" r="B9">
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>35</v>
-      </c>
-      <c t="s" s="1" r="B10">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c t="s" s="3" r="B10">
         <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>38</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -831,45 +882,45 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -886,42 +937,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c t="s" s="4" r="B4">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -938,42 +989,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -990,42 +1041,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>78</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1042,42 +1093,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c t="s" s="5" r="B4">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1094,42 +1145,42 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add text to overview, create navigation to sections
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -23,6 +23,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t>project_title</t>
+  </si>
+  <si>
+    <t>The Legacy of Gov. Rick Perry</t>
+  </si>
+  <si>
+    <t>project_subtitle</t>
+  </si>
+  <si>
+    <t>After 14 years in the governor's office, Rick Perry leaves a lasting mark on Texas. </t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
@@ -32,7 +47,7 @@
     <t>headline</t>
   </si>
   <si>
-    <t>The Lasting Impact of Gov. Rick Perry</t>
+    <t>6 Things Texans Won't Forget About Rick Perry</t>
   </si>
   <si>
     <t>byline</t>
@@ -59,22 +74,55 @@
     <t>index</t>
   </si>
   <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>When Gov. Rick Perry leaves office next month, he will wrap up a three-decade stretch in state elective office that has concluded with his serving as the longest-serving governor in Texas history. 
+Mr. Perry’s 14-year tenure in the state’s highest office coincided with the ever-tightening grip of Republican rule, sweeping conservative reforms and more than a few controversies.
+It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Mr. Perry’s reign, and it added more people than any other state between 2000 and 2010 and has continued to grow.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_1b</t>
+  </si>
+  <si>
+    <t>From his first legislative session as governor in 2001, when Mr. Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used rare emergency powers to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
+Boiling down Mr. Perry’s legacy into a few bullet points is not easy and will undoubtedly leave supporters and detractors alike unsatisfied.
+But memories fade, and not every event that seems newsworthy today will stand out in the history books or become part of the state’s collective political memory. (And there could be a new set of mileposts on a future legacy tour if Mr. Perry runs for president again — a move he is currently considering).
+With those caveats, here are six things people will probably remember years after Mr. Perry has left the Texas Governor’s Mansion.</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Health Care</t>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>headline</t>
   </si>
   <si>
-    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>text_2_header</t>
+  </si>
+  <si>
+    <t>Longevity</t>
   </si>
   <si>
     <t>byline</t>
   </si>
   <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -83,139 +131,131 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-plus-square</t>
+    <t>fa-car</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>health-care</t>
+    <t>transportation</t>
   </si>
   <si>
     <t>share_url</t>
   </si>
   <si>
+    <t>trib.it/shale-life</t>
+  </si>
+  <si>
+    <t>When Mr. Perry hands over power to Gov.-Elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
+Bill Clements, elected in 1978 as the first Republican governor since Reconstruction, was the first to serve two full four-year terms, but they weren’t consecutive. In 1998, George W. Bush became the first governor to win two consecutive four-year terms, but he left for Washington halfway through the second one.
+Mr. Perry, who had been elected lieutenant governor when Mr. Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
+At last count, Mr. Perry had made more than 8,000 appointments, allowing him to put his conservative stamp on every corner of state government — all from a perch that the state’s founding fathers, suspicious of centralized authority, intentionally weakened.
+Mr. Perry championed sweeping curbs on lawsuits, some of the most stringent abortion limits in the nation, the strictest voter ID statute in the country, a constitutional ban on gay marriage and steep cuts to programs once seen as sacrosanct, including public education and women’s health programs.
+People crossed Mr. Perry at their peril, whether they were appointees who dared support a political challenger or lawmakers who opposed his legislative program. Jim Henson, a Texas Tribune pollster and director of the Texas Politics Project at the University of Texas at Austin, said Mr. Perry expanded the powers of the governor’s office “in a way that is certainly not contemplated in the Texas Constitution nor really in the political culture of the state.”
+“I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3_header</t>
+  </si>
+  <si>
+    <t>The Texas Miracle</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
+    <t>Just a test</t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>Also, just a test</t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
     <t>lead_art</t>
   </si>
   <si>
+    <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
+Critics will find plenty wrong with a state that has the highest percentage of uninsured residents in the nation, produces more greenhouse gas emissions than any other state and has led the nation in workplace fatalities for 10 of the last 14 years. 
+But any governor in America would be happy to boast, as Mr. Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
+From 2003 to 2013, Texas produced a third of the net new jobs in America. It has been the top exporting state for the last 12 years in a row, and recently Texas surpassed California as the top exporter of technology, according to the TechAmerica Foundation. 
+Under Mr. Perry, Texas has been given top honors five times for corporate relocations by Site Selection Magazine, and the governor credits the state’s pro-business policies — including millions in tax subsidies used to entice companies such as Toyota to set up its American headquarters here— as a major factor driving the boom.  
+Detractors note the corporate relocations account for a tiny percentage of the jobs Texas has created and say the state — brimming with shale oil — would rank as a major employment center no matter who was governor. 
+Do not expect that, or anything else, to stop Mr. Perry from bragging about the Texas Miracle anytime soon, though.
+</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4_header</t>
+  </si>
+  <si>
+    <t>The Margins Tax
+</t>
+  </si>
+  <si>
+    <t>text_4</t>
+  </si>
+  <si>
     <t>img_1</t>
   </si>
   <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
     <t>img_1_caption</t>
   </si>
   <si>
+    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
+  </si>
+  <si>
     <t>img_1_credit</t>
   </si>
   <si>
+    <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
+At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.
+The solution Mr. Perry advocated: Craft a business tax that applied to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
+The plan drew plenty of foes. Democrats said it still left school badly underfunded. And Republican activists complained (and still do) that the revamped business levy, applied to gross receipts minus certain deductions, constituted an unconstitutional income tax.
+But Mr. Perry got the plan passed with bipartisan support, the schools stayed open and businesses that used to pay nothing became taxpayers for the first time. 
+“Folks may not have liked the end result, but the margins tax, when you look how it came about, it was really Perry’s finest hour,” said Dale Craymer, president of the business-backed Texas Taxpayers and Research Association. “It was a crisis averted.”
+The tax is still unpopular and Republican leaders want to modify it or even get rid of it, but they are likely to find that it is easier said than done.
+</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>project_title</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>The Legacy of Gov. Rick Perry</t>
-  </si>
-  <si>
-    <t>project_subtitle</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>After 14 years in the governor's office, Rick Perry leaves a lasting mark on Texas. </t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/shale-life</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>Just a test</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Also, just a test</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
+    <t>text_5_header</t>
+  </si>
+  <si>
+    <t>The Oops Moment</t>
+  </si>
+  <si>
+    <t>text_5</t>
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, [consectetur](http://) adipiscing elit. Ut condimentum erat at lacinia egestas. Curabitur vitae nunc molestie, gravida nisi eu, tempor augue. Vestibulum mollis at quam ac ultricies. Morbi maximus, ex sit amet ultrices porta, justo nulla sagittis sem, quis imperdiet nulla felis lacinia purus. Ut nisi velit, scelerisque at leo ac, rutrum molestie leo. Mauris efficitur nisl et pharetra sagittis. Nulla ornare sit amet erat non cursus. Sed sit amet diam nec elit tempor sollicitudin. Nunc rutrum, elit et pellentesque euismod, mauris erat dignissim augue, et scelerisque ipsum odio vel nibh. Aenean ac nisi nisi. Proin aliquam, justo nec dictum ullamcorper, lacus lectus ultricies ex, quis venenatis purus ligula et diam. Aliquam at magna purus. Curabitur pulvinar urna vel leo malesuada, eget volutpat dolor sollicitudin. Etiam imperdiet leo ut mollis venenatis.
@@ -226,9 +266,123 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>It’s still hard to watch. 
+For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Mr. Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
+“I would do away with the Education, the, uh, Commerce, and, let’s see,” he said, looking down at his notes for any clues. “I can’t. The third one I can’t. Sorry. Oops.” 
+Commentators pronounced Mr. Perry’s presidential effort dead and in the ensuing weeks, late night comedians made the Texas governor the butt of endless jokes.
+After his inevitable withdrawal from the race weeks later, Mr. Perry blamed health problems and a lack of preparation. Now, with a bespectacled new look, more time to study up and the benefit of hindsight, he is promising a better performance should he run for president again in 2016.
+The significance of the “oops” moment is often overstated in recaps of Mr. Perry’s first presidential bid. According to polling data, his popularity had already declined significantly following fumbles in a previous debate and a strongly worded defense of a Texas policy allowing the children of undocumented immigrants in-state tuition for public colleges and universities. 
+But like Vice President Dan Quayle’s misspelling of potato (with an “e”) in a school classroom in 1992, or Democrat Howard Dean’s primal scream as his presidential campaign was going down the toilet in 2004, Mr. Perry’s 2011 debate meltdown has earned a permanent spot in the political blooper hall of fame.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_6_header</t>
+  </si>
+  <si>
+    <t>The Indictment</t>
+  </si>
+  <si>
+    <t>text_6</t>
+  </si>
+  <si>
+    <t>Political forecasts called for smooth sailing as Mr. Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
+Now, just like the governor’s often messy battles with political rivals and his no-holds-barred approach to legislative negotiation, Mr. Perry is spending his remaining days in office at the center of a swirling controversy he helped create. 
+On Aug. 15, a grand jury indicted Mr. Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
+Mr. Perry blasted the prosecution as a politically motivated “farce,” and has trotted out legal scholars from both sides of the spectrum to criticize it.
+No matter what happens, Mr. Perry’s 11th-hour ride through the criminal justice system guarantees a mention in the history books. He is the first governor since James “Pa” Ferguson to get indicted, and the uncommonly brash way he has confronted the allegations provided a unique twist to the way potential presidential contenders handle criminal justice challenges. 
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_7_header</t>
+  </si>
+  <si>
+    <t>Swagger</t>
+  </si>
+  <si>
+    <t>text_7</t>
+  </si>
+  <si>
+    <t>Granted, swagger is not an event, a policy accomplishment or a political milestone. It is a style — a cocky way of walking, talking and conducting business. And Mr. Perry has made it his calling card.
+When a coyote threatened his Labrador puppy in 2010, Mr. Perry did not grab the pooch and run. He pulled out his pistol and shot. The incident later made the papers. 
+When Mr. Perry was courting the Tea Party in 2009, he did not just promise to get the federal government off the people’s backs. He flirted with secession. 
+And when Mr. Perry got booked on felony charges at the Travis County Courthouse this year, he did not slip in quietly through the back door. He held a press conference on the courthouse square. After smiling for his mug shot, he went out for ice cream in downtown Austin and posted a picture online to show he was keeping his cool. 
+Later, through his political action committee, he sold T-shirts with that same mug shot plastered on the front.
+Love Mr. Perry or hate him, that is swagger.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>Higher Education</t>
   </si>
   <si>
@@ -460,148 +614,148 @@
     <t>Criminal Justice</t>
   </si>
   <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Terri Langford](http://www.texastribune.org/about/staff/terri-langford/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-legal</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>criminal-justice</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>headline</t>
   </si>
   <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
     <t>Texas Enterprise Fund</t>
   </si>
   <si>
     <t>byline</t>
   </si>
   <si>
-    <t>[Terri Langford](http://www.texastribune.org/about/staff/terri-langford/)</t>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
   </si>
   <si>
     <t>headline</t>
   </si>
   <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-bolt</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
     <t>icon</t>
   </si>
   <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>fa-legal</t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>fa-money</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>criminal-justice</t>
-  </si>
-  <si>
-    <t>fa-money</t>
+    <t>texas-enterprise-fund</t>
   </si>
   <si>
     <t>share_url</t>
   </si>
   <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
     <t>slug</t>
   </si>
   <si>
-    <t>texas-enterprise-fund</t>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>share_url</t>
   </si>
   <si>
     <t>tweet_text</t>
   </si>
   <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>text_1</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-bolt</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>energy</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
   </si>
   <si>
     <t>facebook_text</t>
@@ -692,11 +846,11 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
       <alignment/>
@@ -763,6 +917,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="53.14"/>
+    <col min="2" customWidth="1" max="2" width="26.29"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
@@ -776,7 +934,7 @@
       <c t="s" s="1" r="A2">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c t="s" s="2" r="B2">
         <v>3</v>
       </c>
     </row>
@@ -784,39 +942,9 @@
       <c t="s" s="1" r="A3">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>6</v>
-      </c>
-      <c t="s" s="2" r="B4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>10</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -829,87 +957,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>178</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>180</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>185</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c t="s" s="5" r="B4">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>189</v>
+        <v>223</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>190</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>191</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>192</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>193</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>194</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>195</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>196</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>197</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>198</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>199</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -926,87 +1054,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>144</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>146</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>149</v>
+        <v>209</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>151</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>155</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>157</v>
+        <v>214</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>159</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>161</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>164</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>166</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>168</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>170</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>172</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>174</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>176</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>179</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1015,6 +1143,348 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="59.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>29</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>31</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>35</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>37</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>48</v>
+      </c>
+      <c t="s" s="3" r="B9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>50</v>
+      </c>
+      <c t="s" s="3" r="B10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>57</v>
+      </c>
+      <c t="s" s="3" r="B11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>61</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>65</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+  </hyperlinks>
+  <drawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>11</v>
+      </c>
+      <c t="s" s="3" r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="C7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="C8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>41</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="C12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>68</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>75</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>78</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>79</v>
+      </c>
+      <c s="1" r="C19"/>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1026,270 +1496,94 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>18</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>20</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>23</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>24</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>25</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>26</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>27</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>30</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" customWidth="1" max="1" width="53.14"/>
-    <col min="2" customWidth="1" max="2" width="26.29"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>35</v>
-      </c>
-      <c t="s" s="3" r="B2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" customWidth="1" max="2" width="59.71"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>38</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>40</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>41</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>43</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>47</v>
-      </c>
-      <c t="s" s="2" r="B6">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="B7">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>53</v>
-      </c>
-      <c t="s" s="2" r="B9">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>56</v>
-      </c>
-      <c t="s" s="2" r="B10">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>58</v>
-      </c>
-      <c t="s" s="2" r="B11">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>60</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>62</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>64</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>65</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-  </hyperlinks>
-  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1302,87 +1596,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>68</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>69</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>72</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>73</v>
-      </c>
-      <c t="s" s="4" r="B4">
-        <v>74</v>
+        <v>128</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>76</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>78</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>79</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>80</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>81</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>82</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>83</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>85</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1399,87 +1693,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>88</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>91</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>92</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>93</v>
+        <v>109</v>
+      </c>
+      <c t="s" s="4" r="B4">
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>95</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>96</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>101</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>104</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1496,87 +1790,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>106</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>107</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>110</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>114</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>115</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>116</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>117</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>118</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>119</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>120</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>121</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>122</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>123</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1593,87 +1887,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>125</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>126</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>129</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>130</v>
+        <v>166</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>131</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>133</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>134</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>135</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>136</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>137</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>138</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>139</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>140</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>141</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>142</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1690,87 +1984,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>147</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>150</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>156</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>160</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>165</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>169</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>171</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>173</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>175</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>181</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>183</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>186</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more media, fix fitvids load
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -62,200 +62,215 @@
     <t>http://www.texastribune.org/about/staff/jay-root</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>icon</t>
   </si>
   <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
     <t>fa-star</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
     <t>index</t>
   </si>
   <si>
+    <t>text_intro</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/shale-life</t>
+  </si>
+  <si>
+    <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that has concluded with his serving as the longest-serving governor in Texas history. 
+Perry’s 14-year tenure in the state’s highest office coincided with the ever-tightening grip of Republican rule, sweeping conservative reforms and more than a few controversies.
+It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Perry’s reign, and it added more people than any other state between 2000 and 2010 and has continued to grow.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_introb</t>
+  </si>
+  <si>
+    <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
+Boiling down Perry’s legacy into a few bullet points isn’t easy and will undoubtedly leave supporters and detractors alike unsatisfied.
+But memories fade, and not every event that seems newsworthy today will stand out in the history books or become part of the state’s collective political memory. (And there could be a new set of mileposts on a future legacy tour if Perry runs for president again — a move he is currently considering.)
+With those caveats, here are six things people will probably remember years after Perry has left the Texas Governor’s Mansion.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_1_header</t>
+  </si>
+  <si>
+    <t>Longevity</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>Just a test</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>When Gov. Rick Perry leaves office next month, he will wrap up a three-decade stretch in state elective office that has concluded with his serving as the longest-serving governor in Texas history. 
-Mr. Perry’s 14-year tenure in the state’s highest office coincided with the ever-tightening grip of Republican rule, sweeping conservative reforms and more than a few controversies.
-It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Mr. Perry’s reign, and it added more people than any other state between 2000 and 2010 and has continued to grow.
+    <t>Also, just a test</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven and a half years in office, back when the terms lasted only two years.
+Bill Clements, elected in 1978 as the first Republican governor since Reconstruction, was the first to serve two full four-year terms, but they were not consecutive. In 1998, George W. Bush became the first governor to win two consecutive four-year terms, but he left for Washington halfway through the second one.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_1b</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist(. 
+At last count, Perry had made more than 8,000 appointments, allowing him to put his conservative stamp on every corner of state government — all from a perch that the state’s founding fathers, suspicious of centralized authority, intentionally weakened.
+Perry championed sweeping curbs on lawsuits, some of the most stringent abortion limits in the nation, the strictest voter ID statute in the country, a constitutional ban on gay marriage and steep cuts to programs once seen as sacrosanct, including public education and women’s health programs.
+People crossed Perry at their peril, whether they were appointees who [dared support](http://www.yourhoustonnews.com/courier/news/tech-regent-perry-ally-pressured-him-to-resign/article_07eed112-5a72-5e72-bda2-5152511a43a5.html?mode=jqm) a political challenger or lawmakers who opposed his legislative program. Jim Henson, a Texas Tribune pollster and director of the Texas Politics Project at the University of Texas at Austin, said Perry expanded the powers of the governor’s office “in a way that is certainly not contemplated in the Texas Constitution nor really in the political culture of the state.”
+“I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2_header</t>
+  </si>
+  <si>
+    <t>The Texas Miracle</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
+  </si>
+  <si>
+    <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
+Critics will find plenty wrong with a state that has the highest percentage of [uninsured](http://kxan.com/2014/09/16/texas-no-1-for-uninsured-rate-again/) residents in the nation, produces [more](http://www.nytimes.com/2014/07/13/us/texas-leader-in-greenhouse-gases-stands-vulnerable-to-their-effects.html?_r=1) greenhouse gas emissions than any other state and has [led the nation](https://www.texastribune.org/2014/09/11/workplace-deaths-decline-texas-still-no-1/) in workplace fatalities for 10 of the last 14 years. 
+But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
+From 2003 to 2013, Texas produced [a third](http://www.politifact.com/texas/statements/2013/may/09/rick-perry/rick-perry-says-texas-accounted-33-percent-nations/) of the net new jobs in America. It has been the [top exporting state](http://governor.state.tx.us/news/press-release/19379/) for the last 12 years in a row, and recently Texas surpassed California as the top exporter of technology, [according to](http://www.bizjournals.com/sanantonio/blog/2014/02/texas-takes-the-lead-in-technology-exports.html) the TechAmerica Foundation. 
+Under Perry, Texas has been given top honors five times for corporate relocations by Site Selection magazine, and the governor credits the state’s pro-business policies — including millions in tax subsidies used to entice companies such as Toyota to [set up its American headquarters](http://corporatenews.pressroom.toyota.com/releases/toyota+new+north+american+headquarters.htm) here — as a major factor driving the boom.  
+Detractors note that the corporate relocations account for a tiny percentage of the jobs Texas has created and say the state — brimming with shale oil — would rank as a major employment center no matter who was governor. 
+Don’t expect that, or anything else, to stop Perry from bragging about the Texas Miracle anytime soon, though.
 </t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>text_1b</t>
-  </si>
-  <si>
-    <t>From his first legislative session as governor in 2001, when Mr. Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used rare emergency powers to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
-Boiling down Mr. Perry’s legacy into a few bullet points is not easy and will undoubtedly leave supporters and detractors alike unsatisfied.
-But memories fade, and not every event that seems newsworthy today will stand out in the history books or become part of the state’s collective political memory. (And there could be a new set of mileposts on a future legacy tour if Mr. Perry runs for president again — a move he is currently considering).
-With those caveats, here are six things people will probably remember years after Mr. Perry has left the Texas Governor’s Mansion.</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Headline</t>
-  </si>
-  <si>
-    <t>text_2_header</t>
-  </si>
-  <si>
-    <t>Longevity</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>text_2</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/shale-life</t>
-  </si>
-  <si>
-    <t>When Mr. Perry hands over power to Gov.-Elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
-Bill Clements, elected in 1978 as the first Republican governor since Reconstruction, was the first to serve two full four-year terms, but they weren’t consecutive. In 1998, George W. Bush became the first governor to win two consecutive four-year terms, but he left for Washington halfway through the second one.
-Mr. Perry, who had been elected lieutenant governor when Mr. Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
-At last count, Mr. Perry had made more than 8,000 appointments, allowing him to put his conservative stamp on every corner of state government — all from a perch that the state’s founding fathers, suspicious of centralized authority, intentionally weakened.
-Mr. Perry championed sweeping curbs on lawsuits, some of the most stringent abortion limits in the nation, the strictest voter ID statute in the country, a constitutional ban on gay marriage and steep cuts to programs once seen as sacrosanct, including public education and women’s health programs.
-People crossed Mr. Perry at their peril, whether they were appointees who dared support a political challenger or lawmakers who opposed his legislative program. Jim Henson, a Texas Tribune pollster and director of the Texas Politics Project at the University of Texas at Austin, said Mr. Perry expanded the powers of the governor’s office “in a way that is certainly not contemplated in the Texas Constitution nor really in the political culture of the state.”
-“I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)
-</t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>img_1_credit</t>
   </si>
   <si>
     <t>text_3_header</t>
   </si>
   <si>
-    <t>The Texas Miracle</t>
-  </si>
-  <si>
-    <t>text_3</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>Just a test</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Also, just a test</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
-Critics will find plenty wrong with a state that has the highest percentage of uninsured residents in the nation, produces more greenhouse gas emissions than any other state and has led the nation in workplace fatalities for 10 of the last 14 years. 
-But any governor in America would be happy to boast, as Mr. Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
-From 2003 to 2013, Texas produced a third of the net new jobs in America. It has been the top exporting state for the last 12 years in a row, and recently Texas surpassed California as the top exporter of technology, according to the TechAmerica Foundation. 
-Under Mr. Perry, Texas has been given top honors five times for corporate relocations by Site Selection Magazine, and the governor credits the state’s pro-business policies — including millions in tax subsidies used to entice companies such as Toyota to set up its American headquarters here— as a major factor driving the boom.  
-Detractors note the corporate relocations account for a tiny percentage of the jobs Texas has created and say the state — brimming with shale oil — would rank as a major employment center no matter who was governor. 
-Do not expect that, or anything else, to stop Mr. Perry from bragging about the Texas Miracle anytime soon, though.
-</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4_header</t>
+    <t>Bob Daemmrich</t>
   </si>
   <si>
     <t>The Margins Tax
 </t>
   </si>
   <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
+At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3b</t>
+  </si>
+  <si>
+    <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applied to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
+The plan drew plenty of foes. Democrats said it still left schools badly underfunded. And Republican activists complained (and still do) that the revamped business levy, applied to gross receipts minus certain deductions, constituted an unconstitutional income tax.
+But Perry got the plan passed with bipartisan support, the schools stayed open and businesses that used to pay nothing became taxpayers for the first time. 
+“Folks may not have liked the end result, but the margins tax, when you look how it came about, it was really Perry’s finest hour,” said Dale Craymer, president of the business-backed Texas Taxpayers and Research Association. “It was a crisis averted.”
+The tax is still unpopular, and Republican leaders want to modify it or even [get rid of it](http://www.craigestes.org/2014/11/18/texas-business-tax-aka-the-margin-tax-should-be-repealed/), but they’re likely to find that it’s easier said than done.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4_header</t>
+  </si>
+  <si>
+    <t>The Oops Moment</t>
+  </si>
+  <si>
     <t>text_4</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
-At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.
-The solution Mr. Perry advocated: Craft a business tax that applied to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
-The plan drew plenty of foes. Democrats said it still left school badly underfunded. And Republican activists complained (and still do) that the revamped business levy, applied to gross receipts minus certain deductions, constituted an unconstitutional income tax.
-But Mr. Perry got the plan passed with bipartisan support, the schools stayed open and businesses that used to pay nothing became taxpayers for the first time. 
-“Folks may not have liked the end result, but the margins tax, when you look how it came about, it was really Perry’s finest hour,” said Dale Craymer, president of the business-backed Texas Taxpayers and Research Association. “It was a crisis averted.”
-The tax is still unpopular and Republican leaders want to modify it or even get rid of it, but they are likely to find that it is easier said than done.
-</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>text_5_header</t>
-  </si>
-  <si>
-    <t>The Oops Moment</t>
-  </si>
-  <si>
-    <t>text_5</t>
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, [consectetur](http://) adipiscing elit. Ut condimentum erat at lacinia egestas. Curabitur vitae nunc molestie, gravida nisi eu, tempor augue. Vestibulum mollis at quam ac ultricies. Morbi maximus, ex sit amet ultrices porta, justo nulla sagittis sem, quis imperdiet nulla felis lacinia purus. Ut nisi velit, scelerisque at leo ac, rutrum molestie leo. Mauris efficitur nisl et pharetra sagittis. Nulla ornare sit amet erat non cursus. Sed sit amet diam nec elit tempor sollicitudin. Nunc rutrum, elit et pellentesque euismod, mauris erat dignissim augue, et scelerisque ipsum odio vel nibh. Aenean ac nisi nisi. Proin aliquam, justo nec dictum ullamcorper, lacus lectus ultricies ex, quis venenatis purus ligula et diam. Aliquam at magna purus. Curabitur pulvinar urna vel leo malesuada, eget volutpat dolor sollicitudin. Etiam imperdiet leo ut mollis venenatis.
@@ -263,79 +278,144 @@
 </t>
   </si>
   <si>
+    <t>It’s still hard to watch. </t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>It’s still hard to watch. 
-For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Mr. Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
-“I would do away with the Education, the, uh, Commerce, and, let’s see,” he said, looking down at his notes for any clues. “I can’t. The third one I can’t. Sorry. Oops.” 
-Commentators pronounced Mr. Perry’s presidential effort dead and in the ensuing weeks, late night comedians made the Texas governor the butt of endless jokes.
-After his inevitable withdrawal from the race weeks later, Mr. Perry blamed health problems and a lack of preparation. Now, with a bespectacled new look, more time to study up and the benefit of hindsight, he is promising a better performance should he run for president again in 2016.
-The significance of the “oops” moment is often overstated in recaps of Mr. Perry’s first presidential bid. According to polling data, his popularity had already declined significantly following fumbles in a previous debate and a strongly worded defense of a Texas policy allowing the children of undocumented immigrants in-state tuition for public colleges and universities. 
-But like Vice President Dan Quayle’s misspelling of potato (with an “e”) in a school classroom in 1992, or Democrat Howard Dean’s primal scream as his presidential campaign was going down the toilet in 2004, Mr. Perry’s 2011 debate meltdown has earned a permanent spot in the political blooper hall of fame.
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4b</t>
+  </si>
+  <si>
+    <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
+“I would do away with the Education, the, uh, Commerce and, let’s see,” he said, looking down at his notes for any clues. “I can’t. The third one I can’t. Sorry. Oops.” 
+Commentators pronounced Perry’s presidential effort dead, and in the ensuing weeks, late-night comedians made the Texas governor the butt of endless jokes.
+After his inevitable withdrawal from the race weeks later, Perry blamed health problems and a lack of preparation. Now, with a bespectacled new look, more time to study up and the benefit of hindsight, he’s promising a better performance should he run for president again in 2016.
+The significance of the “oops” moment is often overstated in recaps of Perry’s first presidential bid. According to polling data, his popularity had already declined significantly following fumbles in a previous debate and a strongly worded defense of a Texas policy allowing the children of undocumented immigrants in-state tuition for public colleges and universities. 
+But like Vice President Dan Quayle’s [misspelling](http://content.time.com/time/specials/packages/article/0,28804,1834600_1834604_1834585,00.html) of potato (with an “e”) in a school classroom in 1992, or Democrat Howard Dean’s primal scream as his presidential campaign was going down the toilet in 2004, Perry’s 2011 debate meltdown has earned a permanent spot in the political blooper hall of fame.
 </t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
+    <t>text_5_header</t>
+  </si>
+  <si>
+    <t>The Indictment</t>
+  </si>
+  <si>
+    <t>text_5</t>
+  </si>
+  <si>
+    <t>Political forecasts called for smooth sailing as Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
+Now, just like the governor’s often messy battles with political rivals and his no-holds-barred approach to legislative negotiation, Perry is spending his remaining days in office at the center of a swirling controversy he helped create. 
+On Aug. 15, a grand jury indicted Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
+Perry blasted the prosecution as a politically motivated “farce,” and has trotted out [legal scholars](https://www.texastribune.org/2014/11/10/bipartisan-group-lawyers-want-perry-case-dismissed/) from both sides of the spectrum to criticize it.
+No matter what happens, Perry’s 11th-hour ride through the criminal justice system guarantees a mention in the history books. He’s the [first governor since James “Pa” Ferguson](http://www.texastribune.org/2014/08/17/you-couldnt-make-stuff-1917-either/) to get indicted, and the uncommonly brash way he has confronted the allegations provided a unique twist to the way potential presidential contenders handle criminal justice challenges. 
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>text_6_header</t>
   </si>
   <si>
-    <t>The Indictment</t>
+    <t>Swagger</t>
   </si>
   <si>
     <t>text_6</t>
   </si>
   <si>
-    <t>Political forecasts called for smooth sailing as Mr. Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
-Now, just like the governor’s often messy battles with political rivals and his no-holds-barred approach to legislative negotiation, Mr. Perry is spending his remaining days in office at the center of a swirling controversy he helped create. 
-On Aug. 15, a grand jury indicted Mr. Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
-Mr. Perry blasted the prosecution as a politically motivated “farce,” and has trotted out legal scholars from both sides of the spectrum to criticize it.
-No matter what happens, Mr. Perry’s 11th-hour ride through the criminal justice system guarantees a mention in the history books. He is the first governor since James “Pa” Ferguson to get indicted, and the uncommonly brash way he has confronted the allegations provided a unique twist to the way potential presidential contenders handle criminal justice challenges. 
+    <t>Granted, swagger is not an event, a policy accomplishment or a political milestone. It’s a style — a cocky way of walking, talking and conducting business. And Perry has made it his calling card.
+When a coyote threatened his Labrador puppy in 2010, Perry didn’t grab the pooch and run. He pulled out his pistol and shot. The incident later made the papers. 
+When Perry was courting the Tea Party in 2009, he did not just promise to get the federal government off the people’s backs. He flirted with secession. 
+And when Perry got booked on felony charges at the Travis County Courthouse this year, he did not slip in quietly through the back door. He held a press conference on the courthouse square. After smiling for his mug shot, he went out for ice cream near downtown Austin and posted a picture online to show he was keeping his cool. 
+Later, through his political action committee, he sold T-shirts with that same mug shot plastered on the front.
+Love Perry or hate him, that’s swagger.
 </t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>text_7_header</t>
-  </si>
-  <si>
-    <t>Swagger</t>
-  </si>
-  <si>
-    <t>text_7</t>
-  </si>
-  <si>
-    <t>Granted, swagger is not an event, a policy accomplishment or a political milestone. It is a style — a cocky way of walking, talking and conducting business. And Mr. Perry has made it his calling card.
-When a coyote threatened his Labrador puppy in 2010, Mr. Perry did not grab the pooch and run. He pulled out his pistol and shot. The incident later made the papers. 
-When Mr. Perry was courting the Tea Party in 2009, he did not just promise to get the federal government off the people’s backs. He flirted with secession. 
-And when Mr. Perry got booked on felony charges at the Travis County Courthouse this year, he did not slip in quietly through the back door. He held a press conference on the courthouse square. After smiling for his mug shot, he went out for ice cream in downtown Austin and posted a picture online to show he was keeping his cool. 
-Later, through his political action committee, he sold T-shirts with that same mug shot plastered on the front.
-Love Mr. Perry or hate him, that is swagger.
-</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Health Care</t>
+    <t>Higher Education</t>
   </si>
   <si>
     <t>headline</t>
   </si>
   <si>
-    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
-  </si>
-  <si>
     <t>byline</t>
   </si>
   <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -344,13 +424,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-plus-square</t>
+    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>health-care</t>
+    <t>higher-education</t>
   </si>
   <si>
     <t>share_url</t>
@@ -383,7 +463,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Higher Education</t>
+    <t>Public Education</t>
   </si>
   <si>
     <t>headline</t>
@@ -392,7 +472,7 @@
     <t>byline</t>
   </si>
   <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -401,13 +481,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-graduation-cap</t>
+    <t>fa-book</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>higher-education</t>
+    <t>public-education</t>
   </si>
   <si>
     <t>share_url</t>
@@ -440,7 +520,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Public Education</t>
+    <t>Environment</t>
   </si>
   <si>
     <t>headline</t>
@@ -449,7 +529,7 @@
     <t>byline</t>
   </si>
   <si>
-    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
+    <t>[Neena Satija](http://www.texastribune.org/about/staff/neena-satija/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -458,13 +538,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-book</t>
+    <t>fa-tree</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>public-education</t>
+    <t>environment</t>
   </si>
   <si>
     <t>share_url</t>
@@ -497,7 +577,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Environment</t>
+    <t>Energy</t>
   </si>
   <si>
     <t>headline</t>
@@ -506,7 +586,7 @@
     <t>byline</t>
   </si>
   <si>
-    <t>[Neena Satija](http://www.texastribune.org/about/staff/neena-satija/)</t>
+    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -515,13 +595,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-tree</t>
+    <t>fa-bolt</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>environment</t>
+    <t>energy</t>
   </si>
   <si>
     <t>share_url</t>
@@ -641,121 +721,64 @@
     <t>share_url</t>
   </si>
   <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>topic</t>
+    <t>Texas Enterprise Fund</t>
   </si>
   <si>
     <t>headline</t>
   </si>
   <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-money</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>texas-enterprise-fund</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
     <t>tweet_text</t>
-  </si>
-  <si>
-    <t>Texas Enterprise Fund</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-bolt</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-money</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>texas-enterprise-fund</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>energy</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>text_1</t>
   </si>
   <si>
     <t>facebook_text</t>
@@ -957,87 +980,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>191</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>199</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>203</v>
-      </c>
-      <c t="s" s="5" r="B4">
-        <v>204</v>
+        <v>213</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>214</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1054,87 +1077,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>213</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>215</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>216</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>222</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>228</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1154,101 +1177,101 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c t="s" s="3" r="B9">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c t="s" s="3" r="B10">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c t="s" s="3" r="B11">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -1261,13 +1284,13 @@
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1282,6 +1305,109 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="125.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>94</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>96</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>97</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1325,129 +1451,132 @@
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>42</v>
+        <v>50</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="C12">
         <v>53</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>55</v>
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>62</v>
-      </c>
-      <c t="s" s="1" r="C14">
         <v>64</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="B15">
         <v>67</v>
       </c>
+      <c t="s" s="1" r="C15">
+        <v>68</v>
+      </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="B16">
+        <v>70</v>
+      </c>
+      <c t="s" s="1" r="C16">
         <v>71</v>
-      </c>
-      <c t="s" s="1" r="C16">
-        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B17">
         <v>73</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B18">
         <v>76</v>
@@ -1458,22 +1587,51 @@
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>79</v>
-      </c>
-      <c s="1" r="C19"/>
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>81</v>
+      </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>82</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>84</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1481,109 +1639,6 @@
     <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" customWidth="1" max="2" width="125.0"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>83</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>92</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1596,87 +1651,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1693,87 +1748,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c t="s" s="4" r="B4">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1790,87 +1845,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>152</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1887,87 +1942,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>166</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>167</v>
+        <v>175</v>
+      </c>
+      <c t="s" s="5" r="B4">
+        <v>176</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1984,87 +2039,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>180</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>181</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>182</v>
+        <v>229</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>184</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>186</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>188</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>189</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>194</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>197</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>200</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>202</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>205</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>207</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>208</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>210</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add energy, health-care templates
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -23,97 +23,147 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+  </si>
+  <si>
+    <t>6 Things Texans Won't Forget About Rick Perry</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>Jay Root</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>reporter_bio</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>http://www.texastribune.org/about/staff/jay-root</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>text_intro</t>
+  </si>
+  <si>
     <t>project_title</t>
   </si>
   <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>The Legacy of Gov. Rick Perry</t>
   </si>
   <si>
+    <t>text_introb</t>
+  </si>
+  <si>
     <t>project_subtitle</t>
   </si>
   <si>
     <t>After 14 years in the governor's office, Rick Perry leaves a lasting mark on Texas. </t>
   </si>
   <si>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-star</t>
+  </si>
+  <si>
+    <t>text_1_header</t>
+  </si>
+  <si>
+    <t>Medicaid Expansion</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>text_intro</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
+  </si>
+  <si>
     <t>topic</t>
   </si>
   <si>
-    <t>Overview</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>6 Things Texans Won't Forget About Rick Perry</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>Jay Root</t>
-  </si>
-  <si>
-    <t>reporter_bio</t>
-  </si>
-  <si>
-    <t>http://www.texastribune.org/about/staff/jay-root</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A toll road plan &amp;ldquo;as big as Texas&amp;rdquo;</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>fa-star</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>text_intro</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/shale-life</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
+    <t>text_1b</t>
   </si>
   <si>
     <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that has concluded with his serving as the longest-serving governor in Texas history. 
@@ -121,16 +171,31 @@
 It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Perry’s reign, and it added more people than any other state between 2000 and 2010 and has continued to grow.</t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>byline</t>
   </si>
   <si>
     <t>text_introb</t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>Just a test</t>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
+  </si>
+  <si>
+    <t>byline</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
@@ -140,28 +205,36 @@
 </t>
   </si>
   <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>Also, just a test</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.
+Quisque euismod ligula neque, a ornare est porttitor aliquet. Vestibulum eu posuere augue. Cras odio mauris, congue ac consectetur vel, aliquet at diam. Nullam et auctor felis. Nulla urna urna, faucibus eu feugiat ac, tincidunt at diam. Integer quis erat blandit, porta sapien eget, ultricies ex. Quisque ac sapien vel mi ornare semper. Praesent quis convallis lectus, ac molestie est. Vestibulum accumsan metus dui, sed laoreet dui viverra eu. Phasellus interdum consectetur mauris sit amet pharetra. Phasellus egestas felis elit, vel mollis justo auctor tempor. Proin finibus facilisis leo, vel feugiat risus. Proin porta, nisi eget accumsan posuere, lacus urna.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_1_header</t>
   </si>
   <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
     <t>Longevity</t>
   </si>
   <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+    <t>text_2_header</t>
   </si>
   <si>
     <t>text_1</t>
+  </si>
+  <si>
+    <t>Tort Reform</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
   </si>
   <si>
     <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven and a half years in office, back when the terms lasted only two years.
@@ -171,34 +244,44 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2b</t>
   </si>
   <si>
     <t>text_1b</t>
   </si>
   <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>higher-education</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.
+Quisque euismod ligula neque, a ornare est porttitor aliquet. Vestibulum eu posuere augue. Cras odio mauris, congue ac consectetur vel, aliquet at diam. Nullam et auctor felis. Nulla urna urna, faucibus eu feugiat ac, tincidunt at diam. Integer quis erat blandit, porta sapien eget, ultricies ex. Quisque ac sapien vel mi ornare semper. Praesent quis convallis lectus, ac molestie est. Vestibulum accumsan metus dui, sed laoreet dui viverra eu. Phasellus interdum consectetur mauris sit amet pharetra. Phasellus egestas felis elit, vel mollis justo auctor tempor. Proin finibus facilisis leo, vel feugiat risus. Proin porta, nisi eget accumsan posuere, lacus urna.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>text_3_header</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>Women's Health</t>
   </si>
   <si>
     <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist(. 
@@ -208,7 +291,16 @@
 “I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)</t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>img_1</t>
   </si>
   <si>
     <t>text_2_header</t>
@@ -217,40 +309,43 @@
     <t>The Texas Miracle</t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>img_1_caption</t>
   </si>
   <si>
     <t>text_2</t>
   </si>
   <si>
-    <t>text_2</t>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
 Critics will find plenty wrong with a state that has the highest percentage of [uninsured](http://kxan.com/2014/09/16/texas-no-1-for-uninsured-rate-again/) residents in the nation, produces [more](http://www.nytimes.com/2014/07/13/us/texas-leader-in-greenhouse-gases-stands-vulnerable-to-their-effects.html?_r=1) greenhouse gas emissions than any other state and has [led the nation](https://www.texastribune.org/2014/09/11/workplace-deaths-decline-texas-still-no-1/) in workplace fatalities for 10 of the last 14 years. </t>
   </si>
   <si>
+    <t>text_3b</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_2b</t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. 
-Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3</t>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.
+Quisque euismod ligula neque, a ornare est porttitor aliquet. Vestibulum eu posuere augue. Cras odio mauris, congue ac consectetur vel, aliquet at diam. Nullam et auctor felis. Nulla urna urna, faucibus eu feugiat ac, tincidunt at diam. Integer quis erat blandit, porta sapien eget, ultricies ex. Quisque ac sapien vel mi ornare semper. Praesent quis convallis lectus, ac molestie est. Vestibulum accumsan metus dui, sed laoreet dui viverra eu. Phasellus interdum consectetur mauris sit amet pharetra. Phasellus egestas felis elit, vel mollis justo auctor tempor. Proin finibus facilisis leo, vel feugiat risus. Proin porta, nisi eget accumsan posuere, lacus urna.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -264,7 +359,16 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>text_4_header</t>
+  </si>
+  <si>
+    <t>HPV Vaccine</t>
+  </si>
+  <si>
     <t>text_3_header</t>
+  </si>
+  <si>
+    <t>text_4</t>
   </si>
   <si>
     <t>The Margins Tax
@@ -274,29 +378,18 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
 At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+    <t>text_4b</t>
   </si>
   <si>
     <t>markdown</t>
@@ -313,18 +406,34 @@
 </t>
   </si>
   <si>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.
+Quisque euismod ligula neque, a ornare est porttitor aliquet. Vestibulum eu posuere augue. Cras odio mauris, congue ac consectetur vel, aliquet at diam. Nullam et auctor felis. Nulla urna urna, faucibus eu feugiat ac, tincidunt at diam. Integer quis erat blandit, porta sapien eget, ultricies ex. Quisque ac sapien vel mi ornare semper. Praesent quis convallis lectus, ac molestie est. Vestibulum accumsan metus dui, sed laoreet dui viverra eu. Phasellus interdum consectetur mauris sit amet pharetra. Phasellus egestas felis elit, vel mollis justo auctor tempor. Proin finibus facilisis leo, vel feugiat risus. Proin porta, nisi eget accumsan posuere, lacus urna.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_4_header</t>
   </si>
   <si>
+    <t>text_5_header</t>
+  </si>
+  <si>
     <t>The Oops Moment</t>
   </si>
   <si>
+    <t>CPRIT</t>
+  </si>
+  <si>
     <t>text_4</t>
   </si>
   <si>
+    <t>text_5</t>
+  </si>
+  <si>
     <t>It’s still hard to watch. </t>
   </si>
   <si>
@@ -334,7 +443,14 @@
     <t>text_4b</t>
   </si>
   <si>
-    <t>topic</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Phasellus ornare aliquet tortor, sed sollicitudin erat. Nunc feugiat ut felis vitae viverra. Aenean eget risus nibh. Pellentesque ut erat suscipit, mollis massa sed, consectetur sem. Aenean aliquam erat eros, in condimentum magna pellentesque in. Curabitur tempus purus turpis, at malesuada orci elementum in. Suspendisse et sem sed velit tristique molestie. Suspendisse molestie tellus vitae justo bibendum fringilla at id est.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_5b</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -346,13 +462,7 @@
 </t>
   </si>
   <si>
-    <t>Health Care</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>headline</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_5_header</t>
@@ -361,22 +471,14 @@
     <t>The Indictment</t>
   </si>
   <si>
-    <t>Gov. Rick Perry's Impact on Texas Health Care</t>
+    <t>Phasellus a ligula eu ligula vestibulum feugiat. Vivamus arcu felis, condimentum ac finibus tincidunt, tincidunt ut purus. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos. Vivamus vitae gravida neque, quis vehicula diam. Vestibulum ultrices dui eget porta laoreet. Pellentesque facilisis eu dui quis interdum. Sed ullamcorper pharetra odio, vel volutpat lectus condimentum ut. Nam faucibus interdum mauris, volutpat iaculis est rhoncus sed. Suspendisse velit sem, dictum vitae justo et, commodo vulputate justo. Duis vestibulum nisl eu ullamcorper ornare. Vestibulum a arcu elit. Pellentesque scelerisque sit amet leo ac elementum. Etiam libero lectus, congue quis dui porta, convallis molestie quam. Sed quis lacus sit amet nunc lacinia rutrum at nec quam. Curabitur cursus non turpis ac vestibulum. Nullam a nunc at elit mattis interdum vitae cursus lorem.
+Quisque euismod ligula neque, a ornare est porttitor aliquet. Vestibulum eu posuere augue. Cras odio mauris, congue ac consectetur vel, aliquet at diam. Nullam et auctor felis. Nulla urna urna, faucibus eu feugiat ac, tincidunt at diam. Integer quis erat blandit, porta sapien eget, ultricies ex. Quisque ac sapien vel mi ornare semper. Praesent quis convallis lectus, ac molestie est. Vestibulum accumsan metus dui, sed laoreet dui viverra eu. Phasellus interdum consectetur mauris sit amet pharetra. Phasellus egestas felis elit, vel mollis justo auctor tempor. Proin finibus facilisis leo, vel feugiat risus. Proin porta, nisi eget accumsan posuere, lacus urna.</t>
   </si>
   <si>
     <t>text_5</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>Political forecasts called for smooth sailing as Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
@@ -384,34 +486,10 @@
 </t>
   </si>
   <si>
-    <t>fa-plus-square</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>slug</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_5b</t>
-  </si>
-  <si>
-    <t>health-care</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>lead_art</t>
   </si>
   <si>
     <t>On Aug. 15, a grand jury indicted Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
@@ -419,13 +497,7 @@
 No matter what happens, Perry’s 11th-hour ride through the criminal justice system guarantees a mention in the history books. He’s the [first governor since James “Pa” Ferguson](http://www.texastribune.org/2014/08/17/you-couldnt-make-stuff-1917-either/) to get indicted, and the uncommonly brash way he has confronted the allegations provided a unique twist to the way potential presidential contenders handle criminal justice challenges. </t>
   </si>
   <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_6_header</t>
@@ -434,13 +506,7 @@
     <t>Swagger</t>
   </si>
   <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
     <t>text_6</t>
-  </si>
-  <si>
-    <t>text_1</t>
   </si>
   <si>
     <t>Granted, swagger is not an event, a policy accomplishment or a political milestone. It’s a style — a cocky way of walking, talking and conducting business. And Perry has made it his calling card.
@@ -533,7 +599,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Higher Education</t>
+    <t>Public Education</t>
   </si>
   <si>
     <t>headline</t>
@@ -542,7 +608,7 @@
     <t>byline</t>
   </si>
   <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -551,13 +617,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-graduation-cap</t>
+    <t>fa-book</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>higher-education</t>
+    <t>public-education</t>
   </si>
   <si>
     <t>share_url</t>
@@ -590,7 +656,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Public Education</t>
+    <t>Environment</t>
   </si>
   <si>
     <t>headline</t>
@@ -599,7 +665,7 @@
     <t>byline</t>
   </si>
   <si>
-    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
+    <t>[Neena Satija](http://www.texastribune.org/about/staff/neena-satija/)</t>
   </si>
   <si>
     <t>markdown</t>
@@ -608,13 +674,13 @@
     <t>icon</t>
   </si>
   <si>
-    <t>fa-book</t>
+    <t>fa-tree</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
-    <t>public-education</t>
+    <t>environment</t>
   </si>
   <si>
     <t>share_url</t>
@@ -671,63 +737,21 @@
     <t>fa-bolt</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>Immigration</t>
-  </si>
-  <si>
-    <t>[Neena Satija](http://www.texastribune.org/about/staff/neena-satija/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-tree</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
-    <t>environment</t>
+    <t>energy</t>
   </si>
   <si>
     <t>share_url</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
     <t>tweet_text</t>
   </si>
   <si>
-    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
-  </si>
-  <si>
     <t>facebook_text</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -737,169 +761,19 @@
     <t>img_1</t>
   </si>
   <si>
-    <t>icon</t>
+    <t>Perry-Legacy-104.JPG</t>
   </si>
   <si>
     <t>img_1_caption</t>
   </si>
   <si>
+    <t>Gov. Rick Perry at the dedication of the Buffalo Gap Wind Farm in Nolan County, Texas in 2006. </t>
+  </si>
+  <si>
     <t>img_1_credit</t>
   </si>
   <si>
     <t>text_1</t>
-  </si>
-  <si>
-    <t>fa-globe</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>Criminal Justice</t>
-  </si>
-  <si>
-    <t>immigration</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>energy</t>
-  </si>
-  <si>
-    <t>[Terri Langford](http://www.texastribune.org/about/staff/terri-langford/)</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-legal</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>criminal-justice</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>Texas Enterprise Fund</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>fa-money</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>texas-enterprise-fund</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
   </si>
   <si>
     <t>One physical mark of Rick Perry’s 14 years as governor can be seen by driving from Austin through Abilene, then an hour northeast into Paint Creek, the speck of a town where Perry grew up. 
@@ -908,40 +782,10 @@
 </t>
   </si>
   <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_2</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>text_1</t>
   </si>
   <si>
     <t>In 2000, wind farms composed just 116 megawatts of capacity on the state’s main electric grid. That number has since soared to more than 11,000 megawatts, while wind fuels about 10 percent of all generation. (On average, one megawatt-hour of wind energy can power 260 typical Texas homes for an hour.)
@@ -958,6 +802,30 @@
     <t>text_3</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Immigration</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-globe</t>
+  </si>
+  <si>
     <t>Perry also backed a $7 billion electrical transmission project to connect windy, largely empty West Texas to growing cities demanding more power. Completed a year ago, the [Competitive Renewable Energy Zone](http://www.texastribune.org/2013/10/14/7-billion-crez-project-nears-finish-aiding-wind-po/), or CREZ, initiative stretches nearly 3,600 miles and can send up to 18,500 megawatts of power — including from non-wind sources — across the state. 
 “That we were able to build thousands of miles of high-capacity transmission from West Texas to the Panhandle without landowners marching on the capital with pitchforks, it’s pretty remarkable,” said Railroad Commissioner Barry Smitherman, whom Perry appointed to the Public Utility Commission in 2004 and reappointed in 2007. “And the governor had our back on that.” 
 Along with decisions that specifically targeted wind, Smitherman said, Perry’s oversight while the state shifted to a competitive electricity market hastened investment in a variety of fuels, leaving Texas with a balanced energy portfolio.
@@ -966,7 +834,40 @@
 </t>
   </si>
   <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
     <t>text_4</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
   </si>
   <si>
     <t>Hartnett White is not the only Texas Republican scrutinizing wind policy as Perry exits office. Comptroller Susan Combs suggested in September that wind energy has “an unfair market advantage over other power sources.” And PUC Chairwoman Donna Nelson, appointed by Perry in 2011, has [called for study](http://www.houstonchronicle.com/business/energy/article/Study-will-assess-shifting-transmission-costs-to-5607745.php#/0) into whether wind energy companies should chip in for power line upgrades — something no other types generator has been asked to do. 
@@ -977,7 +878,255 @@
 </t>
   </si>
   <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
     <t>text_5</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Criminal Justice</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Terri Langford](http://www.texastribune.org/about/staff/terri-langford/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-legal</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>criminal-justice</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Texas Enterprise Fund</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-money</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>texas-enterprise-fund</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/shale-life</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>Just a test</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>Also, just a test</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. 
+Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4</t>
+  </si>
+  <si>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
 </sst>
 </file>
@@ -1047,11 +1196,11 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
     </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+      <alignment/>
+    </xf>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment/>
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
       <alignment/>
@@ -1119,29 +1268,247 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="53.14"/>
-    <col min="2" customWidth="1" max="2" width="26.29"/>
+    <col min="2" customWidth="1" max="2" width="125.0"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>2</v>
-      </c>
-      <c t="s" s="2" r="B2">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="C3">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>29</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>32</v>
+      </c>
+      <c t="s" s="1" r="C12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>94</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>97</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>100</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>104</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>107</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>113</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>117</v>
+      </c>
+      <c t="s" s="1" r="C24">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>121</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>125</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>129</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>131</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>136</v>
+      </c>
+      <c t="s" s="1" r="C27">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1158,128 +1525,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>189</v>
+        <v>283</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>190</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>191</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>192</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>193</v>
+        <v>286</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>195</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>196</v>
-      </c>
-      <c t="s" s="5" r="B4">
-        <v>197</v>
+        <v>289</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>290</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>233</v>
+        <v>291</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>234</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>238</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>242</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>245</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>248</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>252</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>256</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>260</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>263</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>267</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>275</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
-        <v>280</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>288</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
-        <v>290</v>
-      </c>
-      <c t="s" s="1" r="B16">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>292</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -1293,256 +1619,159 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>225</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>232</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>235</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>240</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>244</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>278</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" customWidth="1" max="2" width="59.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>13</v>
+        <v>302</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>14</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>15</v>
+        <v>304</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>16</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>17</v>
+        <v>306</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>19</v>
+        <v>307</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>21</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>23</v>
+        <v>309</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>25</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>27</v>
+        <v>311</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>28</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>29</v>
-      </c>
-      <c t="s" s="3" r="B6">
-        <v>30</v>
+        <v>313</v>
+      </c>
+      <c t="s" s="2" r="B6">
+        <v>314</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>34</v>
+        <v>315</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>35</v>
+        <v>316</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>37</v>
+        <v>317</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>39</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>41</v>
-      </c>
-      <c t="s" s="3" r="B9">
-        <v>43</v>
+        <v>319</v>
+      </c>
+      <c t="s" s="2" r="B9">
+        <v>320</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>47</v>
-      </c>
-      <c t="s" s="3" r="B10">
-        <v>49</v>
+        <v>321</v>
+      </c>
+      <c t="s" s="2" r="B10">
+        <v>322</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>50</v>
-      </c>
-      <c t="s" s="3" r="B11">
-        <v>51</v>
+        <v>323</v>
+      </c>
+      <c t="s" s="2" r="B11">
+        <v>324</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>52</v>
+        <v>325</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>53</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>54</v>
+        <v>327</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>55</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>56</v>
+        <v>329</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>61</v>
+        <v>330</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>62</v>
+        <v>331</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>64</v>
+        <v>332</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>68</v>
+        <v>333</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>69</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>70</v>
+        <v>335</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>76</v>
+        <v>336</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>77</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>78</v>
+        <v>338</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>81</v>
+        <v>339</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>82</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -1556,102 +1785,133 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" customWidth="1" max="1" width="53.14"/>
+    <col min="2" customWidth="1" max="2" width="26.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>30</v>
+      </c>
+      <c t="s" s="3" r="B2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" customWidth="1" max="2" width="125.0"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>94</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>103</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>104</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>106</v>
+        <v>54</v>
+      </c>
+      <c t="s" s="4" r="B4">
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>110</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>111</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>112</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>115</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>117</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>119</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1671,15 +1931,15 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c t="s" s="1" r="B2">
         <v>7</v>
@@ -1687,324 +1947,324 @@
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>10</v>
-      </c>
-      <c t="s" s="3" r="B4">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c t="s" s="2" r="B4">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>58</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>85</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>90</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>95</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>98</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="B22">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>107</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="B23">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c t="s" s="1" r="B24">
-        <v>121</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c t="s" s="1" r="B25">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="B26">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c s="1" r="C26"/>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c t="s" s="1" r="B27">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c s="1" r="C27"/>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c t="s" s="1" r="B28">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c s="1" r="C28"/>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c t="s" s="1" r="B29">
-        <v>134</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>136</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>138</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>140</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>142</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c t="s" s="1" r="B34">
-        <v>144</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c t="s" s="1" r="B35">
-        <v>146</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="1" r="A36">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="B36">
-        <v>148</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c t="s" s="1" r="B37">
-        <v>150</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2024,87 +2284,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>199</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>200</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>205</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>208</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>211</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>213</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>217</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>218</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>219</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>222</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>223</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2121,87 +2381,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>152</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>153</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>155</v>
+        <v>243</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>156</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>157</v>
-      </c>
-      <c t="s" s="4" r="B4">
-        <v>158</v>
+        <v>245</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>246</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>159</v>
+        <v>249</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>160</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>161</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>162</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>163</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>164</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>165</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>166</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>167</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>168</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>169</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2218,87 +2478,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>250</v>
+        <v>192</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>253</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>257</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>261</v>
+        <v>195</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>264</v>
+        <v>196</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>265</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>268</v>
+        <v>198</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>270</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>272</v>
+        <v>200</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>273</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>276</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>279</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>281</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>282</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>283</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>284</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>285</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>286</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>287</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2315,87 +2575,140 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>206</v>
+        <v>213</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>214</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>220</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>224</v>
+        <v>218</v>
+      </c>
+      <c t="s" s="5" r="B4">
+        <v>219</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>247</v>
+        <v>227</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>228</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>251</v>
+        <v>229</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>230</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>255</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>259</v>
+        <v>232</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>233</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>235</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>236</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>238</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>247</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>251</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>260</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2412,87 +2725,87 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>170</v>
+        <v>264</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>171</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>172</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>173</v>
+        <v>267</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>174</v>
+        <v>268</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>175</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>176</v>
+        <v>270</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>177</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>178</v>
+        <v>272</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>179</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>180</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>181</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>182</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>183</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>184</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>185</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>186</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>187</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>188</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change sub-nav prompt, menu prompt
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -26,7 +26,10 @@
     <t>project_title</t>
   </si>
   <si>
-    <t>The Legacy of Gov. Rick Perry</t>
+    <t>The Perry Legacy:</t>
+  </si>
+  <si>
+    <t>(or just "The Perry Legacy" for the first page)</t>
   </si>
   <si>
     <t>project_subtitle</t>
@@ -53,54 +56,108 @@
     <t>headline</t>
   </si>
   <si>
+    <t>6 Things We Won't Forget About Texas' Longest-Serving Governor</t>
+  </si>
+  <si>
     <t>headline</t>
   </si>
   <si>
-    <t>6 Things Texans Won't Forget About Rick Perry</t>
+    <t>byline</t>
   </si>
   <si>
     <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
   </si>
   <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton) and [Jay Root](http://www.texastribune.org/about/staff/jay-root)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>byline</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton) and [Jay Root](http://www.texastribune.org/about/staff/jay-root)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>icon</t>
   </si>
   <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
     <t>fa-star</t>
   </si>
   <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>slug</t>
   </si>
   <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>trib.it/perry-legacy</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1IVfJqr</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>The six things Texans won’t forget about @GovernorPerry: </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>Here are the six things Texans won't forget about Rick Perry, the state's longest-serving governor: </t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
+  </si>
+  <si>
     <t>text_intro</t>
   </si>
   <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that has concluded with his serving as the longest-serving governor in Texas history. 
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that concluded with his service as the longest-serving governor in Texas history. 
 Perry’s 14-year tenure in the state’s highest office coincided with the ever-tightening grip of Republican rule, sweeping conservative reforms and more than a few controversies.
-It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Perry’s reign, and it added more people than any other state between 2000 and 2010 and has continued to grow.</t>
+It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Perry’s reign, and it added more people than any other state between 2000 and 2010 — numbers that continue to grow.</t>
   </si>
   <si>
     <t>markdown</t>
@@ -109,16 +166,16 @@
     <t>text_introb</t>
   </si>
   <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/shale-life</t>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
@@ -137,10 +194,25 @@
     <t>Longevity</t>
   </si>
   <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven and a half years in office, back when the terms lasted only two years.
+    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
 Bill Clements, elected in 1978 as the first Republican governor since Reconstruction, was the first to serve two full four-year terms, but they were not consecutive. In 1998, George W. Bush became the first governor to win two consecutive four-year terms, but he left for Washington halfway through the second one.</t>
   </si>
   <si>
@@ -150,7 +222,18 @@
     <t>text_1b</t>
   </si>
   <si>
-    <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist(. 
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
 At last count, Perry had made more than 8,000 appointments, allowing him to put his conservative stamp on every corner of state government — all from a perch that the state’s founding fathers, suspicious of centralized authority, intentionally weakened.
 Perry championed sweeping curbs on lawsuits, some of the most stringent abortion limits in the nation, the strictest voter ID statute in the country, a constitutional ban on gay marriage and steep cuts to programs once seen as sacrosanct, including public education and women’s health programs.
 People crossed Perry at their peril, whether they were appointees who [dared support](http://www.yourhoustonnews.com/courier/news/tech-regent-perry-ally-pressured-him-to-resign/article_07eed112-5a72-5e72-bda2-5152511a43a5.html?mode=jqm) a political challenger or lawmakers who opposed his legislative program. Jim Henson, a Texas Tribune pollster and director of the Texas Politics Project at the University of Texas at Austin, said Perry expanded the powers of the governor’s office “in a way that is certainly not contemplated in the Texas Constitution nor really in the political culture of the state.”
@@ -166,7 +249,37 @@
     <t>The Texas Miracle</t>
   </si>
   <si>
+    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
     <t>text_2</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4</t>
+  </si>
+  <si>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
@@ -177,24 +290,6 @@
   </si>
   <si>
     <t>text_2b</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>Just a test</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Also, just a test</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -218,12 +313,6 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
     <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
 At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
   </si>
@@ -234,13 +323,7 @@
     <t>text_3b</t>
   </si>
   <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applied to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
+    <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applies to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
 The plan drew plenty of foes. Democrats said it still left schools badly underfunded. And Republican activists complained (and still do) that the revamped business levy, applied to gross receipts minus certain deductions, constituted an unconstitutional income tax.
 But Perry got the plan passed with bipartisan support, the schools stayed open and businesses that used to pay nothing became taxpayers for the first time. 
 “Folks may not have liked the end result, but the margins tax, when you look how it came about, it was really Perry’s finest hour,” said Dale Craymer, president of the business-backed Texas Taxpayers and Research Association. “It was a crisis averted.”
@@ -257,42 +340,16 @@
     <t>The Oops Moment</t>
   </si>
   <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
     <t>text_4</t>
   </si>
   <si>
-    <t>Governor Rick Perry with large scissors at the opening ceremonies for the final southern portion of SH130 toll road from Georgetown, TX north of Austin to Seguin near San Antonio.</t>
-  </si>
-  <si>
     <t>It’s still hard to watch. </t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
     <t>text_4b</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_2</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -304,19 +361,7 @@
 </t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. 
-Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_5_header</t>
@@ -336,28 +381,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4</t>
-  </si>
-  <si>
     <t>text_5b</t>
-  </si>
-  <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>On Aug. 15, a grand jury indicted Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
@@ -398,7 +422,7 @@
     <t>img_1_caption</t>
   </si>
   <si>
-    <t>Texas Governor Rick Perry at his installation as Governor of Texas in the Senate Chamber, December 22, 2000. This occurred when George W. Bush was elected to the U.S. presidency.</t>
+    <t>Texas Gov. Rick Perry at his installation as governor of Texas in the Senate chamber on Dec. 22, 2000. This occurred when George W. Bush was elected to the U.S. presidency.</t>
   </si>
   <si>
     <t>img_1_credit</t>
@@ -417,7 +441,7 @@
     <t>img_2_caption</t>
   </si>
   <si>
-    <t>Texas Governor Rick Perry (l) shares a laugh with Boeing CEO of Defense, Space and Security Dennis Muilenburg (r) at a bill-signing ceremony at the Boeing plant in south San Antonio. Perry signed a state law exempting certain aircraft from tax assessments when temporarily housed in Texas facilities.</t>
+    <t>Texas Gov. Rick Perry (l) shares a laugh with Boeing CEO of Defense, Space and Security Dennis Muilenburg (r) at a bill-signing ceremony at the Boeing plant in San Antonio. Perry signed a state law exempting certain aircraft from tax assessments when temporarily housed in Texas facilities.</t>
   </si>
   <si>
     <t>img_2_credit</t>
@@ -436,7 +460,7 @@
     <t>img_3_caption</t>
   </si>
   <si>
-    <t>Texas Governor Rick Perry appears in Travis County Court on Thursday to answer charges in an indictment regardinghis veto of funding for the Travis County Public Integrity Unit.</t>
+    <t>Texas Gov. Rick Perry appears in Travis County Court to answer charges in an indictment regarding his veto of funding for the Travis County Public Integrity Unit.</t>
   </si>
   <si>
     <t>img_3_credit</t>
@@ -455,7 +479,7 @@
     <t>img_4_caption</t>
   </si>
   <si>
-    <t>State Rep. Rick Perry listens to Rep. Robert Earley (D-Portland), during the 69th Legislative session on the House floor, on May 13, 1985.</t>
+    <t>Then-state Rep. Rick Perry listens to Rep. Robert Earley (D-Portland) during the 69th Legislature on May 13, 1985.</t>
   </si>
   <si>
     <t>img_4_credit</t>
@@ -473,7 +497,7 @@
     <t>headline</t>
   </si>
   <si>
-    <t>Battles With the Federal Government and at Home</t>
+    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
   </si>
   <si>
     <t>byline</t>
@@ -500,12 +524,21 @@
     <t>share_url</t>
   </si>
   <si>
+    <t>trib.it/1DDl1a9</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
+    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -557,7 +590,7 @@
     <t>img_3_caption</t>
   </si>
   <si>
-    <t>Gov. Rick Perry at announcement of new Institute for Applied Cancer Science at The University of Texas MD Anderson Cancer Center in November 2011.</t>
+    <t>Gov. Rick Perry at the November 2011 announcement of new Institute for Applied Cancer Science at the University of Texas MD Anderson Cancer Center.</t>
   </si>
   <si>
     <t>img_3_credit</t>
@@ -569,7 +602,7 @@
     <t>text_intro</t>
   </si>
   <si>
-    <t>During his 14 years in office, Gov. Rick Perry has championed private-market health care solutions and criticized public programs like Medicaid for being inefficient. He has also led the state’s fight against the federal Affordable Care Act, which he has criticized as federal overreach. But as he wages such battles, he has presided over a state with the highest rate of uninsured in the country.
+    <t>During his 14 years in office, Gov. Rick Perry has championed private-market health care solutions and criticized public programs like Medicaid for being inefficient. He has also led the state’s fight against the Affordable Care Act, which he has criticized as federal overreach. But as he wages such battles, he has presided over a state with the highest rate of uninsured in the country.
 “He has clearly had a very Texas model toward health care reform, which is consistent with his approach to many other policies, focusing on a very limited-government approach,” said Mark P. Jones, a political scientist at Rice University.</t>
   </si>
   <si>
@@ -603,7 +636,7 @@
   <si>
     <t>His view contradicts that of President Obama, whose signature health reform law sought to provide near-universal health coverage in the U.S. The Affordable Care Act encouraged states to expand Medicaid coverage to low-income adults and required everyone else to have health insurance or pay a fine. Perry has challenged the law as “socialized” health care and fiscally irresponsible.
 In 2012, the U.S. Supreme Court ruled that states were not required to expand their Medicaid programs. Days later, Perry penned a [scathing letter](http://governor.state.tx.us/files/press-office/O-SebeliusKathleen201207090024.pdf) to then-U.S. Health and Human Services Secretary Kathleen Sebelius, explaining that he would not allow Texas to expand Medicaid because it “would threaten even Texas with financial ruin.”
-Perry’s stance on Medicaid expansion has drawn praise from fiscal conservatives and criticism from the left, which accused Perry of forsaking the more than 1 million Texans in the “coverage gap” — people who would have been newly eligible for Medicaid.
+Perry’s stance on Medicaid expansion has drawn praise from fiscal conservatives and criticism from the left, which accuses him of forsaking the more than 1 million Texans in the “coverage gap” — people who would have been newly eligible for Medicaid.
 </t>
   </si>
   <si>
@@ -617,15 +650,6 @@
   </si>
   <si>
     <t>text_2</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Higher Education</t>
-  </si>
-  <si>
-    <t>headline</t>
   </si>
   <si>
     <t>Perry won praise from doctors when he led the charge on tort reform in 2003. That year, Texas revised its rules through a constitutional amendment voters passed to cap the amount of awards patients could receive for pain and suffering in medical malpractice lawsuits. 
@@ -637,25 +661,10 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
-  </si>
-  <si>
     <t>text_3_header</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>Women's Health</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>text_3</t>
@@ -691,22 +700,13 @@
     <t>text_4</t>
   </si>
   <si>
-    <t>One of Perry’s most controversial decisions as governor was his executive order to require girls entering the sixth grade to be vaccinated against the human papillomavirus, the principal cause of cervical cancer.</t>
+    <t>One of Perry’s most controversial decisions as governor was his executive order requiring girls entering the sixth grade to be vaccinated against the human papillomavirus, the principal cause of cervical cancer.</t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_4b</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>higher-education</t>
-  </si>
-  <si>
-    <t>share_url</t>
   </si>
   <si>
     <t>Perry’s February 2007 order was soon overturned by lawmakers. At the time, he stood behind his decision, saying that a thousand women would likely be diagnosed with the disease in the next year.
@@ -716,13 +716,7 @@
 </t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_5_header</t>
@@ -731,22 +725,7 @@
     <t>CPRIT</t>
   </si>
   <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
     <t>text_5</t>
-  </si>
-  <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>Perry-Legacy-092.JPG</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
   </si>
   <si>
     <t>Perry was a leading proponent of the Cancer Prevention and Research Institute of Texas, a grant-making entity approved by voters in 2007 to spend $3 billion on cancer research, plus an additional $600 million appropriated by the Legislature for 2012-13. 
@@ -756,37 +735,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>Gov. Rick Perry celebrated with state and local leaders at the ceremonial signing of a merger bill between UT-Pan American and UT-Brownsville in 2013. Left to right, Dr. Juliet Garcia of UT-Brownsville, Dr. Robert Nelsen of UT-Pan American, Gov. Rick Perry,  UT Regent chairman Gene Powell, Dr. Francisco Cigarroa, UT System Chancellor.</t>
-  </si>
-  <si>
     <t>text_5b</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>img_2</t>
-  </si>
-  <si>
-    <t>Perry-Legacy-117.JPG</t>
-  </si>
-  <si>
-    <t>img_2_caption</t>
-  </si>
-  <si>
-    <t>Former University of Texas President Bill Powers during a UT Board of Regents meeting on July 20, 2014.</t>
-  </si>
-  <si>
-    <t>img_2_credit</t>
-  </si>
-  <si>
-    <t>Marjorie Kamys Cotera</t>
-  </si>
-  <si>
-    <t>text_intro</t>
   </si>
   <si>
     <t>One of Peloton’s initial investors was Dallas philanthropist Peter O’Donnell, who has donated $241,000 to Perry’s campaigns since 2000, campaign finance records show. At the time, The Dallas Morning News reported that O’Donnell had also given $1.6 million to the CPRIT Foundation, a nonprofit. State law prohibits the CPRIT Foundation from accepting donations from CPRIT grant recipients. 
@@ -799,6 +748,102 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Heavy Hand in Academic Affairs </t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>higher-education</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/12YF3Lq</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>From in-state tuition for undocumented students to the “Seven Solutions” — @GovernorPerry’s heavy hand in higher ed </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>From in-state tuition for undocumented students to the “Seven Breakthrough Solutions,” a look at Gov. Rick Perry’s heavy hand in higher ed</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>lead_art</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-092.JPG</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry celebrated with state and local leaders at the ceremonial signing of a merger bill between UT-Pan American and UT-Brownsville in 2013. </t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>img_2</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-117.JPG</t>
+  </si>
+  <si>
+    <t>img_2_caption</t>
+  </si>
+  <si>
+    <t>Former University of Texas at Austin President Bill Powers during a UT Board of Regents meeting on July 20, 2014.</t>
+  </si>
+  <si>
+    <t>img_2_credit</t>
+  </si>
+  <si>
+    <t>Marjorie Kamys Cotera</t>
+  </si>
+  <si>
+    <t>text_intro</t>
+  </si>
+  <si>
     <t>As Gov. Rick Perry himself has said — and as his critics are fond of pointing out — he [did not demonstrate significant interest](http://www.texastribune.org/2011/08/02/perry-aggie-years/) in academia while an undergraduate student at Texas A&amp;M University.
 “Four semesters of organic chemistry made a pilot out of me,” he joked in a 2011 speech at Liberty University.
 But during Perry’s time as a statewide elected official, higher education policy has often been at the forefront of his mind. As lieutenant governor, he formed a [Special Commission on 21st Century Colleges and Universities](http://www.senate.state.tx.us/75r/Senate/Commit/archive/21min/pr99/p102799a.htm) in 1999.
@@ -811,8 +856,8 @@
     <t>text_introb</t>
   </si>
   <si>
-    <t>And over the course of his decade and a half as governor, he has certainly had an influence on the state’s colleges and universities, but he has at times pushed and pulled in contradictory directions.
-In recent years, Perry has emerged as a strong critic of rising tuition. In 2011, he [called](http://www.texastribune.org/2011/02/08/perry-to-push-texas-colleges-to-offer-10000-degree/) on the state’s public universities to create undergraduate degrees that cost $10,000 including books. During the 2013 legislative session, he [encouraged](http://www.texastribune.org/2012/10/01/perry-call-financial-disclosures-universities/) the passage of a bill that required public universities to offer payment plans that fixed tuition at a set rate for four years. This year, he [successfully pushed](http://www.texastribune.org/2014/05/20/-state-students-ut-system-keeps-tuition-steady/) for the University of Texas System to keep tuition flat at their academic institutions.
+    <t>And over the course of his decade-and-a-half as governor, he has certainly had influence on the state’s colleges and universities, but he has at times pushed and pulled in contradictory directions.
+In recent years, Perry has emerged as a strong critic of rising tuition. In 2011, he [called](http://www.texastribune.org/2011/02/08/perry-to-push-texas-colleges-to-offer-10000-degree/) on the state’s public universities to create undergraduate degrees that cost $10,000 including books. During the 2013 legislative session, he [encouraged](http://www.texastribune.org/2012/10/01/perry-call-financial-disclosures-universities/) the passage of a bill that required public universities to offer payment plans that fixed tuition at a set rate for four years. This year, he [successfully pushed](http://www.texastribune.org/2014/05/20/-state-students-ut-system-keeps-tuition-steady/) for the University of Texas System to keep tuition flat at its academic institutions.
 “To put a college degree within reach for more students and combat the epidemic of student indebtedness, we should place a far greater emphasis on controlling the spiraling costs of a college education," the governor wrote to the chairman of the UT board.</t>
   </si>
   <si>
@@ -838,8 +883,8 @@
     <t>text_1b</t>
   </si>
   <si>
-    <t>“We must do everything we can to continue making higher education an achievable dream for all Texans,” the governor said in his 2013 State of the State address. And his website [accurately notes](http://www.rickperry.org/issues/education) that more than 200,000 more students are enrolled in the state’s colleges and universities now than then he first took office.
-No doubt many of them are taking advantage of the [TEXAS Grants](http://www.collegeforalltexans.com/index.cfm?ObjectID=E81912E0-DF96-53C5-8EE1C469C7298F15) grant program, the state’s primary source of financial aid for needy students, which was created when Perry was lieutenant governor. As governor, he touted the program, but its [first cuts](http://www.texastribune.org/2011/08/04/day-4-less-financial-aid-texas-students/) also happened on his watch, as did the implementation of rule changes that made the grants harder to access for some students.</t>
+    <t>“We must do everything we can to continue making higher education an achievable dream for all Texans,” the governor said in his 2013 State of the State address. And his website [accurately notes](http://www.rickperry.org/issues/education) that more than 200,000 more students are enrolled in the state’s colleges and universities now than when he first took office.
+No doubt many of them are taking advantage of the [TEXAS Grants](http://www.collegeforalltexans.com/index.cfm?ObjectID=E81912E0-DF96-53C5-8EE1C469C7298F15) program, the state’s primary source of financial aid for needy students, which was created when Perry was lieutenant governor. As governor, he touted the program, but its [first cuts](http://www.texastribune.org/2011/08/04/day-4-less-financial-aid-texas-students/) also happened on his watch, as did the implementation of rule changes that made the grants harder to access for some students.</t>
   </si>
   <si>
     <t>markdown</t>
@@ -873,7 +918,7 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>In 2011, a group of the University of Texas at Austin’s well-heeled and influential alumni pushed back when they feared the reforms were about to be pushed at their university. The controversy has yet to die down, even though the proposals were never put into practice.
+    <t>In 2011, a group of the University of Texas at Austin’s well-heeled and influential alumni pushed back when they feared the reforms were about to be pushed on their university. The controversy has yet to die down, even though the proposals were never put into practice.
 </t>
   </si>
   <si>
@@ -911,15 +956,6 @@
     <t>text_4b</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Public Education</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
     <t>When the issue came up in a nationally televised debate during the Republican presidential primary in 2011, Perry [said](http://www.texastribune.org/2011/09/22/liveblog-fox-newsgoogle-republican-debate/) of those who questioned the policy, “I don’t think you have a heart.” His [poll numbers](http://www.texastribune.org/library/data/rise-and-fall-of-rick-perry-presidential-campaign/) nose-dived and never recovered. Though he expressed regret for the language he used in its defense, he has not backed down on his support for what’s called the Texas DREAM Act.
 Whether the policy remains a memorable part of his legacy will largely depend on whether it survives the coming legislative session. With Perry gone, its continuation is in doubt.
 *Disclosure: Texas A&amp;M University and the University of Texas at Austin are corporate sponsors of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).*</t>
@@ -928,6 +964,18 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Public Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Guarding State Control of Public Schools — With Money on the Line</t>
+  </si>
+  <si>
     <t>byline</t>
   </si>
   <si>
@@ -952,10 +1000,19 @@
     <t>share_url</t>
   </si>
   <si>
+    <t>trib.it/1qTCoh3</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
+    <t>#Perry’s approach to public ed has been to guard state control over classrooms — even when there’s money on the line</t>
+  </si>
+  <si>
     <t>facebook_text</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's approach to public education has been to guard state control over classrooms — even when there’s federal money on the line trib.it/1qTCoh3</t>
   </si>
   <si>
     <t>facebook_art</t>
@@ -997,9 +1054,9 @@
   <si>
     <t>Less than a decade later, as Perry geared up for his own presidential bid, he would propose something radically different: dismantling the U.S. Department of Education and vastly diminishing the role of the federal government in public schools. He would call No Child Left Behind a [“monstrous intrusion into our affairs.”](http://www.nationalreview.com/articles/265309/rick-perry-s-tenth-commandment-kevin-d-williamson/page/0/3)
 Guarding Texas control of public school classrooms has been the most prominent feature of Perry’s approach to education. But as he leaves office, his impact will also be felt in state-level matters, where his involvement has tended to be less public.
-The high-profile battles with Washington began in the summer of 2009, when Texas declined to sign on a nationwide effort to develop common academic standards in reading and math. Known as Common Core, it had the support of both Republican and Democratic policymakers. Only Alaska joined Texas in refusing to participate.
+The high-profile battles with Washington began in the summer of 2009, when Texas declined to sign on to a nationwide effort to develop common academic standards in reading and math. Known as Common Core, it had the support of both Republican and Democratic policymakers. Only Alaska joined Texas in refusing to participate.
 Though it drew little attention at the time, the move was the first sign of the political firestorm that would ignite over the initiative. Four years later, concern over a potential federal takeover of education has driven at least four states to drop them from their public schools, with numerous others facing pressure to do the same. 
-A few months later, a decision not to apply not to apply for the Obama administration’s Race to the Top competition — which meant losing out on $700 million in federal funding — once again made Texas an outlier. The program, which initially set aside $4.35 billion in grants for states that agreed to put certain reforms in place, had until then had largely enjoyed bipartisan praise.
+A few months later, a decision not to apply not to apply for the Obama administration’s Race to the Top competition — which meant losing out on $700 million in federal funding — once again made Texas an outlier. The program, which initially set aside $4.35 billion in grants for states that agreed to put certain reforms in place, had until then largely enjoyed bipartisan praise.
 </t>
   </si>
   <si>
@@ -1024,9 +1081,9 @@
     <t>text_4</t>
   </si>
   <si>
-    <t>Legislators ultimately enacted a historic reduction in funding for public schools: $4 billion in state dollars and an additional almost $1.4 billion in discretionary grants that supported programs including remedial intervention and after-school care.
+    <t>Legislators ultimately enacted a historic reduction in funding for public schools: $4 billion in state dollars and almost $1.4 billion in discretionary grants that supported programs including remedial intervention and after-school care.
 An exchange between two Republicans on the Texas House floor about an amendment that became one of the last efforts to use the Rainy Day Fund for public schools revealed the depth of the governor’s influence:
-“Is it possible,” Rep. Van Taylor of Plano said, “if the amendment stayed in that the governor might veto the bill?”
+“Is it possible,” Rep. Van Taylor of Plano asked, “if the amendment stayed in that the governor might veto the bill?”
 Rep. Phil King of Weatherford replied, “Well, my impression of Gov. Perry is that he usually does what he says that he’s going to do.”
 Those budget cuts gave rise to a massive school finance lawsuit, in which more than two-thirds of Texas school districts sued the state. In August, nearly three years after the trial began, a state district judge in Travis County ruled in their favor, finding the state’s school finance system unconstitutional. 
 The Texas Supreme Court is expected to rule on an appeal of the decision late next year. 
@@ -1070,6 +1127,9 @@
   </si>
   <si>
     <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1wzOUmw</t>
   </si>
   <si>
     <t>tweet_text</t>
@@ -1225,6 +1285,9 @@
     <t>share_url</t>
   </si>
   <si>
+    <t>trib.it/1BMMz8l</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
@@ -1250,6 +1313,9 @@
   </si>
   <si>
     <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
   </si>
   <si>
     <t>text_1</t>
@@ -1293,6 +1359,9 @@
   </si>
   <si>
     <t>text_4</t>
+  </si>
+  <si>
+    <t>topic</t>
   </si>
   <si>
     <t>Hartnett White is not the only Texas Republican scrutinizing wind policy as Perry exits office. Comptroller Susan Combs suggested in September that wind energy has “an unfair market advantage over other power sources.” And PUC Chairwoman Donna Nelson, appointed by Perry in 2011, has [called for study](http://www.houstonchronicle.com/business/energy/article/Study-will-assess-shifting-transmission-costs-to-5607745.php#/0) into whether wind energy companies should chip in for power line upgrades — something no other types generator has been asked to do. 
@@ -1304,18 +1373,15 @@
 </t>
   </si>
   <si>
+    <t>Immigration</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_5</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Immigration</t>
-  </si>
-  <si>
     <t>headline</t>
   </si>
   <si>
@@ -1346,6 +1412,9 @@
     <t>share_url</t>
   </si>
   <si>
+    <t>trib.it/1wzP3pX</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
@@ -1389,6 +1458,9 @@
   </si>
   <si>
     <t>img_2_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
   </si>
   <si>
     <t>text_1</t>
@@ -1486,6 +1558,9 @@
   </si>
   <si>
     <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1zpt9Ws</t>
   </si>
   <si>
     <t>tweet_text</t>
@@ -1607,7 +1682,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Texas Enterprise Fund</t>
+    <t>Enterprise Fund</t>
   </si>
   <si>
     <t>headline</t>
@@ -1638,6 +1713,9 @@
   </si>
   <si>
     <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1wC9dyA</t>
   </si>
   <si>
     <t>tweet_text</t>
@@ -1723,7 +1801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -1732,6 +1810,9 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1781,7 +1862,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -1795,10 +1876,13 @@
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4" applyFill="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
       <alignment/>
     </xf>
   </cellXfs>
@@ -1872,18 +1956,21 @@
       <c t="s" s="1" r="B1">
         <v>1</v>
       </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c t="s" s="2" r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1900,146 +1987,183 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>463</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>465</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>468</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>470</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>472</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>473</v>
+        <v>455</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>456</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>474</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>475</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>476</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>477</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>479</v>
+        <v>462</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>481</v>
+        <v>464</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>485</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>486</v>
+        <v>468</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>488</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>489</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>491</v>
-      </c>
-      <c t="s" s="1" r="C16">
-        <v>492</v>
+        <v>472</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>494</v>
+        <v>474</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>495</v>
+        <v>475</v>
       </c>
     </row>
     <row r="18">
-      <c s="1" r="A18"/>
-      <c s="1" r="C18"/>
+      <c t="s" s="1" r="A18">
+        <v>476</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>477</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>479</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>480</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>482</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>483</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>485</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>486</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>487</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2052,181 +2176,538 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>419</v>
+        <v>488</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>420</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>421</v>
+        <v>490</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>422</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>423</v>
+        <v>492</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>424</v>
+        <v>493</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>425</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>426</v>
+        <v>495</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>427</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>428</v>
+        <v>497</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>429</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>430</v>
+        <v>499</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>500</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>431</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>432</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>433</v>
+        <v>503</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>434</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>435</v>
+        <v>505</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>436</v>
+        <v>506</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>437</v>
+        <v>507</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>438</v>
+        <v>508</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>439</v>
+        <v>509</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>440</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>441</v>
+        <v>511</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>442</v>
+        <v>512</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>513</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>443</v>
+        <v>514</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>444</v>
+        <v>515</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>516</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>445</v>
+        <v>517</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>446</v>
+        <v>518</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>519</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>447</v>
+        <v>520</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>448</v>
+        <v>521</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>449</v>
+        <v>522</v>
       </c>
     </row>
     <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>450</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>451</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>453</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>454</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>456</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>457</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>459</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>460</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>461</v>
-      </c>
+      <c s="1" r="A18"/>
+      <c s="1" r="C18"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>10</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>22</v>
+      </c>
+      <c s="1" r="B5"/>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>23</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>31</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>35</v>
+      </c>
+      <c t="s" s="3" r="B9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>41</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>53</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>61</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>96</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>98</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>103</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>104</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>106</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>107</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>109</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
+        <v>111</v>
+      </c>
+      <c t="s" s="1" r="B28">
+        <v>112</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" s="1" r="A29">
+        <v>114</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>115</v>
+      </c>
+      <c s="1" r="C29"/>
+    </row>
+    <row r="30">
+      <c t="s" s="1" r="A30">
+        <v>116</v>
+      </c>
+      <c t="s" s="1" r="B30">
+        <v>117</v>
+      </c>
+      <c s="1" r="C30"/>
+    </row>
+    <row r="31">
+      <c t="s" s="1" r="A31">
+        <v>118</v>
+      </c>
+      <c t="s" s="1" r="B31">
+        <v>119</v>
+      </c>
+      <c s="1" r="C31"/>
+    </row>
+    <row r="32">
+      <c t="s" s="1" r="A32">
+        <v>120</v>
+      </c>
+      <c t="s" s="1" r="B32">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33">
+      <c t="s" s="1" r="A33">
+        <v>122</v>
+      </c>
+      <c t="s" s="1" r="B33">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
+        <v>124</v>
+      </c>
+      <c t="s" s="1" r="B34">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>126</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>128</v>
+      </c>
+      <c t="s" s="1" r="B36">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
+        <v>130</v>
+      </c>
+      <c t="s" s="1" r="B37">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>132</v>
+      </c>
+      <c t="s" s="1" r="B38">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>134</v>
+      </c>
+      <c t="s" s="1" r="B39">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>136</v>
+      </c>
+      <c t="s" s="1" r="B40">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2238,153 +2719,153 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c t="s" s="1" r="B3">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="C3">
         <v>21</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B5">
         <v>28</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
+        <v>29</v>
+      </c>
+      <c t="s" s="3" r="B6">
         <v>30</v>
-      </c>
-      <c t="s" s="3" r="B6">
-        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c t="s" s="3" r="B9">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c t="s" s="3" r="B10">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c t="s" s="3" r="B11">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>97</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2398,609 +2879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" customWidth="1" max="2" width="65.57"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>9</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>15</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>17</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>19</v>
-      </c>
-      <c s="1" r="B5"/>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>20</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>25</v>
-      </c>
-      <c t="s" s="1" r="C6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="B7">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="C7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>34</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="B9">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="C9">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="B10">
-        <v>40</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>44</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="C12">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>47</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>56</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
-        <v>58</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>61</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="B16">
-        <v>66</v>
-      </c>
-      <c t="s" s="1" r="C16">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>68</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>73</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>89</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>98</v>
-      </c>
-      <c t="s" s="1" r="C22">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>100</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>103</v>
-      </c>
-      <c t="s" s="1" r="C24">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>105</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>106</v>
-      </c>
-      <c s="1" r="C25"/>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>107</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>108</v>
-      </c>
-      <c s="1" r="C26"/>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>109</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>110</v>
-      </c>
-      <c s="1" r="C27"/>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>111</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>113</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
-        <v>115</v>
-      </c>
-      <c t="s" s="1" r="B30">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>117</v>
-      </c>
-      <c t="s" s="1" r="B31">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>119</v>
-      </c>
-      <c t="s" s="1" r="B32">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
-        <v>121</v>
-      </c>
-      <c t="s" s="1" r="B33">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
-        <v>123</v>
-      </c>
-      <c t="s" s="1" r="B34">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>125</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>127</v>
-      </c>
-      <c t="s" s="1" r="B36">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
-        <v>179</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>184</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>185</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>189</v>
-      </c>
-      <c t="s" s="5" r="B4">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>203</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>215</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" s="1" r="A12">
-        <v>217</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>222</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
-        <v>224</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
-        <v>226</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
-        <v>228</v>
-      </c>
-      <c t="s" s="1" r="B16">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>230</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>233</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>235</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>236</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>238</v>
-      </c>
-      <c t="s" s="4" r="B19">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>240</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>241</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>243</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>244</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>246</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>248</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>249</v>
-      </c>
-      <c t="s" s="1" r="C23">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>251</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>253</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>254</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>256</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>257</v>
-      </c>
-      <c t="s" s="1" r="C26">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>259</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>261</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>262</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>264</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>268</v>
-      </c>
-      <c t="s" s="1" r="C29">
-        <v>269</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3012,277 +2891,286 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c t="s" s="4" r="B2">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>135</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>140</v>
+        <v>149</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>141</v>
+        <v>151</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>142</v>
+        <v>153</v>
+      </c>
+      <c t="s" s="5" r="B8">
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>143</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>144</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c s="1" r="C11"/>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c s="1" r="C12"/>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c s="1" r="C13"/>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c s="1" r="C17"/>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c s="1" r="C18"/>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c s="1" r="C19"/>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>165</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c s="1" r="B21"/>
       <c t="s" s="1" r="C21">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c t="s" s="1" r="B22">
-        <v>169</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c t="s" s="4" r="B23">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>172</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c t="s" s="1" r="B24">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c t="s" s="1" r="B25">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c t="s" s="1" r="B26">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c t="s" s="1" r="B27">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c t="s" s="1" r="B28">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c t="s" s="1" r="B29">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c t="s" s="1" r="C32">
         <v>208</v>
@@ -3290,36 +3178,310 @@
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
+        <v>209</v>
+      </c>
+      <c t="s" s="1" r="B33">
         <v>210</v>
-      </c>
-      <c t="s" s="1" r="B33">
-        <v>211</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
+        <v>211</v>
+      </c>
+      <c t="s" s="1" r="B34">
+        <v>212</v>
+      </c>
+      <c t="s" s="1" r="C34">
         <v>213</v>
-      </c>
-      <c t="s" s="1" r="B34">
-        <v>218</v>
-      </c>
-      <c t="s" s="1" r="C34">
-        <v>219</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
+        <v>214</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>215</v>
+      </c>
+      <c t="s" s="1" r="C35">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>217</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>219</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
         <v>221</v>
       </c>
-      <c t="s" s="1" r="B35">
+      <c t="s" s="1" r="B3">
+        <v>222</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>224</v>
+      </c>
+      <c t="s" s="6" r="B4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>226</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>228</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>230</v>
+      </c>
+      <c t="s" s="1" r="B7">
         <v>231</v>
       </c>
-      <c t="s" s="1" r="C35">
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
         <v>232</v>
       </c>
+      <c t="s" s="5" r="B8">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>236</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>238</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>240</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>242</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>244</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16">
+      <c t="s" s="1" r="A16">
+        <v>246</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>248</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>249</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>251</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>252</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>254</v>
+      </c>
+      <c t="s" s="4" r="B19">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>256</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>257</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>259</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>260</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>262</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>264</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>265</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>267</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>269</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>270</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>272</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>273</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>275</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
+        <v>277</v>
+      </c>
+      <c t="s" s="1" r="B28">
+        <v>278</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" s="1" r="A29">
+        <v>280</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>281</v>
+      </c>
+      <c t="s" s="1" r="C29">
+        <v>282</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3332,139 +3494,154 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>266</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>267</v>
+        <v>285</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>286</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>272</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>274</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>275</v>
+        <v>292</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>276</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>277</v>
+        <v>294</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>295</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>278</v>
+        <v>296</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>297</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>279</v>
+        <v>298</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>299</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>280</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>281</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>283</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>285</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>287</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>290</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>292</v>
+        <v>312</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>293</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>294</v>
+        <v>314</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>296</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>299</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3480,177 +3657,183 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>301</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>303</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>305</v>
+        <v>325</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>308</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>310</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>311</v>
+        <v>331</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>332</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>312</v>
+        <v>333</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>313</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>314</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>315</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>316</v>
+        <v>337</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>317</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>319</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>321</v>
+        <v>342</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>323</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>326</v>
+        <v>347</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>327</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>328</v>
+        <v>349</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>330</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>331</v>
+        <v>352</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>333</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>334</v>
+        <v>355</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>336</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>337</v>
+        <v>358</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>338</v>
+        <v>359</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>339</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>340</v>
+        <v>361</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>342</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3663,178 +3846,153 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>378</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>383</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>384</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>385</v>
+        <v>371</v>
+      </c>
+      <c t="s" s="7" r="B4">
+        <v>372</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>387</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>388</v>
+        <v>375</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>376</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>389</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>390</v>
+        <v>378</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>391</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>392</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>394</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>396</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>398</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>400</v>
-      </c>
-      <c s="1" r="C14"/>
+        <v>388</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>389</v>
+      </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>402</v>
-      </c>
-      <c s="1" r="C15"/>
+        <v>391</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>392</v>
+      </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>403</v>
-      </c>
-      <c s="1" r="B16"/>
-      <c s="1" r="C16"/>
+        <v>393</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>394</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>395</v>
+      </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>407</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>408</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>410</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>411</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>413</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>414</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>416</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>417</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>418</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3847,143 +4005,185 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>343</v>
+        <v>397</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>344</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>345</v>
+        <v>402</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>346</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>347</v>
+        <v>404</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>348</v>
+        <v>405</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>349</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>350</v>
-      </c>
-      <c t="s" s="6" r="B4">
-        <v>351</v>
+        <v>407</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>408</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>352</v>
+        <v>409</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>353</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>354</v>
+        <v>411</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>412</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>355</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>356</v>
+        <v>414</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>357</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>358</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>359</v>
+        <v>417</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>360</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>361</v>
+        <v>419</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>362</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>363</v>
+        <v>421</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>422</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>364</v>
+        <v>423</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>365</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>366</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>367</v>
+        <v>425</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>368</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>369</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>370</v>
+        <v>427</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>371</v>
-      </c>
-      <c t="s" s="1" r="C16">
-        <v>372</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>373</v>
+        <v>429</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>374</v>
+        <v>430</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>375</v>
+        <v>431</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>376</v>
+        <v>432</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>433</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>435</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>436</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>438</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>439</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>441</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>442</v>
+      </c>
+      <c t="s" s="1" r="C21">
+        <v>443</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
move nav-menu into container
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -44,13 +44,7 @@
     <t>topic</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Overview</t>
-  </si>
-  <si>
-    <t>Transportation</t>
+    <t>What We'll Remember</t>
   </si>
   <si>
     <t>headline</t>
@@ -59,63 +53,30 @@
     <t>6 Things We Won't Forget About Texas' Longest-Serving Governor</t>
   </si>
   <si>
-    <t>headline</t>
-  </si>
-  <si>
     <t>byline</t>
   </si>
   <si>
-    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
-  </si>
-  <si>
     <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton) and [Jay Root](http://www.texastribune.org/about/staff/jay-root)</t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
     <t>icon</t>
   </si>
   <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
     <t>fa-star</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
     <t>share_url</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
     <t>trib.it/perry-legacy</t>
   </si>
   <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1IVfJqr</t>
-  </si>
-  <si>
     <t>tweet_text</t>
   </si>
   <si>
@@ -131,28 +92,10 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
     <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
-    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
-  </si>
-  <si>
     <t>text_intro</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that concluded with his service as the longest-serving governor in Texas history. 
@@ -163,19 +106,28 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>text_introb</t>
   </si>
   <si>
-    <t>lead_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
@@ -185,31 +137,34 @@
 </t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>fa-car</t>
   </si>
   <si>
     <t>text_1_header</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
     <t>Longevity</t>
   </si>
   <si>
-    <t>img_1_caption</t>
+    <t>transportation</t>
   </si>
   <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1IVfJqr</t>
   </si>
   <si>
     <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
@@ -222,15 +177,22 @@
     <t>text_1b</t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_2</t>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
@@ -243,43 +205,25 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>lead_art</t>
+  </si>
+  <si>
     <t>text_2_header</t>
   </si>
   <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
     <t>The Texas Miracle</t>
   </si>
   <si>
-    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
     <t>text_2</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3</t>
-  </si>
-  <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4</t>
-  </si>
-  <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
@@ -290,6 +234,21 @@
   </si>
   <si>
     <t>text_2b</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>text_1</t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -303,7 +262,18 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>text_3_header</t>
+  </si>
+  <si>
+    <t>text_2</t>
   </si>
   <si>
     <t>The Margins Tax
@@ -313,14 +283,44 @@
     <t>text_3</t>
   </si>
   <si>
+    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
 At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
   </si>
   <si>
+    <t>text_4</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_3b</t>
+  </si>
+  <si>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applies to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>text_4b</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -370,7 +376,13 @@
     <t>The Indictment</t>
   </si>
   <si>
+    <t>headline</t>
+  </si>
+  <si>
     <t>text_5</t>
+  </si>
+  <si>
+    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
   </si>
   <si>
     <t>Political forecasts called for smooth sailing as Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
@@ -432,13 +444,40 @@
 </t>
   </si>
   <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
     <t>img_2_url</t>
   </si>
   <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
     <t>Perry-Legacy-110.JPG</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
     <t>img_2_caption</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1DDl1a9</t>
   </si>
   <si>
     <t>Texas Gov. Rick Perry (l) shares a laugh with Boeing CEO of Defense, Space and Security Dennis Muilenburg (r) at a bill-signing ceremony at the Boeing plant in San Antonio. Perry signed a state law exempting certain aircraft from tax assessments when temporarily housed in Texas facilities.</t>
@@ -460,7 +499,13 @@
     <t>img_3_caption</t>
   </si>
   <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
     <t>Texas Gov. Rick Perry appears in Travis County Court to answer charges in an indictment regarding his veto of funding for the Travis County Public Integrity Unit.</t>
+  </si>
+  <si>
+    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
   </si>
   <si>
     <t>img_3_credit</t>
@@ -470,12 +515,18 @@
 </t>
   </si>
   <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
     <t>img_4_url</t>
   </si>
   <si>
     <t>Perry-Legacy-093.JPG</t>
   </si>
   <si>
+    <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
+  </si>
+  <si>
     <t>img_4_caption</t>
   </si>
   <si>
@@ -486,57 +537,6 @@
   </si>
   <si>
     <t>Texas State Library &amp; Archives Commision</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Health Care</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-plus-square</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>health-care</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1DDl1a9</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
   </si>
   <si>
     <t>facebook_art</t>
@@ -709,6 +709,12 @@
     <t>text_4b</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
     <t>Perry’s February 2007 order was soon overturned by lawmakers. At the time, he stood behind his decision, saying that a thousand women would likely be diagnosed with the disease in the next year.
 "I challenge legislators to look these women in the eyes and tell them, 'We could have prevented this disease for your daughters and granddaughters, but we just didn't have the gumption to address all the misguided and misleading political rhetoric,’” Perry [said](http://www.chron.com/news/article/Perry-yields-on-HPV-vaccines-chides-lawmakers-1830709.php).
 Perry also brushed off criticism that he had [close ties to Merck](http://www.kbtx.com/home/headlines/5546651.html), the only manufacturer of the vaccine at the time, whose lobbyist was Mike Toomey, the governor’s former chief of staff. 
@@ -719,13 +725,34 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Heavy Hand in Academic Affairs </t>
+  </si>
+  <si>
     <t>text_5_header</t>
   </si>
   <si>
     <t>CPRIT</t>
   </si>
   <si>
+    <t>byline</t>
+  </si>
+  <si>
     <t>text_5</t>
+  </si>
+  <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>Perry was a leading proponent of the Cancer Prevention and Research Institute of Texas, a grant-making entity approved by voters in 2007 to spend $3 billion on cancer research, plus an additional $600 million appropriated by the Legislature for 2012-13. 
@@ -746,33 +773,6 @@
   </si>
   <si>
     <t>markdown</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Higher Education</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Heavy Hand in Academic Affairs </t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>slug</t>
@@ -1135,9 +1135,15 @@
     <t>tweet_text</t>
   </si>
   <si>
+    <t>Texans have breathed clearer air since @GovernorPerry took office. But who deserves the credit? </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>Texans have breathed clearer air since Gov. Rick Perry took office. But who deserves the credit? </t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -1153,7 +1159,7 @@
     <t>img_1_caption</t>
   </si>
   <si>
-    <t>NRG Coal powered electrical generation plant in Fort Bend County near Richmond, Texas in 2013.</t>
+    <t>An NRG coal-powered electrical generation plant in Fort Bend County near Richmond, Texas in 2013.</t>
   </si>
   <si>
     <t>img_1_credit</t>
@@ -1171,7 +1177,7 @@
     <t>img_2_caption</t>
   </si>
   <si>
-    <t>Afternoon rush hour traffic on IH-35 near downtown Austin on Nov. 24, 2014.
+    <t>Afternoon rush hour traffic on I-35 near downtown Austin on Nov. 24, 2014.
 </t>
   </si>
   <si>
@@ -1214,7 +1220,7 @@
 “He has the worst environmental record that I’ve seen in the 30 years that I’ve been working on this issue,” Smith said, arguing that federal environmental rules  — which Perry opposed — are largely responsible for cleaning up Texas’ air. 
 Federal mileage and emission standards have improved air quality across the country, not just in Texas, said Elena Craft, a health scientist and air pollution expert with the Environmental Defense Fund. “I can’t think of something that Perry himself has promoted,” she said. (Texas officials point out that average ozone [reductions](https://www.tceq.texas.gov/airquality/airsuccess/air-success-criteria) in Texas have been better than other states, or the country as a whole.)
 Smith and Craft also pointed to Perry’s opposition to nearly every federal attempt to reduce air pollution. During Perry’s tenure, Texas has sued the Environmental Protection Agency more than a dozen times, for the most part unsuccessfully. 
-The U.S. Supreme Court [struck down](http://www.texastribune.org/2014/04/29/texas-loses-fight-against-epa-air-pollution-rule/) Texas’ challenges to a federal rule governing interstate pollution and largely [dismissed](http://www.texastribune.org/2014/06/23/latest-epa-supreme-court-ruling-largely-loss-texas/) objections to climate change regulations. A federal appeals court also [ruled against](http://www.cadc.uscourts.gov/internet/opinions.nsf/284AC47088C07D0985257CBB004F0795/%24file/12-1100-1488346.pdf) Texas’ lawsuit over a federal rule on mercury and air toxic emissions limits from coal plants, and the Supreme Court has [said](http://www.nytimes.com/2014/11/26/us/politics/supreme-court-to-hear-case-on-costs-of-clean-air-act.html) it will take up the case.
+The U.S. Supreme Court [struck down](http://www.texastribune.org/2014/04/29/texas-loses-fight-against-epa-air-pollution-rule/) Texas’ challenges to a federal rule governing interstate pollution and largely [dismissed](http://www.texastribune.org/2014/06/23/latest-epa-supreme-court-ruling-largely-loss-texas/) objections to climate change regulations. A federal appeals court also [ruled against](http://www.cadc.uscourts.gov/internet/opinions.nsf/284AC47088C07D0985257CBB004F0795/%24file/12-1100-1488346.pdf) Texas’ lawsuit over a federal rule on mercury and toxic emissions limits from coal plants, and the Supreme Court has [said](http://www.nytimes.com/2014/11/26/us/politics/supreme-court-to-hear-case-on-costs-of-clean-air-act.html) it will take up the case.
 </t>
   </si>
   <si>
@@ -1239,7 +1245,7 @@
     <t>text_5</t>
   </si>
   <si>
-    <t>But today, environmental advocates and doctors across the state worry that the air quality gains Texas has made in the last 15 years are eroding. San Antonio’s ozone levels [began rising](http://www.texastribune.org/2013/08/01/is-the-eagle-ford-shale-polluting-san-antonio/) in 2007, while the Dallas-Fort Worth region’s ozone decreases [appear to be flat-lining](http://www.texastribune.org/2014/07/16/dfw-struggles-air-quality-improvements/), although the state has said that may be due to an unusually hot summer in 2011. 
+    <t>Today, environmental advocates and doctors across the state worry that the air quality gains Texas has made in the last 15 years are eroding. San Antonio’s ozone levels [began rising](http://www.texastribune.org/2013/08/01/is-the-eagle-ford-shale-polluting-san-antonio/) in 2007, while the Dallas-Fort Worth region’s ozone decreases [appear to be flat-lining](http://www.texastribune.org/2014/07/16/dfw-struggles-air-quality-improvements/), although the state has said that may be due to an unusually hot summer in 2011. 
 Most recently, Texas’ top environmental officials blasted the EPA’s proposal to lower the ozone standard further, saying it would cost billions of dollars with no evidence of a public health benefit. That drew [criticism](http://www.texastribune.org/2014/10/21/battle-over-science-ozone-pollution/) from many health professionals and scientists, the overwhelming majority of whom say a lower ozone standard is critical to public health. 
 “There’s something like a thousand new scientific studies that show that air pollution is even more dangerous than we thought,” said Luke Metzger, director of the advocacy group Environment Texas. He called the state’s opposition to a new ozone standard “the latest example of Rick Perry and his appointees standing up for big polluters and putting them ahead of Texas families’ health and the protection of our natural resources.”
 *Disclosure: The Texas Public Policy foundation is a corporate sponsor of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).*
@@ -1291,7 +1297,13 @@
     <t>tweet_text</t>
   </si>
   <si>
+    <t>Under @GovernorPerry, Texas has become the nation’s hands-down leader in wind energy generation</t>
+  </si>
+  <si>
     <t>facebook_text</t>
+  </si>
+  <si>
+    <t>During Gov. Rick Perry's tenure, Texas has become the nation’s hands-down leader in wind energy generation</t>
   </si>
   <si>
     <t>facebook_art</t>
@@ -1347,6 +1359,18 @@
     <t>text_3</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Immigration</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Compassion, Tempered by a Broken System</t>
+  </si>
+  <si>
     <t>Perry also backed a $7 billion electrical transmission project to connect windy, largely empty West Texas to growing cities demanding more power. Completed a year ago, the [Competitive Renewable Energy Zone](http://www.texastribune.org/2013/10/14/7-billion-crez-project-nears-finish-aiding-wind-po/), or CREZ, initiative stretches nearly 3,600 miles and can send up to 18,500 megawatts of power — including from non-wind sources — across the state. 
 “That we were able to build thousands of miles of high-capacity transmission from West Texas to the Panhandle without landowners marching on the Capitol with pitchforks, it’s pretty remarkable,” said Railroad Commissioner Barry Smitherman, whom Perry appointed to the Public Utility Commission in 2004 and reappointed in 2007. “And the governor had our back on that.” 
 Along with decisions that specifically targeted wind, Smitherman said, Perry’s oversight while the state shifted to a competitive electricity market hastened investment in a variety of fuels, leaving Texas with a balanced energy portfolio.
@@ -1355,13 +1379,37 @@
 </t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
   </si>
   <si>
     <t>text_4</t>
   </si>
   <si>
-    <t>topic</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-globe</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1wzP3pX</t>
   </si>
   <si>
     <t>Hartnett White is not the only Texas Republican scrutinizing wind policy as Perry exits office. Comptroller Susan Combs suggested in September that wind energy has “an unfair market advantage over other power sources.” And PUC Chairwoman Donna Nelson, appointed by Perry in 2011, has [called for study](http://www.houstonchronicle.com/business/energy/article/Study-will-assess-shifting-transmission-costs-to-5607745.php#/0) into whether wind energy companies should chip in for power line upgrades — something no other types generator has been asked to do. 
@@ -1369,58 +1417,25 @@
 “In Texas we have implemented common-sense policies that have enabled us to build a successful wind industry that can thrive on its own,” Nashed added. 
 But some environmentalists wonder if Perry’s fervor has waned, pointing to his failure to defend wind energy producers in their recent political battles.
 “Perry is bipolar on wind. He plugged into when he saw he could get a political benefit. And now that the winds have changed in the Republican Party, he’s unplugged himself from one of his greatest environmental victories,” said Tom “Smitty” Smith, director of the Texas office of Public Citizen. 
-Disclosure: The Texas Public Policy foundation is a corporate sponsor of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed here. (http://www.texastribune.org/support-us/donors-and-members/)
+Disclosure: The Texas Public Policy foundation is a corporate sponsor of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).
 </t>
   </si>
   <si>
-    <t>Immigration</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_5</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Compassion, Tempered by a Broken System</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-globe</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>immigration</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1wzP3pX</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>tweet_text</t>
   </si>
   <si>
+    <t>.@GovernorPerry's track record on immigration: Compassion, tempered by a broken system </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>Gov. Rick Perry's track record on immigration includes compassion, tempered by a broken system.</t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -1436,7 +1451,7 @@
     <t>img_1_caption</t>
   </si>
   <si>
-    <t>Detainees sleep in a holding cell at a U.S. Customs and Border Protection processing facility, Wednesday, June 18, 2014, in Brownsville,Texas.</t>
+    <t>Detainees sleep in a holding cell at a U.S. Customs and Border Protection processing facility on June 18, 2014, in Brownsville.</t>
   </si>
   <si>
     <t>img_1_credit</t>
@@ -1454,7 +1469,7 @@
     <t>img_2_caption</t>
   </si>
   <si>
-    <t>Hundreds of people rally at the Texas Capitol protesting legislation that would require Texas peace officers to check immigration status of suspected illegal aliens accused of crimes. The bill would model similar laws that have caused uproar for months in Arizona.</t>
+    <t>Hundreds of people rally at the Texas Capitol protesting legislation that would require Texas peace officers to check the immigration status of suspected illegal aliens accused of crimes. The bill would model similar laws that have caused uproar for months in Arizona.</t>
   </si>
   <si>
     <t>img_2_credit</t>
@@ -1479,7 +1494,7 @@
   <si>
     <t>Thirteen years later, Perry’s frustration remains intact. But critics argue his compassion toward the undocumented population has waned since he took office, pointing to his recent track record on immigration. 
 Some residents say Perry has offended their communities with policies leading to “militarization” of the border, including his 2014 order deploying the Texas National Guard and a multimillion-dollar surge of state police to the Rio Grande Valley. The influx of law enforcement has since been expanded to include the entire Texas-Mexico border: a 1,254-mile stretch of terrain Perry has insisted is porous, and that Washington ignores.
-The tuition bill and border surge two bookend Perry’s evolution on immigration. It includes what would be considered a moderate stance as recently as 2007, one year after his predecessor, former President George W. Bush, failed to convince Congress to pass a comprehensive immigration reform bill.
+The tuition bill and border surge bookend Perry’s evolution on immigration. It includes what would be considered a moderate stance as recently as 2007, one year after his predecessor, former President George W. Bush, failed to convince Congress to pass a comprehensive immigration reform bill.
 “Illegal immigration drains the resources of our schools, our hospitals and our law enforcement agencies. But I do not believe it is realistic to deport 12 million people already here illegally,” Perry said in his 2007 inaugural speech, according to a transcript. “We have to understand why millions of people come here, and why many more have died trying. It is for something as basic as the freedom to find a job and feed their families.”</t>
   </si>
   <si>
@@ -1566,9 +1581,15 @@
     <t>tweet_text</t>
   </si>
   <si>
+    <t>.@GovernorPerry ushered in criminal justice reform by not standing in its way. </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>Gov. Rick Perry ushered in criminal justice reform by not standing in its way.</t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -1602,7 +1623,7 @@
     <t>img_2_caption</t>
   </si>
   <si>
-    <t>May 16th, 2013: Governor Rick Perry ceremonially signs Senate Bill 1611 which improves Texas criminal justice system ensuring a more open discovery process.</t>
+    <t>Gov. Rick Perry ceremonially signs a Senate bill that ensures a more open criminal court discovery process on May 16, 2013.</t>
   </si>
   <si>
     <t>img_2_credit</t>
@@ -1721,9 +1742,15 @@
     <t>tweet_text</t>
   </si>
   <si>
+    <t>As @GovernorPerry leaves office, a cloud hangs over his signature economic development initiative</t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>As Gov. Rick Perry leaves office, a cloud hangs over his signature economic development initiative — the Texas Enterprise Fund. </t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
@@ -1739,7 +1766,7 @@
     <t>img_1_caption</t>
   </si>
   <si>
-    <t>Gov. Rick Perry announces at the Holt Caterpillar facility in San Antonio, Texas that he will not seek a fourth full term as Texas Governor in 2014. </t>
+    <t>Gov. Rick Perry announces at the Holt Caterpillar facility in San Antonio that he will not seek a fourth full term as Texas governor. </t>
   </si>
   <si>
     <t>img_1_credit</t>
@@ -1987,176 +2014,182 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>457</v>
+        <v>462</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>463</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>458</v>
+        <v>464</v>
+      </c>
+      <c t="s" s="5" r="B8">
+        <v>465</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>459</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>460</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>462</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>464</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>466</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>468</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>470</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>472</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>475</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>478</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>484</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -2176,141 +2209,147 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>489</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>494</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>496</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>498</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>500</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>501</v>
+        <v>508</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>509</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>502</v>
+        <v>510</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>511</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>503</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>504</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>505</v>
+        <v>514</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>506</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>508</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>510</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>513</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>516</v>
+        <v>525</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>519</v>
+        <v>528</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>521</v>
+        <v>530</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>522</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18">
@@ -2332,378 +2371,168 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="65.57"/>
+    <col min="2" customWidth="1" max="2" width="59.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>22</v>
-      </c>
-      <c s="1" r="B5"/>
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>42</v>
+      </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c t="s" s="3" r="B9">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>41</v>
-      </c>
-      <c t="s" s="1" r="B10">
-        <v>44</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c t="s" s="3" r="B10">
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>46</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="C11">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c t="s" s="3" r="B11">
+        <v>63</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>61</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>68</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>81</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
         <v>90</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="C22">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>98</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>99</v>
-      </c>
-      <c t="s" s="1" r="C23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>101</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>103</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>104</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>106</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>107</v>
-      </c>
-      <c t="s" s="1" r="C26">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>109</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>111</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>112</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>114</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>115</v>
-      </c>
-      <c s="1" r="C29"/>
-    </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
-        <v>116</v>
-      </c>
-      <c t="s" s="1" r="B30">
-        <v>117</v>
-      </c>
-      <c s="1" r="C30"/>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>118</v>
-      </c>
-      <c t="s" s="1" r="B31">
-        <v>119</v>
-      </c>
-      <c s="1" r="C31"/>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>120</v>
-      </c>
-      <c t="s" s="1" r="B32">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
-        <v>122</v>
-      </c>
-      <c t="s" s="1" r="B33">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
-        <v>124</v>
-      </c>
-      <c t="s" s="1" r="B34">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>126</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>128</v>
-      </c>
-      <c t="s" s="1" r="B36">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37">
-      <c t="s" s="1" r="A37">
-        <v>130</v>
-      </c>
-      <c t="s" s="1" r="B37">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>132</v>
-      </c>
-      <c t="s" s="1" r="B38">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39">
-      <c t="s" s="1" r="A39">
-        <v>134</v>
-      </c>
-      <c t="s" s="1" r="B39">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
-        <v>136</v>
-      </c>
-      <c t="s" s="1" r="B40">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
     <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2714,168 +2543,378 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="59.71"/>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="B1">
         <v>7</v>
-      </c>
-      <c t="s" s="1" r="B1">
-        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>28</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c s="1" r="B5"/>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c t="s" s="3" r="B9">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>47</v>
-      </c>
-      <c t="s" s="3" r="B10">
-        <v>48</v>
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>49</v>
-      </c>
-      <c t="s" s="3" r="B11">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>35</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>59</v>
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>47</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="B17">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="B18">
         <v>78</v>
       </c>
-      <c t="s" s="1" r="C17">
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
         <v>79</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>96</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>98</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>103</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>106</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>108</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>111</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>113</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
+        <v>115</v>
+      </c>
+      <c t="s" s="1" r="B28">
+        <v>116</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" s="1" r="A29">
+        <v>118</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>119</v>
+      </c>
+      <c s="1" r="C29"/>
+    </row>
+    <row r="30">
+      <c t="s" s="1" r="A30">
+        <v>120</v>
+      </c>
+      <c t="s" s="1" r="B30">
+        <v>121</v>
+      </c>
+      <c s="1" r="C30"/>
+    </row>
+    <row r="31">
+      <c t="s" s="1" r="A31">
+        <v>122</v>
+      </c>
+      <c t="s" s="1" r="B31">
+        <v>123</v>
+      </c>
+      <c s="1" r="C31"/>
+    </row>
+    <row r="32">
+      <c t="s" s="1" r="A32">
+        <v>128</v>
+      </c>
+      <c t="s" s="1" r="B32">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33">
+      <c t="s" s="1" r="A33">
+        <v>133</v>
+      </c>
+      <c t="s" s="1" r="B33">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
+        <v>137</v>
+      </c>
+      <c t="s" s="1" r="B34">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>139</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>141</v>
+      </c>
+      <c t="s" s="1" r="B36">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
+        <v>145</v>
+      </c>
+      <c t="s" s="1" r="B37">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>148</v>
+      </c>
+      <c t="s" s="1" r="B38">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>151</v>
+      </c>
+      <c t="s" s="1" r="B39">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>153</v>
+      </c>
+      <c t="s" s="1" r="B40">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
     <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2891,69 +2930,69 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>139</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c t="s" s="4" r="B2">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c t="s" s="5" r="B8">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9">
@@ -3170,40 +3209,40 @@
         <v>206</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c t="s" s="1" r="B34">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c t="s" s="1" r="B35">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>216</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3223,37 +3262,37 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c t="s" s="6" r="B4">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5">
@@ -3710,123 +3749,129 @@
       <c t="s" s="1" r="A7">
         <v>333</v>
       </c>
+      <c t="s" s="1" r="B7">
+        <v>334</v>
+      </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>336</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3846,147 +3891,151 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c t="s" s="7" r="B4">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>377</v>
+        <v>379</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>380</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>378</v>
+        <v>381</v>
+      </c>
+      <c t="s" s="5" r="B8">
+        <v>382</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>389</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>400</v>
+        <v>415</v>
       </c>
     </row>
     <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>401</v>
-      </c>
+      <c s="1" r="A18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4005,7 +4054,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>399</v>
@@ -4013,171 +4062,177 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c t="s" s="1" r="B3">
         <v>405</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>413</v>
+        <v>416</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>417</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>414</v>
+        <v>418</v>
+      </c>
+      <c t="s" s="5" r="B8">
+        <v>419</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>434</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c t="s" s="1" r="B20">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>440</v>
+        <v>445</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
put nav-menu in container, adjust margin-left when open
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -92,7 +92,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+    <t>images/2014/12/17/perrylegacy-share_homepage_2.png</t>
   </si>
   <si>
     <t>text_intro</t>
@@ -106,28 +106,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
     <t>text_introb</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
@@ -137,34 +116,16 @@
 </t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>fa-car</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_1_header</t>
   </si>
   <si>
-    <t>slug</t>
-  </si>
-  <si>
     <t>Longevity</t>
   </si>
   <si>
-    <t>transportation</t>
-  </si>
-  <si>
     <t>text_1</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1IVfJqr</t>
   </si>
   <si>
     <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
@@ -175,24 +136,6 @@
   </si>
   <si>
     <t>text_1b</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
@@ -205,25 +148,13 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>lead_art</t>
-  </si>
-  <si>
     <t>text_2_header</t>
   </si>
   <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
     <t>The Texas Miracle</t>
   </si>
   <si>
     <t>text_2</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
@@ -234,21 +165,6 @@
   </si>
   <si>
     <t>text_2b</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -262,18 +178,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>text_3_header</t>
-  </si>
-  <si>
-    <t>text_2</t>
   </si>
   <si>
     <t>The Margins Tax
@@ -283,44 +188,14 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3</t>
-  </si>
-  <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
 At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
   </si>
   <si>
-    <t>text_4</t>
-  </si>
-  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_3b</t>
-  </si>
-  <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applies to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
@@ -350,12 +225,6 @@
   </si>
   <si>
     <t>text_4b</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Health Care</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -376,13 +245,7 @@
     <t>The Indictment</t>
   </si>
   <si>
-    <t>headline</t>
-  </si>
-  <si>
     <t>text_5</t>
-  </si>
-  <si>
-    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
   </si>
   <si>
     <t>Political forecasts called for smooth sailing as Perry prepared for the final victory lap at the end of his long tenure. A felony indictment changed all that.
@@ -444,40 +307,13 @@
 </t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
     <t>img_2_url</t>
   </si>
   <si>
-    <t>fa-plus-square</t>
-  </si>
-  <si>
     <t>Perry-Legacy-110.JPG</t>
   </si>
   <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>health-care</t>
-  </si>
-  <si>
     <t>img_2_caption</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1DDl1a9</t>
   </si>
   <si>
     <t>Texas Gov. Rick Perry (l) shares a laugh with Boeing CEO of Defense, Space and Security Dennis Muilenburg (r) at a bill-signing ceremony at the Boeing plant in San Antonio. Perry signed a state law exempting certain aircraft from tax assessments when temporarily housed in Texas facilities.</t>
@@ -499,13 +335,7 @@
     <t>img_3_caption</t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
     <t>Texas Gov. Rick Perry appears in Travis County Court to answer charges in an indictment regarding his veto of funding for the Travis County Public Integrity Unit.</t>
-  </si>
-  <si>
-    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
   </si>
   <si>
     <t>img_3_credit</t>
@@ -515,34 +345,195 @@
 </t>
   </si>
   <si>
+    <t>img_4_url</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-093.JPG</t>
+  </si>
+  <si>
+    <t>img_4_caption</t>
+  </si>
+  <si>
+    <t>Then-state Rep. Rick Perry listens to Rep. Robert Earley (D-Portland) during the 69th Legislature on May 13, 1985.</t>
+  </si>
+  <si>
+    <t>img_4_credit</t>
+  </si>
+  <si>
+    <t>Texas State Library &amp; Archives Commision</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1IVfJqr</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
-    <t>img_4_url</t>
-  </si>
-  <si>
-    <t>Perry-Legacy-093.JPG</t>
+    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>images/2014/12/17/perrylegacy-share_transpo.png</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
+    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4</t>
+  </si>
+  <si>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1DDl1a9</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
   </si>
   <si>
     <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
   </si>
   <si>
-    <t>img_4_caption</t>
-  </si>
-  <si>
-    <t>Then-state Rep. Rick Perry listens to Rep. Robert Earley (D-Portland) during the 69th Legislature on May 13, 1985.</t>
-  </si>
-  <si>
-    <t>img_4_credit</t>
-  </si>
-  <si>
-    <t>Texas State Library &amp; Archives Commision</t>
-  </si>
-  <si>
     <t>facebook_art</t>
-  </si>
-  <si>
-    <t>lead_art</t>
   </si>
   <si>
     <t>img_1</t>
@@ -703,16 +694,37 @@
     <t>One of Perry’s most controversial decisions as governor was his executive order requiring girls entering the sixth grade to be vaccinated against the human papillomavirus, the principal cause of cervical cancer.</t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
   </si>
   <si>
     <t>text_4b</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Higher Education</t>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Heavy Hand in Academic Affairs </t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>Perry’s February 2007 order was soon overturned by lawmakers. At the time, he stood behind his decision, saying that a thousand women would likely be diagnosed with the disease in the next year.
@@ -725,34 +737,13 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Heavy Hand in Academic Affairs </t>
-  </si>
-  <si>
     <t>text_5_header</t>
   </si>
   <si>
     <t>CPRIT</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
     <t>text_5</t>
-  </si>
-  <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-graduation-cap</t>
   </si>
   <si>
     <t>Perry was a leading proponent of the Cancer Prevention and Research Institute of Texas, a grant-making entity approved by voters in 2007 to spend $3 billion on cancer research, plus an additional $600 million appropriated by the Legislature for 2012-13. 
@@ -802,7 +793,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_highered_1.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1018,7 +1009,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_publiced_1.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1147,7 +1138,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_enviro.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1242,7 +1233,34 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
     <t>text_5</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Texas Now Hands-Down Leader in Wind Power</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-bolt</t>
   </si>
   <si>
     <t>Today, environmental advocates and doctors across the state worry that the air quality gains Texas has made in the last 15 years are eroding. San Antonio’s ozone levels [began rising](http://www.texastribune.org/2013/08/01/is-the-eagle-ford-shale-polluting-san-antonio/) in 2007, while the Dallas-Fort Worth region’s ozone decreases [appear to be flat-lining](http://www.texastribune.org/2014/07/16/dfw-struggles-air-quality-improvements/), although the state has said that may be due to an unusually hot summer in 2011. 
@@ -1255,33 +1273,6 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Texas Now Hands-Down Leader in Wind Power</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Jim Malewitz](http://www.texastribune.org/about/staff/jim-malewitz/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-bolt</t>
-  </si>
-  <si>
     <t>slug</t>
   </si>
   <si>
@@ -1309,7 +1300,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_energy_4.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1359,18 +1350,6 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Immigration</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Compassion, Tempered by a Broken System</t>
-  </si>
-  <si>
     <t>Perry also backed a $7 billion electrical transmission project to connect windy, largely empty West Texas to growing cities demanding more power. Completed a year ago, the [Competitive Renewable Energy Zone](http://www.texastribune.org/2013/10/14/7-billion-crez-project-nears-finish-aiding-wind-po/), or CREZ, initiative stretches nearly 3,600 miles and can send up to 18,500 megawatts of power — including from non-wind sources — across the state. 
 “That we were able to build thousands of miles of high-capacity transmission from West Texas to the Panhandle without landowners marching on the Capitol with pitchforks, it’s pretty remarkable,” said Railroad Commissioner Barry Smitherman, whom Perry appointed to the Public Utility Commission in 2004 and reappointed in 2007. “And the governor had our back on that.” 
 Along with decisions that specifically targeted wind, Smitherman said, Perry’s oversight while the state shifted to a competitive electricity market hastened investment in a variety of fuels, leaving Texas with a balanced energy portfolio.
@@ -1379,37 +1358,10 @@
 </t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_4</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-globe</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>immigration</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1wzP3pX</t>
   </si>
   <si>
     <t>Hartnett White is not the only Texas Republican scrutinizing wind policy as Perry exits office. Comptroller Susan Combs suggested in September that wind energy has “an unfair market advantage over other power sources.” And PUC Chairwoman Donna Nelson, appointed by Perry in 2011, has [called for study](http://www.houstonchronicle.com/business/energy/article/Study-will-assess-shifting-transmission-costs-to-5607745.php#/0) into whether wind energy companies should chip in for power line upgrades — something no other types generator has been asked to do. 
@@ -1424,6 +1376,45 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Immigration</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Compassion, Tempered by a Broken System</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Julian Aguilar](http://www.texastribune.org/about/staff/julian-aguilar/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-globe</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>immigration</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1wzP3pX</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
@@ -1439,7 +1430,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_immigration_1.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1593,7 +1584,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_justice_1.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1754,7 +1745,7 @@
     <t>facebook_art</t>
   </si>
   <si>
-    <t>lead_art</t>
+    <t>images/2014/12/17/perrylegacy-share_enterprise.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1889,7 +1880,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
@@ -1900,14 +1891,17 @@
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3" applyFill="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4" applyFill="1">
       <alignment/>
+    </xf>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
+      <alignment horizontal="left"/>
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
       <alignment/>
@@ -2014,183 +2008,150 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>450</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>451</v>
+        <v>494</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>452</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>453</v>
+        <v>496</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>454</v>
+        <v>497</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>455</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>456</v>
+        <v>499</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>457</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>458</v>
+        <v>501</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>459</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>460</v>
+        <v>503</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>461</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>462</v>
+        <v>505</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>463</v>
+        <v>506</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>464</v>
-      </c>
-      <c t="s" s="5" r="B8">
-        <v>465</v>
+        <v>507</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>508</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>466</v>
+        <v>509</v>
+      </c>
+      <c t="s" s="7" r="B9">
+        <v>510</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>467</v>
+        <v>511</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>512</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>468</v>
+        <v>513</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>469</v>
+        <v>514</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>470</v>
+        <v>515</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>471</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>472</v>
+        <v>517</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>473</v>
+        <v>518</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>519</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>474</v>
+        <v>520</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>475</v>
+        <v>521</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>522</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>476</v>
+        <v>523</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>477</v>
+        <v>524</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>525</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>478</v>
+        <v>526</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>479</v>
+        <v>527</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>528</v>
       </c>
     </row>
     <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>480</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>481</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>483</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>484</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>486</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>487</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>489</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>490</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>492</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>493</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>494</v>
-      </c>
+      <c s="1" r="A17"/>
+      <c s="1" r="C17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2209,152 +2170,181 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>495</v>
+        <v>446</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>496</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>497</v>
+        <v>448</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>498</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>499</v>
+        <v>450</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>500</v>
+        <v>451</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>501</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>502</v>
+        <v>453</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>503</v>
+        <v>454</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>504</v>
+        <v>455</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>505</v>
+        <v>456</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>506</v>
+        <v>457</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>507</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>508</v>
+        <v>459</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>509</v>
+        <v>460</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>510</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>511</v>
+        <v>461</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>462</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>512</v>
+        <v>463</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>464</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>513</v>
+        <v>465</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>466</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>514</v>
+        <v>467</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>515</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>516</v>
+        <v>469</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>517</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>519</v>
+        <v>472</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>520</v>
+        <v>473</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>521</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>522</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>523</v>
+        <v>475</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>524</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>525</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>526</v>
+        <v>477</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>527</v>
+        <v>478</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>528</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>529</v>
+        <v>480</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>530</v>
+        <v>481</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>531</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18">
-      <c s="1" r="A18"/>
-      <c s="1" r="C18"/>
+      <c t="s" s="1" r="A18">
+        <v>483</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>484</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>486</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>487</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>489</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>490</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>491</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2371,168 +2361,377 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="59.71"/>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>40</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>42</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c s="1" r="B5"/>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>50</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>52</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>53</v>
-      </c>
-      <c t="s" s="3" r="B9">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>57</v>
-      </c>
-      <c t="s" s="3" r="B10">
-        <v>59</v>
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>62</v>
-      </c>
-      <c t="s" s="3" r="B11">
-        <v>63</v>
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>70</v>
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>75</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>80</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>84</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>48</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>52</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>57</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>60</v>
+      </c>
+      <c t="s" s="1" r="C23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>64</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>65</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>68</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>70</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="B28">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" s="1" r="A29">
+        <v>75</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>76</v>
+      </c>
+      <c s="1" r="C29"/>
+    </row>
+    <row r="30">
+      <c t="s" s="1" r="A30">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="B30">
+        <v>78</v>
+      </c>
+      <c s="1" r="C30"/>
+    </row>
+    <row r="31">
+      <c t="s" s="1" r="A31">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="B31">
+        <v>80</v>
+      </c>
+      <c s="1" r="C31"/>
+    </row>
+    <row r="32">
+      <c t="s" s="1" r="A32">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="B32">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33">
+      <c t="s" s="1" r="A33">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="B33">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="B34">
         <v>86</v>
       </c>
-      <c t="s" s="1" r="B17">
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
         <v>89</v>
       </c>
-      <c t="s" s="1" r="C17">
+      <c t="s" s="1" r="B36">
         <v>90</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="B37">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="B38">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="B39">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>97</v>
+      </c>
+      <c t="s" s="1" r="B40">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
   </hyperlinks>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2543,376 +2742,156 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="65.57"/>
+    <col min="2" customWidth="1" max="2" width="59.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>7</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>9</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>12</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>15</v>
-      </c>
-      <c s="1" r="B5"/>
+        <v>108</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>109</v>
+      </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>17</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>19</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>21</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>22</v>
-      </c>
-      <c t="s" s="3" r="B9">
-        <v>23</v>
+        <v>116</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>117</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>24</v>
-      </c>
-      <c t="s" s="1" r="B10">
-        <v>25</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>26</v>
+        <v>118</v>
+      </c>
+      <c t="s" s="3" r="B10">
+        <v>119</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>35</v>
-      </c>
-      <c t="s" s="1" r="C11">
-        <v>37</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>41</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>47</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>56</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>60</v>
+        <v>131</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>66</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>72</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>79</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="C22">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>98</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>101</v>
-      </c>
-      <c t="s" s="1" r="C23">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>103</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>106</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>108</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>110</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>111</v>
-      </c>
-      <c t="s" s="1" r="C26">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>113</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>115</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>116</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>118</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>119</v>
-      </c>
-      <c s="1" r="C29"/>
-    </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
-        <v>120</v>
-      </c>
-      <c t="s" s="1" r="B30">
-        <v>121</v>
-      </c>
-      <c s="1" r="C30"/>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>122</v>
-      </c>
-      <c t="s" s="1" r="B31">
-        <v>123</v>
-      </c>
-      <c s="1" r="C31"/>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>128</v>
-      </c>
-      <c t="s" s="1" r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
-        <v>133</v>
-      </c>
-      <c t="s" s="1" r="B33">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
-        <v>137</v>
-      </c>
-      <c t="s" s="1" r="B34">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>139</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>141</v>
-      </c>
-      <c t="s" s="1" r="B36">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="37">
-      <c t="s" s="1" r="A37">
-        <v>145</v>
-      </c>
-      <c t="s" s="1" r="B37">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>148</v>
-      </c>
-      <c t="s" s="1" r="B38">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39">
-      <c t="s" s="1" r="A39">
-        <v>151</v>
-      </c>
-      <c t="s" s="1" r="B39">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
-        <v>153</v>
-      </c>
-      <c t="s" s="1" r="B40">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId2"/>
   </hyperlinks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -2930,187 +2909,193 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>105</v>
-      </c>
-      <c t="s" s="4" r="B2">
-        <v>107</v>
+        <v>138</v>
+      </c>
+      <c t="s" s="5" r="B2">
+        <v>139</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>129</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>132</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>147</v>
-      </c>
-      <c t="s" s="5" r="B8">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>152</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>156</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>155</v>
+      </c>
+      <c s="1" r="C10"/>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
+        <v>156</v>
+      </c>
+      <c t="s" s="1" r="B11">
         <v>157</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>158</v>
       </c>
       <c s="1" r="C11"/>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
+        <v>158</v>
+      </c>
+      <c t="s" s="1" r="B12">
         <v>159</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>160</v>
       </c>
       <c s="1" r="C12"/>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
+        <v>160</v>
+      </c>
+      <c t="s" s="1" r="B13">
         <v>161</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>162</v>
       </c>
       <c s="1" r="C13"/>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
+        <v>162</v>
+      </c>
+      <c t="s" s="1" r="B14">
         <v>163</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>164</v>
       </c>
       <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
+        <v>164</v>
+      </c>
+      <c t="s" s="1" r="B15">
         <v>165</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>166</v>
       </c>
       <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
+        <v>166</v>
+      </c>
+      <c t="s" s="1" r="B16">
         <v>167</v>
-      </c>
-      <c t="s" s="1" r="B16">
-        <v>168</v>
       </c>
       <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
+        <v>168</v>
+      </c>
+      <c t="s" s="1" r="B17">
         <v>169</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>170</v>
       </c>
       <c s="1" r="C17"/>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
+        <v>170</v>
+      </c>
+      <c t="s" s="1" r="B18">
         <v>171</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>172</v>
       </c>
       <c s="1" r="C18"/>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
+        <v>172</v>
+      </c>
+      <c t="s" s="1" r="B19">
         <v>173</v>
       </c>
-      <c t="s" s="1" r="B19">
+      <c t="s" s="1" r="C19">
         <v>174</v>
       </c>
-      <c s="1" r="C19"/>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
         <v>175</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c s="1" r="B20"/>
+      <c t="s" s="1" r="C20">
         <v>176</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
+        <v>177</v>
+      </c>
+      <c t="s" s="1" r="B21">
         <v>178</v>
-      </c>
-      <c s="1" r="B21"/>
-      <c t="s" s="1" r="C21">
-        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
+        <v>179</v>
+      </c>
+      <c t="s" s="5" r="B22">
         <v>180</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c t="s" s="1" r="C22">
         <v>181</v>
       </c>
     </row>
@@ -3118,7 +3103,7 @@
       <c t="s" s="1" r="A23">
         <v>182</v>
       </c>
-      <c t="s" s="4" r="B23">
+      <c t="s" s="1" r="B23">
         <v>183</v>
       </c>
       <c t="s" s="1" r="C23">
@@ -3132,15 +3117,15 @@
       <c t="s" s="1" r="B24">
         <v>186</v>
       </c>
-      <c t="s" s="1" r="C24">
-        <v>187</v>
-      </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
+        <v>187</v>
+      </c>
+      <c t="s" s="1" r="B25">
         <v>188</v>
       </c>
-      <c t="s" s="1" r="B25">
+      <c t="s" s="1" r="C25">
         <v>189</v>
       </c>
     </row>
@@ -3151,15 +3136,15 @@
       <c t="s" s="1" r="B26">
         <v>191</v>
       </c>
-      <c t="s" s="1" r="C26">
-        <v>192</v>
-      </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
+        <v>192</v>
+      </c>
+      <c t="s" s="1" r="B27">
         <v>193</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c t="s" s="1" r="C27">
         <v>194</v>
       </c>
     </row>
@@ -3181,68 +3166,57 @@
       <c t="s" s="1" r="B29">
         <v>199</v>
       </c>
-      <c t="s" s="1" r="C29">
-        <v>200</v>
-      </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
+        <v>200</v>
+      </c>
+      <c t="s" s="1" r="B30">
         <v>201</v>
       </c>
-      <c t="s" s="1" r="B30">
-        <v>202</v>
+      <c t="s" s="1" r="C30">
+        <v>203</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>209</v>
-      </c>
-      <c t="s" s="1" r="C32">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>214</v>
+        <v>218</v>
+      </c>
+      <c t="s" s="1" r="C33">
+        <v>219</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c t="s" s="1" r="B34">
         <v>221</v>
       </c>
       <c t="s" s="1" r="C34">
         <v>222</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>223</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>224</v>
-      </c>
-      <c t="s" s="1" r="C35">
-        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3262,126 +3236,135 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c t="s" s="6" r="B4">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>232</v>
-      </c>
-      <c t="s" s="5" r="B8">
-        <v>233</v>
+        <v>229</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>230</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>234</v>
+        <v>231</v>
+      </c>
+      <c t="s" s="7" r="B9">
+        <v>232</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>235</v>
+        <v>233</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>234</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
+        <v>235</v>
+      </c>
+      <c t="s" s="1" r="B11">
         <v>236</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>237</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
+        <v>237</v>
+      </c>
+      <c t="s" s="1" r="B12">
         <v>238</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>239</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
+        <v>239</v>
+      </c>
+      <c t="s" s="1" r="B13">
         <v>240</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>241</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
+        <v>241</v>
+      </c>
+      <c t="s" s="1" r="B14">
         <v>242</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>243</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
+        <v>243</v>
+      </c>
+      <c t="s" s="1" r="B15">
         <v>244</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>245</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
+        <v>245</v>
+      </c>
+      <c t="s" s="1" r="B16">
         <v>246</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c t="s" s="1" r="C16">
         <v>247</v>
       </c>
     </row>
@@ -3400,18 +3383,18 @@
       <c t="s" s="1" r="A18">
         <v>251</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c t="s" s="5" r="B18">
         <v>252</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>253</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
+        <v>253</v>
+      </c>
+      <c t="s" s="1" r="B19">
         <v>254</v>
       </c>
-      <c t="s" s="4" r="B19">
+      <c t="s" s="1" r="C19">
         <v>255</v>
       </c>
     </row>
@@ -3433,15 +3416,15 @@
       <c t="s" s="1" r="B21">
         <v>260</v>
       </c>
-      <c t="s" s="1" r="C21">
-        <v>261</v>
-      </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
+        <v>261</v>
+      </c>
+      <c t="s" s="1" r="B22">
         <v>262</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c t="s" s="1" r="C22">
         <v>263</v>
       </c>
     </row>
@@ -3452,15 +3435,15 @@
       <c t="s" s="1" r="B23">
         <v>265</v>
       </c>
-      <c t="s" s="1" r="C23">
-        <v>266</v>
-      </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
+        <v>266</v>
+      </c>
+      <c t="s" s="1" r="B24">
         <v>267</v>
       </c>
-      <c t="s" s="1" r="B24">
+      <c t="s" s="1" r="C24">
         <v>268</v>
       </c>
     </row>
@@ -3482,15 +3465,15 @@
       <c t="s" s="1" r="B26">
         <v>273</v>
       </c>
-      <c t="s" s="1" r="C26">
-        <v>274</v>
-      </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
+        <v>274</v>
+      </c>
+      <c t="s" s="1" r="B27">
         <v>275</v>
       </c>
-      <c t="s" s="1" r="B27">
+      <c t="s" s="1" r="C27">
         <v>276</v>
       </c>
     </row>
@@ -3503,17 +3486,6 @@
       </c>
       <c t="s" s="1" r="C28">
         <v>279</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>280</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>281</v>
-      </c>
-      <c t="s" s="1" r="C29">
-        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3533,102 +3505,111 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>300</v>
+        <v>297</v>
+      </c>
+      <c t="s" s="7" r="B9">
+        <v>298</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>301</v>
+        <v>299</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>300</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
+        <v>301</v>
+      </c>
+      <c t="s" s="1" r="B11">
         <v>302</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>303</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
+        <v>303</v>
+      </c>
+      <c t="s" s="1" r="B12">
         <v>304</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>305</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
+        <v>305</v>
+      </c>
+      <c t="s" s="1" r="B13">
         <v>306</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c t="s" s="1" r="C13">
         <v>307</v>
       </c>
     </row>
@@ -3663,17 +3644,6 @@
       </c>
       <c t="s" s="1" r="C16">
         <v>316</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>317</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>318</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3690,189 +3660,152 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="2" customWidth="1" max="2" width="63.71"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>320</v>
+        <v>360</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>321</v>
+        <v>362</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>323</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>324</v>
+        <v>365</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>326</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>327</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>328</v>
+        <v>368</v>
+      </c>
+      <c t="s" s="8" r="B4">
+        <v>369</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>329</v>
+        <v>372</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>330</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>331</v>
+        <v>374</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>332</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>333</v>
+        <v>376</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>334</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>335</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>336</v>
+        <v>378</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>379</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>337</v>
+        <v>380</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>381</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>338</v>
+        <v>382</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>383</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>339</v>
+        <v>384</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>341</v>
+        <v>386</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>342</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>343</v>
+        <v>388</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>344</v>
+        <v>389</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>390</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>345</v>
+        <v>391</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>346</v>
+        <v>392</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>393</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>347</v>
+        <v>394</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>348</v>
+        <v>395</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>396</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>349</v>
+        <v>397</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>350</v>
+        <v>398</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>399</v>
       </c>
     </row>
     <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>351</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>352</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>354</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>355</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>357</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>358</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>360</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>361</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>363</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>364</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>365</v>
-      </c>
+      <c s="1" r="A17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3888,154 +3821,187 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" customWidth="1" max="2" width="63.71"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>366</v>
+        <v>317</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>367</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>368</v>
+        <v>319</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>369</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>370</v>
+        <v>321</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>371</v>
+        <v>322</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>372</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>373</v>
-      </c>
-      <c t="s" s="7" r="B4">
-        <v>374</v>
+        <v>324</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>325</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>375</v>
+        <v>326</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>376</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>377</v>
+        <v>328</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>378</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>379</v>
+        <v>330</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>380</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>381</v>
-      </c>
-      <c t="s" s="5" r="B8">
-        <v>382</v>
+        <v>332</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>333</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>383</v>
+        <v>334</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>335</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>384</v>
+        <v>336</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>337</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>385</v>
+        <v>338</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>386</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>387</v>
+        <v>340</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>388</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>389</v>
+        <v>342</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>390</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>391</v>
+        <v>344</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>392</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>393</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>394</v>
+        <v>346</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>395</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>396</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>397</v>
+        <v>348</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>404</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>406</v>
+        <v>351</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>414</v>
+        <v>352</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>415</v>
+        <v>353</v>
       </c>
     </row>
     <row r="18">
-      <c s="1" r="A18"/>
+      <c t="s" s="1" r="A18">
+        <v>354</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>355</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>357</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>358</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>361</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>370</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>371</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4054,131 +4020,140 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c t="s" s="1" r="B3">
         <v>405</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
+        <v>407</v>
+      </c>
+      <c t="s" s="1" r="B4">
         <v>408</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>409</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
+        <v>409</v>
+      </c>
+      <c t="s" s="1" r="B5">
         <v>410</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>411</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
+        <v>411</v>
+      </c>
+      <c t="s" s="3" r="B6">
         <v>412</v>
-      </c>
-      <c t="s" s="3" r="B6">
-        <v>413</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>418</v>
-      </c>
-      <c t="s" s="5" r="B8">
-        <v>419</v>
+        <v>415</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>416</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>420</v>
+        <v>417</v>
+      </c>
+      <c t="s" s="7" r="B9">
+        <v>418</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>421</v>
+        <v>419</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>420</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
+        <v>421</v>
+      </c>
+      <c t="s" s="1" r="B11">
         <v>422</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>423</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
+        <v>423</v>
+      </c>
+      <c t="s" s="1" r="B12">
         <v>424</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>425</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
+        <v>425</v>
+      </c>
+      <c t="s" s="1" r="B13">
         <v>426</v>
       </c>
-      <c t="s" s="1" r="B13">
-        <v>427</v>
-      </c>
+      <c s="1" r="C13"/>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
+        <v>427</v>
+      </c>
+      <c t="s" s="1" r="B14">
         <v>428</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>429</v>
       </c>
       <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
+        <v>429</v>
+      </c>
+      <c t="s" s="1" r="B15">
         <v>430</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>431</v>
       </c>
       <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
+        <v>431</v>
+      </c>
+      <c t="s" s="1" r="B16">
         <v>432</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c t="s" s="1" r="C16">
         <v>433</v>
       </c>
-      <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
@@ -4222,17 +4197,6 @@
       </c>
       <c t="s" s="1" r="C20">
         <v>445</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>446</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>447</v>
-      </c>
-      <c t="s" s="1" r="C21">
-        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 5.5 sections, neena copy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -50,7 +50,7 @@
     <t>headline</t>
   </si>
   <si>
-    <t>6 Things We Won't Forget About Texas' Longest-Serving Governor</t>
+    <t>Five — And a Half — Things We Won't Forget About Texas' Longest-Serving Governor</t>
   </si>
   <si>
     <t>byline</t>
@@ -77,91 +77,28 @@
     <t>trib.it/perry-legacy</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1IVfJqr</t>
-  </si>
-  <si>
     <t>tweet_text</t>
   </si>
   <si>
     <t>The six things Texans won’t forget about @GovernorPerry: </t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
-  </si>
-  <si>
     <t>facebook_text</t>
   </si>
   <si>
-    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
+    <t>Here are the six things Texans won't forget about Rick Perry, the state's longest-serving governor: </t>
   </si>
   <si>
     <t>facebook_art</t>
   </si>
   <si>
-    <t>Here are the six things Texans won't forget about Rick Perry, the state's longest-serving governor: </t>
-  </si>
-  <si>
-    <t>perrylegacy-fb-share_transpo.png</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
     <t>perrylegacy-fb-share_home.png</t>
   </si>
   <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
-  </si>
-  <si>
     <t>text_intro</t>
   </si>
   <si>
-    <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that concluded with his service as the longest-serving governor in Texas history. 
+    <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that concluded with his being the longest-serving governor in Texas history. 
 Perry’s 14-year tenure in the state’s highest office coincided with the ever-tightening grip of Republican rule, sweeping conservative reforms and more than a few controversies.
 It was also marked by unprecedented population growth and an enviable economic expansion in Texas. The state led the nation in job creation during Perry’s reign, and it added more people than any other state between 2000 and 2010 — numbers that continue to grow.</t>
   </si>
@@ -169,58 +106,59 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
     <t>text_introb</t>
   </si>
   <si>
-    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
 Boiling down Perry’s legacy into a few bullet points isn’t easy and will undoubtedly leave supporters and detractors alike unsatisfied.
 But memories fade, and not every event that seems newsworthy today will stand out in the history books or become part of the state’s collective political memory. (And there could be a new set of mileposts on a future legacy tour if Perry runs for president again — a move he is currently considering.)
-With those caveats, here are six things people will probably remember years after Perry has left the Texas Governor’s Mansion.
+With those caveats, here are five — and a half — things people will probably remember years after Perry has left the Texas Governor’s Mansion.
 </t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>byline</t>
   </si>
   <si>
     <t>text_1_header</t>
   </si>
   <si>
-    <t>Longevity</t>
-  </si>
-  <si>
-    <t>text_2</t>
+    <t>1. Longevity</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
   </si>
   <si>
     <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
@@ -230,22 +168,16 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>text_3</t>
+    <t>share_url</t>
   </si>
   <si>
     <t>text_1b</t>
   </si>
   <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4</t>
+    <t>trib.it/1IVfJqr</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
   </si>
   <si>
     <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
@@ -255,35 +187,67 @@
 “I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)</t>
   </si>
   <si>
-    <t>markdown</t>
+    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
   </si>
   <si>
     <t>text_2_header</t>
   </si>
   <si>
-    <t>The Texas Miracle</t>
+    <t>2. The Texas Miracle</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
   </si>
   <si>
     <t>text_2</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>perrylegacy-fb-share_transpo.png</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
 Critics will find plenty wrong with a state that has the highest percentage of [uninsured](http://kxan.com/2014/09/16/texas-no-1-for-uninsured-rate-again/) residents in the nation, produces [more](http://www.nytimes.com/2014/07/13/us/texas-leader-in-greenhouse-gases-stands-vulnerable-to-their-effects.html?_r=1) greenhouse gas emissions than any other state and has [led the nation](https://www.texastribune.org/2014/09/11/workplace-deaths-decline-texas-still-no-1/) in workplace fatalities for 10 of the last 14 years. </t>
   </si>
   <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_2b</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
+  </si>
+  <si>
+    <t>text_1</t>
+  </si>
+  <si>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -297,11 +261,26 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2</t>
+  </si>
+  <si>
     <t>text_3_header</t>
   </si>
   <si>
-    <t>The Margins Tax
+    <t>3. The Margins Tax
 </t>
+  </si>
+  <si>
+    <t>text_3</t>
+  </si>
+  <si>
+    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_3</t>
@@ -315,6 +294,15 @@
   </si>
   <si>
     <t>text_3b</t>
+  </si>
+  <si>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applies to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
@@ -331,7 +319,7 @@
     <t>text_4_header</t>
   </si>
   <si>
-    <t>The Oops Moment</t>
+    <t>4. The Oops Moment</t>
   </si>
   <si>
     <t>text_4</t>
@@ -346,16 +334,7 @@
     <t>text_4b</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Health Care</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
+    <t>text_4</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -370,10 +349,19 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
     <t>text_5_header</t>
   </si>
   <si>
-    <t>The Indictment</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>5. The Indictment</t>
   </si>
   <si>
     <t>text_5</t>
@@ -390,48 +378,21 @@
     <t>text_5b</t>
   </si>
   <si>
-    <t>byline</t>
-  </si>
-  <si>
     <t>On Aug. 15, a grand jury indicted Perry on two felony counts — abuse of official capacity and coercion of a public servant — stemming from his 2013 veto of funds destined for a special investigative unit inside the Travis County district attorney’s office.
 Perry blasted the prosecution as a politically motivated “farce,” and has trotted out [legal scholars](https://www.texastribune.org/2014/11/10/bipartisan-group-lawyers-want-perry-case-dismissed/) from both sides of the spectrum to criticize it.
 No matter what happens, Perry’s 11th-hour ride through the criminal justice system guarantees a mention in the history books. He’s the [first governor since James “Pa” Ferguson](http://www.texastribune.org/2014/08/17/you-couldnt-make-stuff-1917-either/) to get indicted, and the uncommonly brash way he has confronted the allegations provided a unique twist to the way potential presidential contenders handle criminal justice challenges. </t>
   </si>
   <si>
-    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_6_header</t>
   </si>
   <si>
-    <t>Swagger</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-plus-square</t>
+    <t>5.5. Swagger</t>
   </si>
   <si>
     <t>text_6</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>health-care</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1DDl1a9</t>
   </si>
   <si>
     <t>Granted, swagger is not an event, a policy accomplishment or a political milestone. It’s a style — a cocky way of walking, talking and conducting business. And Perry has made it his calling card.
@@ -465,28 +426,16 @@
 </t>
   </si>
   <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
     <t>img_2_url</t>
   </si>
   <si>
     <t>Perry-Legacy-110.JPG</t>
   </si>
   <si>
-    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
-  </si>
-  <si>
     <t>img_2_caption</t>
   </si>
   <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
     <t>Texas Gov. Rick Perry (l) shares a laugh with Boeing CEO of Defense, Space and Security Dennis Muilenburg (r) at a bill-signing ceremony at the Boeing plant in San Antonio. Perry signed a state law exempting certain aircraft from tax assessments when temporarily housed in Texas facilities.</t>
-  </si>
-  <si>
-    <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
   </si>
   <si>
     <t>img_2_credit</t>
@@ -496,31 +445,16 @@
 </t>
   </si>
   <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
     <t>img_3_url</t>
   </si>
   <si>
-    <t>perrylegacy-fb-share_health.png</t>
-  </si>
-  <si>
     <t>Perry-Legacy-096.JPG</t>
   </si>
   <si>
-    <t>img_1</t>
-  </si>
-  <si>
     <t>img_3_caption</t>
   </si>
   <si>
-    <t>Perry-Legacy-101.JPG</t>
-  </si>
-  <si>
     <t>Texas Gov. Rick Perry appears in Travis County Court to answer charges in an indictment regarding his veto of funding for the Travis County Public Integrity Unit.</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
   </si>
   <si>
     <t>img_3_credit</t>
@@ -530,37 +464,103 @@
 </t>
   </si>
   <si>
+    <t>img_4_url</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-093.JPG</t>
+  </si>
+  <si>
+    <t>img_4_caption</t>
+  </si>
+  <si>
+    <t>Then-state Rep. Rick Perry listens to Rep. Robert Earley (D-Portland) during the 69th Legislature on May 13, 1985.</t>
+  </si>
+  <si>
+    <t>img_4_credit</t>
+  </si>
+  <si>
+    <t>Texas State Library &amp; Archives Commision</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Health Care</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Battles With the Feds — and at Home — Over Medicaid, Women's Health</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Alexa Ura](http://www.texastribune.org/about/staff/alexa-ura/) and [Edgar Walters](http://www.texastribune.org/about/staff/edgar-walters/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-plus-square</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>health-care</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1DDl1a9</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>During his long tenure, some of @GovernorPerry’s toughest battles have been over health care, women’s health </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>During his long tenure, some of Gov. Rick Perry’s toughest battles have been over health care — from Medicaid and the Affordable Care Act to women’s health and the HPV vaccine. </t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>perrylegacy-fb-share_health.png</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-101.JPG</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
     <t>Texans protest Gov. Rick Perry's decision not to expand Medicaid coverage to impoverished adults under the Affordable Care Act in September 2013.</t>
   </si>
   <si>
-    <t>img_4_url</t>
-  </si>
-  <si>
     <t>img_1_credit</t>
   </si>
   <si>
-    <t>Perry-Legacy-093.JPG</t>
-  </si>
-  <si>
     <t>Callie Richmond</t>
   </si>
   <si>
-    <t>img_4_caption</t>
-  </si>
-  <si>
     <t>img_2</t>
   </si>
   <si>
-    <t>Then-state Rep. Rick Perry listens to Rep. Robert Earley (D-Portland) during the 69th Legislature on May 13, 1985.</t>
-  </si>
-  <si>
     <t>Perry-Legacy-102.JPG</t>
-  </si>
-  <si>
-    <t>img_4_credit</t>
-  </si>
-  <si>
-    <t>Texas State Library &amp; Archives Commision</t>
   </si>
   <si>
     <t>img_2_caption</t>
@@ -672,27 +672,6 @@
   </si>
   <si>
     <t>text_3b</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Higher Education</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Heavy Hand in Academic Affairs </t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>That year, the Republican-led Legislature slashed the state’s budget for family planning by two-thirds — a move aimed at preventing health providers even loosely affiliated with abortion providers, namely Planned Parenthood, from receiving state tax dollars.
@@ -706,12 +685,6 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-graduation-cap</t>
-  </si>
-  <si>
     <t>text_4_header</t>
   </si>
   <si>
@@ -749,24 +722,6 @@
     <t>text_5</t>
   </si>
   <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>higher-education</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/12YF3Lq</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>From in-state tuition for undocumented students to the “Seven Solutions” — @GovernorPerry’s heavy hand in higher ed </t>
-  </si>
-  <si>
     <t>Perry was a leading proponent of the Cancer Prevention and Research Institute of Texas, a grant-making entity approved by voters in 2007 to spend $3 billion on cancer research, plus an additional $600 million appropriated by the Legislature for 2012-13. 
 The agency became mired in controversy in 2012 after an oversight committee [disclosed](http://www.texastribune.org/2013/01/28/state-audit-exposes-problems-cancer-institute/) that the agency had approved an $11 million grant to biotech company [Peloton Therapeutics](http://www.pelotontherapeutics.com/index.html) without scientific review.</t>
   </si>
@@ -774,19 +729,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
     <t>text_5b</t>
-  </si>
-  <si>
-    <t>From in-state tuition for undocumented students to the “Seven Breakthrough Solutions,” a look at Gov. Rick Perry’s heavy hand in higher ed</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>perrylegacy-fb-share_highered.png</t>
   </si>
   <si>
     <t>One of Peloton’s initial investors was Dallas philanthropist Peter O’Donnell, who has donated $241,000 to Perry’s campaigns since 2000, campaign finance records show. At the time, The Dallas Morning News reported that O’Donnell had also given $1.6 million to the CPRIT Foundation, a nonprofit. State law prohibits the CPRIT Foundation from accepting donations from CPRIT grant recipients. 
@@ -797,6 +740,63 @@
   </si>
   <si>
     <t>markdown</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Higher Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>A Heavy Hand in Academic Affairs </t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-graduation-cap</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>higher-education</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/12YF3Lq</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>From in-state tuition for undocumented students to the “Seven Solutions” — @GovernorPerry’s heavy hand in higher ed </t>
+  </si>
+  <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
+    <t>From in-state tuition for undocumented students to the “Seven Breakthrough Solutions,” a look at Gov. Rick Perry’s heavy hand in higher ed</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>perrylegacy-fb-share_highered.png</t>
   </si>
   <si>
     <t>img_1</t>
@@ -1372,7 +1372,7 @@
 “In Texas we have implemented common-sense policies that have enabled us to build a successful wind industry that can thrive on its own,” Nashed added. 
 But some environmentalists wonder if Perry’s fervor has waned, pointing to his failure to defend wind energy producers in their recent political battles.
 “Perry is bipolar on wind. He plugged into when he saw he could get a political benefit. And now that the winds have changed in the Republican Party, he’s unplugged himself from one of his greatest environmental victories,” said Tom “Smitty” Smith, director of the Texas office of Public Citizen. 
-Disclosure: The Texas Public Policy foundation is a corporate sponsor of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).
+*Disclosure: The Texas Public Policy foundation is a corporate sponsor of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).*
 </t>
   </si>
   <si>
@@ -2011,181 +2011,150 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>447</v>
+        <v>493</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>448</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>449</v>
+        <v>495</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>450</v>
+        <v>496</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>451</v>
+        <v>497</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>452</v>
+        <v>498</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>453</v>
+        <v>499</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>454</v>
+        <v>500</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>455</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>456</v>
+        <v>502</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>457</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>458</v>
+        <v>504</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>459</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>460</v>
+        <v>506</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>461</v>
+        <v>507</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>462</v>
-      </c>
-      <c t="s" s="4" r="B8">
-        <v>463</v>
+        <v>508</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>509</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>464</v>
-      </c>
-      <c t="s" s="4" r="B9">
-        <v>465</v>
+        <v>510</v>
+      </c>
+      <c t="s" s="7" r="B9">
+        <v>511</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>466</v>
+        <v>512</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>467</v>
+        <v>513</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>468</v>
+        <v>514</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>469</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>470</v>
+        <v>516</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>471</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>472</v>
+        <v>518</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>473</v>
+        <v>519</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>520</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>474</v>
+        <v>521</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>475</v>
+        <v>522</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>523</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>476</v>
+        <v>524</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>477</v>
+        <v>525</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>526</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>478</v>
+        <v>527</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>479</v>
+        <v>528</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>480</v>
+        <v>529</v>
       </c>
     </row>
     <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>481</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>482</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>484</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>485</v>
-      </c>
-      <c t="s" s="1" r="C18">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>487</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>488</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>490</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>491</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>492</v>
-      </c>
+      <c s="1" r="A17"/>
+      <c s="1" r="C17"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2204,150 +2173,181 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>493</v>
+        <v>447</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>494</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>495</v>
+        <v>449</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>496</v>
+        <v>450</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>497</v>
+        <v>451</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>498</v>
+        <v>452</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>499</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>500</v>
+        <v>454</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>501</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>502</v>
+        <v>456</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>503</v>
+        <v>457</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>504</v>
+        <v>458</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>505</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>506</v>
+        <v>460</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>507</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>508</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>509</v>
+        <v>462</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>463</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>510</v>
-      </c>
-      <c t="s" s="7" r="B9">
-        <v>511</v>
+        <v>464</v>
+      </c>
+      <c t="s" s="4" r="B9">
+        <v>465</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>512</v>
+        <v>466</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>513</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>514</v>
+        <v>468</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>515</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>516</v>
+        <v>470</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>517</v>
+        <v>471</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>518</v>
+        <v>472</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>519</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>520</v>
+        <v>473</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>521</v>
+        <v>474</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>522</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>523</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>524</v>
+        <v>476</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>525</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>526</v>
+        <v>477</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>527</v>
+        <v>478</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>528</v>
+        <v>479</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>529</v>
+        <v>480</v>
       </c>
     </row>
     <row r="17">
-      <c s="1" r="A17"/>
-      <c s="1" r="C17"/>
+      <c t="s" s="1" r="A17">
+        <v>481</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>482</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>484</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>485</v>
+      </c>
+      <c t="s" s="1" r="C18">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>487</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>488</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>490</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>491</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>492</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2364,322 +2364,370 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="125.0"/>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>97</v>
+        <v>6</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>98</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>99</v>
-      </c>
-      <c t="s" s="5" r="B2">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>113</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>116</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>117</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>119</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>120</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c s="1" r="B5"/>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>122</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>134</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>136</v>
-      </c>
-      <c t="s" s="4" r="B8">
-        <v>138</v>
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c t="s" s="4" r="B9">
-        <v>143</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>145</v>
+        <v>24</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>147</v>
-      </c>
-      <c s="1" r="C10"/>
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>26</v>
+      </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>149</v>
+        <v>27</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>152</v>
-      </c>
-      <c s="1" r="C11"/>
+        <v>32</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>33</v>
+      </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>154</v>
+        <v>35</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>156</v>
-      </c>
-      <c s="1" r="C12"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>160</v>
-      </c>
-      <c s="1" r="C13"/>
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>45</v>
+      </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>163</v>
+        <v>47</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>164</v>
-      </c>
-      <c s="1" r="C14"/>
+        <v>50</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>52</v>
+      </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>166</v>
-      </c>
-      <c s="1" r="C15"/>
+        <v>55</v>
+      </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>168</v>
-      </c>
-      <c s="1" r="C16"/>
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>63</v>
+      </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>169</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>170</v>
-      </c>
-      <c s="1" r="C17"/>
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>73</v>
+      </c>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>171</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>172</v>
-      </c>
-      <c s="1" r="C18"/>
+        <v>76</v>
+      </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>173</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>175</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>176</v>
-      </c>
-      <c s="1" r="B20"/>
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>86</v>
+      </c>
       <c t="s" s="1" r="C20">
-        <v>177</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>178</v>
+        <v>88</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>179</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>180</v>
-      </c>
-      <c t="s" s="5" r="B22">
-        <v>181</v>
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>91</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>182</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>183</v>
+        <v>93</v>
       </c>
       <c t="s" s="1" r="B23">
-        <v>184</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>185</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
-        <v>186</v>
+        <v>98</v>
       </c>
       <c t="s" s="1" r="B24">
-        <v>187</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>188</v>
+        <v>101</v>
       </c>
       <c t="s" s="1" r="B25">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>190</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>191</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="B26">
-        <v>192</v>
+        <v>105</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>106</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>193</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="B27">
-        <v>194</v>
-      </c>
-      <c t="s" s="1" r="C27">
-        <v>195</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>196</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B28">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>205</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>208</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="B29">
-        <v>209</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c s="1" r="C29"/>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>211</v>
-      </c>
-      <c t="s" s="1" r="C30">
-        <v>212</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c s="1" r="C30"/>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>213</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>214</v>
-      </c>
-      <c t="s" s="1" r="C31">
-        <v>215</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c s="1" r="C31"/>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>216</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>217</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>218</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>225</v>
-      </c>
-      <c t="s" s="1" r="C33">
-        <v>226</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="B34">
-        <v>232</v>
-      </c>
-      <c t="s" s="1" r="C34">
-        <v>233</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>124</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>126</v>
+      </c>
+      <c t="s" s="1" r="B36">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
+        <v>128</v>
+      </c>
+      <c t="s" s="1" r="B37">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>130</v>
+      </c>
+      <c t="s" s="1" r="B38">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>132</v>
+      </c>
+      <c t="s" s="1" r="B39">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>134</v>
+      </c>
+      <c t="s" s="1" r="B40">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2702,145 +2750,145 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c t="s" s="4" r="B9">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c t="s" s="3" r="B10">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2859,370 +2907,322 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="65.57"/>
+    <col min="2" customWidth="1" max="2" width="125.0"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>6</v>
+        <v>136</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>9</v>
+        <v>138</v>
+      </c>
+      <c t="s" s="5" r="B2">
+        <v>139</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>12</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>14</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>15</v>
-      </c>
-      <c s="1" r="B5"/>
+        <v>145</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>146</v>
+      </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>16</v>
+        <v>147</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>17</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>32</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>39</v>
+        <v>151</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>152</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c t="s" s="4" r="B9">
-        <v>42</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>46</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>47</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c s="1" r="C10"/>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="C11">
-        <v>55</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c s="1" r="C11"/>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>59</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c s="1" r="C12"/>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>61</v>
+        <v>161</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>64</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>65</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c s="1" r="C13"/>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>67</v>
+        <v>163</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>72</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c s="1" r="C14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>74</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c s="1" r="C15"/>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="C16">
-        <v>78</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c s="1" r="C16"/>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>80</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="B17">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>82</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c s="1" r="C17"/>
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>83</v>
+        <v>171</v>
       </c>
       <c t="s" s="1" r="B18">
-        <v>84</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c s="1" r="C18"/>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c t="s" s="1" r="B19">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>87</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>89</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c s="1" r="B20"/>
       <c t="s" s="1" r="C20">
-        <v>90</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>91</v>
+        <v>178</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>92</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>94</v>
+        <v>180</v>
+      </c>
+      <c t="s" s="5" r="B22">
+        <v>181</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>95</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>96</v>
+        <v>183</v>
       </c>
       <c t="s" s="1" r="B23">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>102</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c t="s" s="1" r="B24">
-        <v>104</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c t="s" s="1" r="B25">
-        <v>106</v>
+        <v>189</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>107</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>108</v>
+        <v>191</v>
       </c>
       <c t="s" s="1" r="B26">
-        <v>110</v>
-      </c>
-      <c t="s" s="1" r="C26">
-        <v>112</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>114</v>
+        <v>193</v>
       </c>
       <c t="s" s="1" r="B27">
-        <v>115</v>
+        <v>194</v>
+      </c>
+      <c t="s" s="1" r="C27">
+        <v>195</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>118</v>
+        <v>196</v>
       </c>
       <c t="s" s="1" r="B28">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>124</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c t="s" s="1" r="B29">
-        <v>126</v>
-      </c>
-      <c s="1" r="C29"/>
+        <v>200</v>
+      </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>128</v>
-      </c>
-      <c s="1" r="C30"/>
+        <v>202</v>
+      </c>
+      <c t="s" s="1" r="C30">
+        <v>203</v>
+      </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>129</v>
+        <v>204</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>130</v>
-      </c>
-      <c s="1" r="C31"/>
+        <v>205</v>
+      </c>
+      <c t="s" s="1" r="C31">
+        <v>206</v>
+      </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>133</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>137</v>
+        <v>210</v>
+      </c>
+      <c t="s" s="1" r="C33">
+        <v>211</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>139</v>
+        <v>212</v>
       </c>
       <c t="s" s="1" r="B34">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>142</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>146</v>
-      </c>
-      <c t="s" s="1" r="B36">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37">
-      <c t="s" s="1" r="A37">
-        <v>150</v>
-      </c>
-      <c t="s" s="1" r="B37">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>153</v>
-      </c>
-      <c t="s" s="1" r="B38">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39">
-      <c t="s" s="1" r="A39">
-        <v>157</v>
-      </c>
-      <c t="s" s="1" r="B39">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
-        <v>161</v>
-      </c>
-      <c t="s" s="1" r="B40">
-        <v>162</v>
+        <v>213</v>
+      </c>
+      <c t="s" s="1" r="C34">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3242,77 +3242,77 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>198</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>200</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>203</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c t="s" s="6" r="B4">
-        <v>207</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c t="s" s="4" r="B8">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c t="s" s="7" r="B9">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
change shareline links in macro
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -50,52 +50,115 @@
     <t>headline</t>
   </si>
   <si>
-    <t>Five — And a Half — Things We Won't Forget About Texas' Longest-Serving Governor</t>
+    <t>Five — and a Half — Things We Won't Forget About Texas' Longest-Serving Governor</t>
+  </si>
+  <si>
+    <t>topic</t>
   </si>
   <si>
     <t>byline</t>
   </si>
   <si>
+    <t>Transportation</t>
+  </si>
+  <si>
     <t>[Reeve Hamilton](http://www.texastribune.org/about/staff/reeve-hamilton) and [Jay Root](http://www.texastribune.org/about/staff/jay-root)</t>
   </si>
   <si>
     <t>markdown</t>
   </si>
   <si>
+    <t>headline</t>
+  </si>
+  <si>
     <t>icon</t>
   </si>
   <si>
+    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
+  </si>
+  <si>
     <t>fa-star</t>
   </si>
   <si>
     <t>slug</t>
   </si>
   <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>share_url</t>
   </si>
   <si>
+    <t>icon</t>
+  </si>
+  <si>
     <t>trib.it/perry-legacy</t>
   </si>
   <si>
+    <t>fa-car</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>share_url</t>
+  </si>
+  <si>
+    <t>trib.it/1IVfJqr</t>
+  </si>
+  <si>
     <t>tweet_text</t>
   </si>
   <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
     <t>The six things Texans won’t forget about @GovernorPerry: </t>
   </si>
   <si>
+    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
+  </si>
+  <si>
     <t>facebook_text</t>
   </si>
   <si>
+    <t>facebook_text</t>
+  </si>
+  <si>
     <t>Here are the six things Texans won't forget about Rick Perry, the state's longest-serving governor: </t>
   </si>
   <si>
+    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
+  </si>
+  <si>
     <t>facebook_art</t>
   </si>
   <si>
     <t>perrylegacy-fb-share_home.png</t>
   </si>
   <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>perrylegacy-fb-share_transpo.png</t>
+  </si>
+  <si>
     <t>text_intro</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
   </si>
   <si>
     <t>When Gov. Rick Perry leaves office next month, he’ll wrap up a three-decade stretch in state elective office that concluded with his being the longest-serving governor in Texas history. 
@@ -109,16 +172,16 @@
     <t>text_introb</t>
   </si>
   <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Transportation</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>A Toll Road Plan &amp;ldquo;as Big as Texas&amp;rdquo;</t>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Bob Daemmrich</t>
   </si>
   <si>
     <t>From his first legislative session as governor in 2001, when Perry shocked the political establishment with a record 82 vetoes, to his final days in office, when he used [rare emergency powers](http://www.texastribune.org/2014/08/05/lawmakers-question-perrys-funding-guard-border/) to send National Guard troops to the state’s border with Mexico, the ruggedly handsome farm boy from West Texas signaled early and often that he would cut a unique and flashy trail through the state’s political countryside.
@@ -131,7 +194,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>byline</t>
+    <t>text_1</t>
   </si>
   <si>
     <t>text_1_header</t>
@@ -140,25 +203,18 @@
     <t>1. Longevity</t>
   </si>
   <si>
-    <t>[Aman Batheja](http://www.texastribune.org/about/staff/aman-batheja/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>text_1</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-car</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>transportation</t>
+    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
+"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
+The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_2</t>
   </si>
   <si>
     <t>When Perry hands over power to Gov.-elect Greg Abbott on Jan. 20, he will have served 5,144 days in office, making the previous records seem puny and insignificant. Gov. Allan Shivers, who took over after Gov. Beauford Jester died in 1949, previously held the distinction as the longest continuously serving governor with a mere seven-and-a-half years in office, back when the terms lasted only two years.
@@ -168,16 +224,16 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>share_url</t>
-  </si>
-  <si>
     <t>text_1b</t>
   </si>
   <si>
-    <t>trib.it/1IVfJqr</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
+    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
   </si>
   <si>
     <t>Perry, who had been elected lieutenant governor when Bush won his second term, was sworn into office as the 47th Texas governor on Dec. 21, 2000, and he went on to win three consecutive four-year terms. He has used the longevity to wield power with an increasingly tight fist. 
@@ -187,13 +243,7 @@
 “I think Perry really learned how to use the office,” he said. (U.T.-Austin is a corporate sponsor of The Texas Tribune.)</t>
   </si>
   <si>
-    <t>.@GovernorPerry’s Trans-Texas Corridor never materialized, but he still left his mark on Texas’ road-funding approach </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
+    <t>markdown</t>
   </si>
   <si>
     <t>text_2_header</t>
@@ -202,22 +252,19 @@
     <t>2. The Texas Miracle</t>
   </si>
   <si>
-    <t>Gov. Rick Perry's Trans-Texas Corridor never materialized, but he still left his mark on the state's approach to funding roads. trib.it/1IVfJqr</t>
+    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
+And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
+Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
+Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
   </si>
   <si>
     <t>text_2</t>
   </si>
   <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>perrylegacy-fb-share_transpo.png</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>http://s3.amazonaws.com/static.texastribune.org/media/images/SH130-4.jpg</t>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4</t>
   </si>
   <si>
     <t>The most appropriate use of the word “miracle” in relation to Texas is in the eyes of the beholder.
@@ -230,24 +277,13 @@
     <t>text_2b</t>
   </si>
   <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry at the opening ceremony for the southern portion of the SH130 toll road from Georgetown to Seguin.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Bob Daemmrich</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>Rick Perry was just a year into his tenure as governor when he proposed the Trans-Texas Corridor, a massive 4,000-mile network of privately operated toll roads, railroad tracks and utility lines that would take 50 years to build.  
-"This plan is as big as Texas and as ambitious as our people," Perry said at the first of many events touting the project. 
-The corridor he envisioned would never become a reality, but he still managed to leave his mark on the state’s approach to funding roads. Under his leadership, Texas has been the country’s most aggressive supporter of tolling and private-sector investment in transportation. </t>
+    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
+Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
+As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
+Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
+  </si>
+  <si>
+    <t>markdown</t>
   </si>
   <si>
     <t>But any governor in America would be happy to boast, as Perry has, about the kind of economic expansion Texas has experienced in the last decade or so.
@@ -261,12 +297,6 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_2</t>
-  </si>
-  <si>
     <t>text_3_header</t>
   </si>
   <si>
@@ -277,15 +307,6 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>Despite millions of dollars spent on planning, the caustic public response to the Trans-Texas Corridor would ultimately doom it. Activists [decried the project](http://www.texastribune.org/2012/11/30/tolling-texans-toll-projects-spread-state-funds-la/) as a boondoggle, an infringement on property rights, a textbook example of crony capitalism and a pathway to a Texas in which avoiding tolls on everyday trips would become impossible. Eventually, opposition to the Trans-Texas Corridor became the default position for political candidates across the state, regardless of party affiliation. </t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3</t>
-  </si>
-  <si>
     <t>Texas was in trouble in 2005 when the state Supreme Court declared the state’s school finance system unconstitutional. The chief concern was that too many districts were charging the maximum rate for local property taxes, prompting the high court to declare that Texas had effectively adopted a prohibited statewide property tax.
 At the same time, the state’s loophole-ridden business tax had become all but voluntary. It applied only to corporations and limited liability companies, so many reformulated as non-taxable limited partnerships to avoid paying it.</t>
   </si>
@@ -294,15 +315,6 @@
   </si>
   <si>
     <t>text_3b</t>
-  </si>
-  <si>
-    <t>Perry tried for years to salvage the project (he repeatedly warned that Texas’ only transportation options were “toll roads, slow roads or no roads”) but eventually gave up the fight. In 2011, he signed a bill expunging the last references to the Trans-Texas Corridor in state law.
-And yet, Perry’s vision of toll roads blossoming across Texas didn’t exactly fade away. His early push for the Trans-Texas Corridor jump-started a building boom of highways paid for by future toll revenue, often with private-sector investment playing a role. Texas now has more than 500 miles of tolled highways, most of them constructed over the last decade.
-Overall, Texas added more than 6,600 new highway miles between 2001 and 2012, including those with and without tolls. While that’s more than any other state, it’s [among the lowest in the country](http://www.politifact.com/texas/statements/2014/jan/28/rick-perry/texas-change-highway-miles-not-no-1-adjusted-size/) when adjusted for Texas’ fast-growing population.
-Texans have paid the same gas tax — 38.4 cents per gallon — since 1993, and at both the state and at the federal level, there has been little political interest in raising it. </t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>The [solution](http://governor.state.tx.us/news/press-release/2429/) Perry advocated: Craft a business tax that applies to most companies regardless of structure, raise the cigarette tax by a $1 a pack and use all that money to reduce property taxes while giving teachers a $2,000 pay raise.
@@ -332,9 +344,6 @@
   </si>
   <si>
     <t>text_4b</t>
-  </si>
-  <si>
-    <t>text_4</t>
   </si>
   <si>
     <t>For 53 cringe-inducing seconds during a nationally televised Republican primary debate on Nov. 9, 2011, Perry desperately searched his frozen brain for the name of the third federal department he wanted to shut down if elected president.
@@ -349,16 +358,7 @@
     <t>markdown</t>
   </si>
   <si>
-    <t>“That’s why we embraced visionary approaches to finance road construction,” Perry said in a speech in January. “Pay-as-you-go just didn’t pour enough asphalt and concrete to meet our growing needs.” 
-Since 2003, Texas has helped close the gap between its transportation needs and available funds by borrowing billions of dollars and outsourcing more of its road work to the private sector.
-As Perry’s tenure comes to a close, the Texas Department of Transportation finds itself with an annual funding shortfall of $5 billion. An oil-drilling boom in South and West Texas is helping relieve some of that while also creating new challenges, including crumbling rural roads and a [spike in vehicle crashes](http://apps.texastribune.org/shale-life/deadly-roads/). 
-Across the state, worsening traffic is [creating concerns](http://www.texastribune.org/2014/07/09/traffic-forecasts-worsen-fears-miracle-slowing/) that the state’s strong economic performance in recent years could eventually falter as businesses find the state’s road network unmanageable. In the Capitol, both Republicans and Democrats are showing [signs of tolling fatigue](http://www.texastribune.org/2014/07/04/perry-exits-texas-gop-shifting-away-toll-roads/) and expressing interest in approaching the issue in different ways in a post-Perry era.</t>
-  </si>
-  <si>
     <t>text_5_header</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>5. The Indictment</t>
@@ -799,21 +799,60 @@
     <t>perrylegacy-fb-share_highered.png</t>
   </si>
   <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Public Education</t>
+  </si>
+  <si>
+    <t>headline</t>
+  </si>
+  <si>
+    <t>Guarding State Control of Public Schools — With Money on the Line</t>
+  </si>
+  <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
+  </si>
+  <si>
     <t>img_1</t>
   </si>
   <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>Perry-Legacy-092.JPG</t>
   </si>
   <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>fa-book</t>
+  </si>
+  <si>
     <t>img_1_caption</t>
   </si>
   <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>public-education</t>
+  </si>
+  <si>
     <t>Gov. Rick Perry celebrated with state and local leaders at the ceremonial signing of a merger bill between UT-Pan American and UT-Brownsville in 2013. </t>
   </si>
   <si>
+    <t>share_url</t>
+  </si>
+  <si>
     <t>img_1_credit</t>
   </si>
   <si>
+    <t>trib.it/1qTCoh3</t>
+  </si>
+  <si>
     <t>Bob Daemmrich</t>
   </si>
   <si>
@@ -836,6 +875,15 @@
   </si>
   <si>
     <t>text_intro</t>
+  </si>
+  <si>
+    <t>tweet_text</t>
+  </si>
+  <si>
+    <t>#Perry’s approach to public ed has been to guard state control over classrooms — even when there’s money on the line</t>
+  </si>
+  <si>
+    <t>facebook_text</t>
   </si>
   <si>
     <t>As Gov. Rick Perry himself has said — and as his critics are fond of pointing out — he [did not demonstrate significant interest](http://www.texastribune.org/2011/08/02/perry-aggie-years/) in academia while an undergraduate student at Texas A&amp;M University.
@@ -847,7 +895,37 @@
     <t>markdown</t>
   </si>
   <si>
+    <t>Gov. Rick Perry's approach to public education has been to guard state control over classrooms — even when there’s federal money on the line trib.it/1qTCoh3</t>
+  </si>
+  <si>
     <t>text_introb</t>
+  </si>
+  <si>
+    <t>facebook_art</t>
+  </si>
+  <si>
+    <t>perrylegacy-fb-share_publiced.png</t>
+  </si>
+  <si>
+    <t>img_1</t>
+  </si>
+  <si>
+    <t>Perry-Legacy-022.JPG</t>
+  </si>
+  <si>
+    <t>img_1_caption</t>
+  </si>
+  <si>
+    <t>Gov. Rick Perry speaks at the Texas State Board of Education meeting in February 2013.</t>
+  </si>
+  <si>
+    <t>img_1_credit</t>
+  </si>
+  <si>
+    <t>Marjorie Kamys Cotera</t>
+  </si>
+  <si>
+    <t>text_1</t>
   </si>
   <si>
     <t>And over the course of his decade-and-a-half as governor, he has certainly had influence on the state’s colleges and universities, but he has at times pushed and pulled in contradictory directions.
@@ -867,10 +945,20 @@
     <t>text_1</t>
   </si>
   <si>
+    <t>When Gov. Rick Perry took power 14 years ago, the Texas public education system had just become a laboratory for federal policy. 
+A Texas governor had won the White House on a promise to spread what he called the “Texas miracle” — the package of reforms credited with boosting performance in the state’s public schools. Those policies inspired the George W. Bush administration’s signature No Child Left Behind Act, which greatly expanded federal regulation of public education.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>But it was on Perry’s watch in 2003 that the state’s approach to higher education tuition fundamentally changed. 
 That year, the ability to set tuition at the state’s public universities was transferred from the Legislature to the schools’ respective governing boards — the members of which have all been appointed by the governor. Since tuition was deregulated, average tuition and fees statewide has more than doubled.</t>
   </si>
   <si>
+    <t>text_2</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
@@ -891,6 +979,20 @@
   </si>
   <si>
     <t>text_2</t>
+  </si>
+  <si>
+    <t>Less than a decade later, as Perry geared up for his own presidential bid, he would propose something radically different: dismantling the U.S. Department of Education and vastly diminishing the role of the federal government in public schools. He would call No Child Left Behind a [“monstrous intrusion into our affairs.”](http://www.nationalreview.com/articles/265309/rick-perry-s-tenth-commandment-kevin-d-williamson/page/0/3)
+Guarding Texas control of public school classrooms has been the most prominent feature of Perry’s approach to education. But as he leaves office, his impact will also be felt in state-level matters, where his involvement has tended to be less public.
+The high-profile battles with Washington began in the summer of 2009, when Texas declined to sign on to a nationwide effort to develop common academic standards in reading and math. Known as Common Core, it had the support of both Republican and Democratic policymakers. Only Alaska joined Texas in refusing to participate.
+Though it drew little attention at the time, the move was the first sign of the political firestorm that would ignite over the initiative. Four years later, concern over a potential federal takeover of education has driven at least four states to drop them from their public schools, with numerous others facing pressure to do the same. 
+A few months later, a decision not to apply for the Obama administration’s Race to the Top competition — which meant losing out on $700 million in federal funding — once again made Texas an outlier. The program, which initially set aside $4.35 billion in grants for states that agreed to put certain reforms in place, had until then largely enjoyed bipartisan praise.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_3</t>
   </si>
   <si>
     <t>In 2009, he [signed legislation](http://www.capitol.state.tx.us/BillLookup/History.aspx?LegSess=81R&amp;Bill=HB51) that dedicated millions to incentivizing research activities at public universities that aspire to “tier one” status. He was, at the time, pushing policies he had unveiled the year before that set academic researchers on edge.
@@ -907,154 +1009,6 @@
   </si>
   <si>
     <t>UT-Austin Tensions</t>
-  </si>
-  <si>
-    <t>text_3</t>
-  </si>
-  <si>
-    <t>In 2011, a group of the University of Texas at Austin’s well-heeled and influential alumni pushed back when they feared the reforms were about to be pushed on their university. The controversy has yet to die down, even though the proposals were never put into practice.
-</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_3b</t>
-  </si>
-  <si>
-    <t>The tensions at UT-Austin have largely morphed from policy disagreements to personality conflicts. One of the system’s regents, who — like all the others — was appointed by Perry, was [censured](http://www.texastribune.org/2014/08/11/transparency-committee-exploring-multiple-options/) by lawmakers this year after a yearlong investigation into his antagonism toward the flagship university. The UT System’s [chancellor](http://www.texastribune.org/2014/02/09/report-cigarroa-step-down-ut-chancellor/) and UT-Austin’s [president](http://www.texastribune.org/2014/07/09/cigarroa-powers-resignation-effective-june-2/) have both announced plans to step down.
-Perry encouraged the conflict, comparing the fight to the Battle of the Bulge in an email to some of the regents.
-While the UT community has been mired in controversy, Perry helped the A&amp;M community build itself up into a force to be reckoned with. He has steered large state grants to his alma mater to establish a nascent biotech corridor in Bryan-College Station, and he encouraged the school’s successful move to the Southeastern Conference.</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4_header</t>
-  </si>
-  <si>
-    <t>In-State Tuition</t>
-  </si>
-  <si>
-    <t>text_4</t>
-  </si>
-  <si>
-    <t>The issue that Perry has perhaps been most consistent on could also prove to have been the most politically damaging to him.
-In 2001, he signed a bill ensuring that the children of undocumented immigrants could pay in-state tuition prices at public colleges and universities. He has stood by that decision, even in the face of strong opposition from his own party.
-</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_4b</t>
-  </si>
-  <si>
-    <t>When the issue came up in a nationally televised debate during the Republican presidential primary in 2011, Perry [said](http://www.texastribune.org/2011/09/22/liveblog-fox-newsgoogle-republican-debate/) of those who questioned the policy, “I don’t think you have a heart.” His [poll numbers](http://www.texastribune.org/library/data/rise-and-fall-of-rick-perry-presidential-campaign/) nose-dived and never recovered. Though he expressed regret for the language he used in its defense, he has not backed down on his support for what’s called the Texas DREAM Act.
-Whether the policy remains a memorable part of his legacy will largely depend on whether it survives the coming legislative session. With Perry gone, its continuation is in doubt.
-*Disclosure: Texas A&amp;M University and the University of Texas at Austin are corporate sponsors of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).*</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>Public Education</t>
-  </si>
-  <si>
-    <t>headline</t>
-  </si>
-  <si>
-    <t>Guarding State Control of Public Schools — With Money on the Line</t>
-  </si>
-  <si>
-    <t>byline</t>
-  </si>
-  <si>
-    <t>[Morgan Smith](http://www.texastribune.org/about/staff/morgan-smith/)</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>fa-book</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>public-education</t>
-  </si>
-  <si>
-    <t>share_url</t>
-  </si>
-  <si>
-    <t>trib.it/1qTCoh3</t>
-  </si>
-  <si>
-    <t>tweet_text</t>
-  </si>
-  <si>
-    <t>#Perry’s approach to public ed has been to guard state control over classrooms — even when there’s money on the line</t>
-  </si>
-  <si>
-    <t>facebook_text</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry's approach to public education has been to guard state control over classrooms — even when there’s federal money on the line trib.it/1qTCoh3</t>
-  </si>
-  <si>
-    <t>facebook_art</t>
-  </si>
-  <si>
-    <t>perrylegacy-fb-share_publiced.png</t>
-  </si>
-  <si>
-    <t>img_1</t>
-  </si>
-  <si>
-    <t>Perry-Legacy-022.JPG</t>
-  </si>
-  <si>
-    <t>img_1_caption</t>
-  </si>
-  <si>
-    <t>Gov. Rick Perry speaks at the Texas State Board of Education meeting in February 2013.</t>
-  </si>
-  <si>
-    <t>img_1_credit</t>
-  </si>
-  <si>
-    <t>Marjorie Kamys Cotera</t>
-  </si>
-  <si>
-    <t>text_1</t>
-  </si>
-  <si>
-    <t>When Gov. Rick Perry took power 14 years ago, the Texas public education system had just become a laboratory for federal policy. 
-A Texas governor had won the White House on a promise to spread what he called the “Texas miracle” — the package of reforms credited with boosting performance in the state’s public schools. Those policies inspired the George W. Bush administration’s signature No Child Left Behind Act, which greatly expanded federal regulation of public education.</t>
-  </si>
-  <si>
-    <t>markdown</t>
-  </si>
-  <si>
-    <t>text_2</t>
-  </si>
-  <si>
-    <t>Less than a decade later, as Perry geared up for his own presidential bid, he would propose something radically different: dismantling the U.S. Department of Education and vastly diminishing the role of the federal government in public schools. He would call No Child Left Behind a [“monstrous intrusion into our affairs.”](http://www.nationalreview.com/articles/265309/rick-perry-s-tenth-commandment-kevin-d-williamson/page/0/3)
-Guarding Texas control of public school classrooms has been the most prominent feature of Perry’s approach to education. But as he leaves office, his impact will also be felt in state-level matters, where his involvement has tended to be less public.
-The high-profile battles with Washington began in the summer of 2009, when Texas declined to sign on to a nationwide effort to develop common academic standards in reading and math. Known as Common Core, it had the support of both Republican and Democratic policymakers. Only Alaska joined Texas in refusing to participate.
-Though it drew little attention at the time, the move was the first sign of the political firestorm that would ignite over the initiative. Four years later, concern over a potential federal takeover of education has driven at least four states to drop them from their public schools, with numerous others facing pressure to do the same. 
-A few months later, a decision not to apply not to apply for the Obama administration’s Race to the Top competition — which meant losing out on $700 million in federal funding — once again made Texas an outlier. The program, which initially set aside $4.35 billion in grants for states that agreed to put certain reforms in place, had until then largely enjoyed bipartisan praise.
-</t>
-  </si>
-  <si>
-    <t>markdown</t>
   </si>
   <si>
     <t>text_3</t>
@@ -1069,10 +1023,20 @@
 </t>
   </si>
   <si>
+    <t>In 2011, a group of the University of Texas at Austin’s well-heeled and influential alumni pushed back when they feared the reforms were about to be pushed on their university. The controversy has yet to die down, even though the proposals were never put into practice.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
     <t>text_4</t>
+  </si>
+  <si>
+    <t>text_3b</t>
   </si>
   <si>
     <t>Legislators ultimately enacted a historic reduction in funding for public schools: $4 billion in state dollars and almost $1.4 billion in discretionary grants that supported programs including remedial intervention and after-school care.
@@ -1084,6 +1048,42 @@
 </t>
   </si>
   <si>
+    <t>The tensions at UT-Austin have largely morphed from policy disagreements to personality conflicts. One of the system’s regents, who — like all the others — was appointed by Perry, was [censured](http://www.texastribune.org/2014/08/11/transparency-committee-exploring-multiple-options/) by lawmakers this year after a yearlong investigation into his antagonism toward the flagship university. The UT System’s [chancellor](http://www.texastribune.org/2014/02/09/report-cigarroa-step-down-ut-chancellor/) and UT-Austin’s [president](http://www.texastribune.org/2014/07/09/cigarroa-powers-resignation-effective-june-2/) have both announced plans to step down.
+Perry encouraged the conflict, comparing the fight to the Battle of the Bulge in an email to some of the regents.
+While the UT community has been mired in controversy, Perry helped the A&amp;M community build itself up into a force to be reckoned with. He has steered large state grants to his alma mater to establish a nascent biotech corridor in Bryan-College Station, and he encouraged the school’s successful move to the Southeastern Conference.</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4_header</t>
+  </si>
+  <si>
+    <t>In-State Tuition</t>
+  </si>
+  <si>
+    <t>text_4</t>
+  </si>
+  <si>
+    <t>The issue that Perry has perhaps been most consistent on could also prove to have been the most politically damaging to him.
+In 2001, he signed a bill ensuring that the children of undocumented immigrants could pay in-state tuition prices at public colleges and universities. He has stood by that decision, even in the face of strong opposition from his own party.
+</t>
+  </si>
+  <si>
+    <t>markdown</t>
+  </si>
+  <si>
+    <t>text_4b</t>
+  </si>
+  <si>
+    <t>When the issue came up in a nationally televised debate during the Republican presidential primary in 2011, Perry [said](http://www.texastribune.org/2011/09/22/liveblog-fox-newsgoogle-republican-debate/) of those who questioned the policy, “I don’t think you have a heart.” His [poll numbers](http://www.texastribune.org/library/data/rise-and-fall-of-rick-perry-presidential-campaign/) nose-dived and never recovered. Though he expressed regret for the language he used in its defense, he has not backed down on his support for what’s called the Texas DREAM Act.
+Whether the policy remains a memorable part of his legacy will largely depend on whether it survives the coming legislative session. With Perry gone, its continuation is in doubt.
+*Disclosure: Texas A&amp;M University and the University of Texas at Austin are corporate sponsors of The Texas Tribune. A complete list of Tribune donors and sponsors can be viewed [here](http://www.texastribune.org/support-us/donors-and-members/).*</t>
+  </si>
+  <si>
     <t>markdown</t>
   </si>
   <si>
@@ -1198,7 +1198,7 @@
     <t>Perry’s fans say he deserves credit for his business-friendly approach that got results by focusing on Texas-flavored solutions over onerous federal regulations. 
 Not so, say environmental advocates. Texans breathe better in spite of a governor who fought the very federal regulations primarily responsible for improving the air, they say.
 “Texas has focused on implementing smart regulations that have helped clean our air while allowing us to grow one of the most dynamic economies in the nation and achieve significant population growth,” Perry spokeswoman Lucy Nashed wrote in an email. 
-Under a landmark initiative started in 2001 called the [Texas Emissions Reduction Plan (TERP)](http://www.tceq.state.tx.us/assets/public/comm_exec/pubs/sfr/079-14.pdf), the state has doled out more than $905 million in incentives to replace or upgrade older engines and equipment. 
+Under a landmark initiative started in 2001 called the [Texas Emissions Reduction Plan (TERP)](http://www.tceq.state.tx.us/assets/public/comm_exec/pubs/sfr/079-14.pdf), the state has doled out more than $905 million in incentives to replace or upgrade older engines and equipment. In recent years, however, [hundreds of millions of dollars](http://www.lbb.state.tx.us/Documents/Publications/Issue_Briefs/527_TERP.pdf) meant for TERP have instead been used to balance the state’s budget. 
 Nashed also noted a dramatic expansion of wind power and new [energy efficiency](http://governor.state.tx.us/initiatives/energy/) and [renewable energy](http://governor.state.tx.us/files/ecodev/renewable_energy.pdf) targets, along with laws encouraging more nuclear plants and “clean coal” technology.
 But Tom “Smitty” Smith, an environmental advocate and director of the advocacy group Public Citizen, said much of the credit for those initiatives goes to former Gov. George W. Bush. Smith said it was Bush who [signed into law](http://www.legis.state.tx.us/tlodocs/76R/analysis/html/SB00007F.htm) some of the state’s first renewable energy goals, along with cracking down on pollution from old power plants. 
 </t>
@@ -1210,10 +1210,9 @@
     <t>text_3</t>
   </si>
   <si>
-    <t>Also, Smith said, [hundreds of millions of dollars](http://www.lbb.state.tx.us/Documents/Publications/Issue_Briefs/527_TERP.pdf) meant for TERP have instead been used to balance the state’s budget in recent years. 
-“He has the worst environmental record that I’ve seen in the 30 years that I’ve been working on this issue,” Smith said, arguing that federal environmental rules  — which Perry opposed — are largely responsible for cleaning up Texas’ air. 
+    <t>“He has the worst environmental record that I’ve seen in the 30 years that I’ve been working on this issue,” Smith said, arguing that federal environmental rules  — which Perry opposed — are largely responsible for cleaning up Texas’ air. 
 Federal mileage and emission standards have improved air quality across the country, not just in Texas, said Elena Craft, a health scientist and air pollution expert with the Environmental Defense Fund. “I can’t think of something that Perry himself has promoted,” she said. (Texas officials point out that average ozone [reductions](https://www.tceq.texas.gov/airquality/airsuccess/air-success-criteria) in Texas have been better than other states, or the country as a whole.)
-Smith and Craft also pointed to Perry’s opposition to nearly every federal attempt to reduce air pollution. During Perry’s tenure, Texas has sued the Environmental Protection Agency more than a dozen times, for the most part unsuccessfully. 
+Smith and Craft also noted Perry’s opposition to nearly every federal attempt to reduce air pollution. During Perry’s tenure, Texas has sued the Environmental Protection Agency more than a dozen times, for the most part unsuccessfully. 
 The U.S. Supreme Court [struck down](http://www.texastribune.org/2014/04/29/texas-loses-fight-against-epa-air-pollution-rule/) Texas’ challenges to a federal rule governing interstate pollution and largely [dismissed](http://www.texastribune.org/2014/06/23/latest-epa-supreme-court-ruling-largely-loss-texas/) objections to climate change regulations. A federal appeals court also [ruled against](http://www.cadc.uscourts.gov/internet/opinions.nsf/284AC47088C07D0985257CBB004F0795/%24file/12-1100-1488346.pdf) Texas’ lawsuit over a federal rule on mercury and toxic emissions limits from coal plants, and the Supreme Court has [said](http://www.nytimes.com/2014/11/26/us/politics/supreme-court-to-hear-case-on-costs-of-clean-air-act.html) it will take up the case.
 </t>
   </si>
@@ -1226,10 +1225,10 @@
   <si>
     <t>Texas did win a challenge to the EPA’s rejection of one air permitting program [in 2012](https://www.texasattorneygeneral.gov/oagnews/release.php?id=4111), although many companies had [already](http://www.texastribune.org/2011/01/13/texas-companies-navigate-environmental-agencies-di/) transitioned away from it before the [decision](https://www.texasattorneygeneral.gov/newspubs/releases/2012/081312flex_permits_opinion.pdf). 
 Even the unsuccessful lawsuits weren’t a total loss, because they asserted Texas’ independence and at times forced the EPA to revise its rules, said Josiah Neeley, Texas director of the R Street Institute, a conservative think tank. 
-Kathleen Hartnett White, whom Perry appointed to the Texas Commission on Environmental Quality in 2001, called Perry’s leadership “a win for the environment and a win for the economy.”
-For instance, she noted, when the EPA clumsily suggested that Texas cap emissions of dozens of different volatile organic compounds that [help create](http://www.epa.gov/groundlevelozone/) ozone, Perry promoted flexibility for Houston industries. The state instead focused on a few of the worst offenders. 
-During Perry’s second term, the state launched a market-based cap-and-trade program for just those pollutants for Houston-area polluters. But the other part of Houston’s ozone success — a similar market-based cap-and-trade program for nitrogen oxide emissions, which also create smog — was developed before he took office. 
-Plus, all those efforts to reduce ozone were a result of the federal government lowering the ozone standard in 1997. So are the feds or the state responsible for ozone improvements? “I think it’s a mix of both,” said White, now with the conservative Texas Public Policy Foundation.
+Kathleen Hartnett White, whom Perry appointed to the Texas Commission on Environmental Quality from 2001 to 2007, called Perry’s leadership “a win for the environment and a win for the economy.”
+For instance, she noted, when the EPA clumsily suggested that Texas cap emissions of dozens of different volatile organic compounds that [help create](http://www.epa.gov/groundlevelozone/) ozone, Perry promoted flexibility for Houston industries. The state instead focused on a few of the worst offenders and created a market-based cap-and-trade program just for those among Houston-area polluters.
+Many also attribute reductions in Houston’s smog to a drastic decrease in emissions of nitrogen oxide — achieved in part by a similar cap-and-trade program for that pollutant, which was developed before Perry took office. 
+Plus, those efforts to reduce such pollution were largely in response to the federal government lowering the ozone standard in 1997. So are the feds or the state responsible for ozone improvements? “I think it’s a mix of both,” said White, now with the conservative Texas Public Policy Foundation.
 </t>
   </si>
   <si>
@@ -1682,7 +1681,7 @@
     <t>text_5</t>
   </si>
   <si>
-    <t>By 2011, the number of prisoners had fallen enough that the first prison in Texas history was shuttered. A state jail and pre-parole later also closed.  
+    <t>By 2011, the number of prisoners had fallen enough that the first prison in Texas history was shuttered. A state jail and pre-parole facility later also closed.  
 TDCJ Executive Director Brad Livingston credits Perry's support for those reforms, even during fiscally leaner years.
 In 2011, when Perry and lawmakers faced "fiscal challenges," the governor stuck by TDCJ and the state’s investment in substance abuse treatment beds, Livingston said. 
 "Gov. Perry and his administration have been certainly pivotal in all of this," Livingston said.
@@ -2364,377 +2363,158 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="65.57"/>
+    <col min="2" customWidth="1" max="2" width="59.71"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>14</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>15</v>
-      </c>
-      <c s="1" r="B5"/>
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>28</v>
+      </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c t="s" s="4" r="B9">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>24</v>
-      </c>
-      <c t="s" s="1" r="B10">
-        <v>25</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>26</v>
+        <v>44</v>
+      </c>
+      <c t="s" s="3" r="B10">
+        <v>45</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="C11">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>52</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>74</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>64</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>75</v>
-      </c>
-      <c t="s" s="1" r="B18">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>83</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>86</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="C22">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="C23">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>98</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>101</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>104</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>105</v>
-      </c>
-      <c t="s" s="1" r="C26">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>107</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>109</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>110</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>112</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>113</v>
-      </c>
-      <c s="1" r="C29"/>
-    </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
-        <v>114</v>
-      </c>
-      <c t="s" s="1" r="B30">
-        <v>115</v>
-      </c>
-      <c s="1" r="C30"/>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>116</v>
-      </c>
-      <c t="s" s="1" r="B31">
-        <v>117</v>
-      </c>
-      <c s="1" r="C31"/>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>118</v>
-      </c>
-      <c t="s" s="1" r="B32">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
-        <v>120</v>
-      </c>
-      <c t="s" s="1" r="B33">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
-        <v>122</v>
-      </c>
-      <c t="s" s="1" r="B34">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
-        <v>124</v>
-      </c>
-      <c t="s" s="1" r="B35">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>126</v>
-      </c>
-      <c t="s" s="1" r="B36">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37">
-      <c t="s" s="1" r="A37">
-        <v>128</v>
-      </c>
-      <c t="s" s="1" r="B37">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>130</v>
-      </c>
-      <c t="s" s="1" r="B38">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39">
-      <c t="s" s="1" r="A39">
-        <v>132</v>
-      </c>
-      <c t="s" s="1" r="B39">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
-        <v>134</v>
-      </c>
-      <c t="s" s="1" r="B40">
-        <v>135</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2745,158 +2525,377 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" customWidth="1" max="2" width="59.71"/>
+    <col min="2" customWidth="1" max="2" width="65.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>43</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c s="1" r="B5"/>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>56</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c t="s" s="4" r="B9">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>60</v>
-      </c>
-      <c t="s" s="3" r="B10">
-        <v>61</v>
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>84</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>78</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="B18">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>86</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="B22">
         <v>94</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c t="s" s="1" r="C22">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>96</v>
+      </c>
+      <c t="s" s="1" r="B23">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="C16">
+      <c t="s" s="1" r="C23">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
         <v>99</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>102</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>104</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>105</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>107</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
+        <v>109</v>
+      </c>
+      <c t="s" s="1" r="B28">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29">
+      <c t="s" s="1" r="A29">
+        <v>112</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>113</v>
+      </c>
+      <c s="1" r="C29"/>
+    </row>
+    <row r="30">
+      <c t="s" s="1" r="A30">
+        <v>114</v>
+      </c>
+      <c t="s" s="1" r="B30">
+        <v>115</v>
+      </c>
+      <c s="1" r="C30"/>
+    </row>
+    <row r="31">
+      <c t="s" s="1" r="A31">
+        <v>116</v>
+      </c>
+      <c t="s" s="1" r="B31">
+        <v>117</v>
+      </c>
+      <c s="1" r="C31"/>
+    </row>
+    <row r="32">
+      <c t="s" s="1" r="A32">
+        <v>118</v>
+      </c>
+      <c t="s" s="1" r="B32">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33">
+      <c t="s" s="1" r="A33">
+        <v>120</v>
+      </c>
+      <c t="s" s="1" r="B33">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
+        <v>122</v>
+      </c>
+      <c t="s" s="1" r="B34">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>124</v>
+      </c>
+      <c t="s" s="1" r="B35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>126</v>
+      </c>
+      <c t="s" s="1" r="B36">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
+        <v>128</v>
+      </c>
+      <c t="s" s="1" r="B37">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>130</v>
+      </c>
+      <c t="s" s="1" r="B38">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>132</v>
+      </c>
+      <c t="s" s="1" r="B39">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>134</v>
+      </c>
+      <c t="s" s="1" r="B40">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3242,256 +3241,145 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>216</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>218</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>222</v>
-      </c>
-      <c t="s" s="6" r="B4">
-        <v>223</v>
+        <v>243</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>244</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>225</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>227</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>228</v>
+        <v>260</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>229</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>230</v>
-      </c>
-      <c t="s" s="4" r="B8">
-        <v>231</v>
+        <v>262</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>265</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c t="s" s="7" r="B9">
-        <v>233</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>234</v>
+        <v>269</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>235</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>238</v>
+        <v>273</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>239</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>240</v>
+        <v>275</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>241</v>
+        <v>281</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>282</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>243</v>
+        <v>292</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>293</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>245</v>
+        <v>300</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>302</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>246</v>
+        <v>304</v>
       </c>
       <c t="s" s="1" r="B16">
-        <v>247</v>
+        <v>306</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>249</v>
-      </c>
-      <c t="s" s="1" r="B17">
-        <v>250</v>
-      </c>
-      <c t="s" s="1" r="C17">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>252</v>
-      </c>
-      <c t="s" s="5" r="B18">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>254</v>
-      </c>
-      <c t="s" s="1" r="B19">
-        <v>255</v>
-      </c>
-      <c t="s" s="1" r="C19">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>257</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>258</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
-        <v>260</v>
-      </c>
-      <c t="s" s="1" r="B21">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>262</v>
-      </c>
-      <c t="s" s="1" r="B22">
-        <v>263</v>
-      </c>
-      <c t="s" s="1" r="C22">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>265</v>
-      </c>
-      <c t="s" s="1" r="B23">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
-        <v>267</v>
-      </c>
-      <c t="s" s="1" r="B24">
-        <v>268</v>
-      </c>
-      <c t="s" s="1" r="C24">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>270</v>
-      </c>
-      <c t="s" s="1" r="B25">
-        <v>271</v>
-      </c>
-      <c t="s" s="1" r="C25">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>273</v>
-      </c>
-      <c t="s" s="1" r="B26">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>275</v>
-      </c>
-      <c t="s" s="1" r="B27">
-        <v>276</v>
-      </c>
-      <c t="s" s="1" r="C27">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>278</v>
-      </c>
-      <c t="s" s="1" r="B28">
-        <v>279</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>280</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3511,144 +3399,255 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>282</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>283</v>
+        <v>217</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>284</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>285</v>
+        <v>219</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>286</v>
+        <v>220</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>287</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>288</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>289</v>
+        <v>222</v>
+      </c>
+      <c t="s" s="6" r="B4">
+        <v>223</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>290</v>
+        <v>224</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>291</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>292</v>
+        <v>226</v>
       </c>
       <c t="s" s="3" r="B6">
-        <v>293</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>294</v>
+        <v>228</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>295</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>296</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>297</v>
+        <v>230</v>
+      </c>
+      <c t="s" s="4" r="B8">
+        <v>231</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>298</v>
+        <v>232</v>
       </c>
       <c t="s" s="7" r="B9">
-        <v>299</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>301</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>302</v>
+        <v>245</v>
       </c>
       <c t="s" s="1" r="B11">
-        <v>303</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>304</v>
+        <v>250</v>
       </c>
       <c t="s" s="1" r="B12">
-        <v>305</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>306</v>
+        <v>253</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>307</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>308</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>309</v>
+        <v>255</v>
       </c>
       <c t="s" s="1" r="B14">
-        <v>310</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>311</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>312</v>
+        <v>257</v>
       </c>
       <c t="s" s="1" r="B15">
-        <v>313</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>314</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
+        <v>259</v>
+      </c>
+      <c t="s" s="1" r="B16">
+        <v>263</v>
+      </c>
+      <c t="s" s="1" r="C16">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>266</v>
+      </c>
+      <c t="s" s="1" r="B17">
+        <v>276</v>
+      </c>
+      <c t="s" s="1" r="C17">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>278</v>
+      </c>
+      <c t="s" s="5" r="B18">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" s="1" r="A19">
+        <v>280</v>
+      </c>
+      <c t="s" s="1" r="B19">
+        <v>283</v>
+      </c>
+      <c t="s" s="1" r="C19">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>286</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>287</v>
+      </c>
+      <c t="s" s="1" r="C20">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" s="1" r="A21">
+        <v>289</v>
+      </c>
+      <c t="s" s="1" r="B21">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22">
+      <c t="s" s="1" r="A22">
+        <v>291</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>295</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" s="1" r="A23">
+        <v>297</v>
+      </c>
+      <c t="s" s="1" r="B23">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" s="1" r="A24">
+        <v>299</v>
+      </c>
+      <c t="s" s="1" r="B24">
+        <v>301</v>
+      </c>
+      <c t="s" s="1" r="C24">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>305</v>
+      </c>
+      <c t="s" s="1" r="B25">
+        <v>307</v>
+      </c>
+      <c t="s" s="1" r="C25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26">
+      <c t="s" s="1" r="A26">
+        <v>310</v>
+      </c>
+      <c t="s" s="1" r="B26">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>312</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>313</v>
+      </c>
+      <c t="s" s="1" r="C27">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="28">
+      <c t="s" s="1" r="A28">
         <v>315</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c t="s" s="1" r="B28">
         <v>316</v>
       </c>
-      <c t="s" s="1" r="C16">
+      <c t="s" s="1" r="C28">
         <v>317</v>
       </c>
     </row>

</xml_diff>